<commit_message>
vault backup: 2026-01-06 21:23:48
</commit_message>
<xml_diff>
--- a/Excalidraw/switch.xlsx
+++ b/Excalidraw/switch.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="731">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="736">
   <si>
     <t>DSA</t>
   </si>
@@ -1346,6 +1346,12 @@
 Eventual consistency: smaller R, W</t>
   </si>
   <si>
+    <t xml:space="preserve">Data vault modelling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">structuring data into three distinct entities: Hubs (business keys), Links (relationships), and Satellites (descriptive attributes for hubs). optimized for historical tracking, auditing, and scalability</t>
+  </si>
+  <si>
     <t>HLD</t>
   </si>
   <si>
@@ -1412,10 +1418,23 @@
     <t xml:space="preserve">Design a Key-Value Store (DynamoDB)</t>
   </si>
   <si>
+    <t xml:space="preserve">consistent hashing with virtual nodes, replication, quorum-based reads/writes, and configurable consistency</t>
+  </si>
+  <si>
+    <t>https://github.com/yashaggarwal85d/Neural-Vault/blob/main/Excalidraw/Design%20a%20Key-Value%20Store%20(DynamoDB).md</t>
+  </si>
+  <si>
     <t xml:space="preserve">Database Internals</t>
   </si>
   <si>
     <t xml:space="preserve">Design a Distributed Cache (Redis)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lets take the assumptions - 
+functional requirements - 
+1. Users should be able to store the value (string) via keys (string), get them, overwride them
+2. Each key value pair should have a time to live, eviction can be based of LRU or LFU algorithms
+3. </t>
   </si>
   <si>
     <t xml:space="preserve">Design a Notification Service</t>
@@ -2277,7 +2296,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2350,6 +2369,12 @@
         <bgColor indexed="47"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -2399,7 +2424,7 @@
       <diagonal style="none"/>
     </border>
   </borders>
-  <cellStyleXfs count="12">
+  <cellStyleXfs count="13">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="1" fillId="2" borderId="1" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="2" fillId="3" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
@@ -2412,8 +2437,9 @@
     <xf fontId="3" fillId="10" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="5" fillId="11" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="6" fillId="12" borderId="2" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="3" fillId="13" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="3" fillId="8" borderId="0" numFmtId="0" xfId="7" applyFont="1" applyFill="1"/>
     <xf fontId="3" fillId="7" borderId="0" numFmtId="0" xfId="6" applyFont="1" applyFill="1"/>
@@ -2453,17 +2479,23 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
     </xf>
+    <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="4" fillId="9" borderId="0" numFmtId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf fontId="3" fillId="6" borderId="0" numFmtId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf fontId="3" fillId="4" borderId="0" numFmtId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf fontId="3" fillId="13" borderId="0" numFmtId="0" xfId="12" applyFont="1" applyFill="1"/>
     <xf fontId="3" fillId="7" borderId="0" numFmtId="0" xfId="6" applyFont="1" applyFill="1">
       <protection hidden="0" locked="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="12">
+  <cellStyles count="13">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -2476,6 +2508,7 @@
     <cellStyle name="60% - Accent6" xfId="9" builtinId="52"/>
     <cellStyle name="Bad" xfId="10" builtinId="27"/>
     <cellStyle name="Input" xfId="11" builtinId="20"/>
+    <cellStyle name="Accent1" xfId="12" builtinId="29"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2944,7 +2977,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A132" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A140" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -6469,1399 +6502,1402 @@
       <c r="E141"/>
       <c r="F141"/>
     </row>
-    <row r="142" ht="14.25">
-      <c r="B142" s="9"/>
-      <c r="C142"/>
-      <c r="D142"/>
-      <c r="E142"/>
-      <c r="F142"/>
-    </row>
-    <row r="143" ht="13.5" customHeight="1">
-      <c r="A143" s="4"/>
-      <c r="B143" s="4"/>
-      <c r="C143" s="6"/>
-      <c r="D143" s="6"/>
-      <c r="E143" s="6"/>
-      <c r="F143" s="6"/>
-    </row>
-    <row r="144" ht="14.25">
+    <row r="142" ht="71.25">
+      <c r="A142" s="21" t="s">
+        <v>440</v>
+      </c>
+      <c r="B142" s="12" t="s">
+        <v>441</v>
+      </c>
+      <c r="C142" s="22"/>
+      <c r="D142" s="22"/>
+      <c r="E142" s="22"/>
+      <c r="F142" s="22"/>
+    </row>
+    <row r="143" ht="14.25">
+      <c r="B143" s="9"/>
+      <c r="C143"/>
+      <c r="D143"/>
+      <c r="E143"/>
+      <c r="F143"/>
+    </row>
+    <row r="144" ht="13.5" customHeight="1">
+      <c r="A144" s="4"/>
+      <c r="B144" s="4"/>
       <c r="C144" s="6"/>
       <c r="D144" s="6"/>
       <c r="E144" s="6"/>
       <c r="F144" s="6"/>
     </row>
     <row r="145" ht="14.25">
-      <c r="A145" s="5" t="s">
-        <v>440</v>
-      </c>
-      <c r="B145" s="5"/>
-      <c r="C145" s="5"/>
-      <c r="D145" s="5"/>
-      <c r="E145" s="5"/>
-      <c r="F145" s="5"/>
-    </row>
-    <row r="146" s="0" customFormat="1" ht="14.25">
-      <c r="A146" s="19" t="s">
+      <c r="C145" s="6"/>
+      <c r="D145" s="6"/>
+      <c r="E145" s="6"/>
+      <c r="F145" s="6"/>
+    </row>
+    <row r="146" ht="14.25">
+      <c r="A146" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="B146" s="5"/>
+      <c r="C146" s="5"/>
+      <c r="D146" s="5"/>
+      <c r="E146" s="5"/>
+      <c r="F146" s="5"/>
+    </row>
+    <row r="147" s="0" customFormat="1" ht="14.25">
+      <c r="A147" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B146" s="19" t="s">
+      <c r="B147" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C146" s="19" t="s">
-        <v>441</v>
-      </c>
-      <c r="D146" s="19" t="s">
+      <c r="C147" s="19" t="s">
+        <v>443</v>
+      </c>
+      <c r="D147" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E146" s="4" t="s">
+      <c r="E147" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F146" s="4"/>
-      <c r="G146"/>
-      <c r="H146"/>
-      <c r="I146"/>
-      <c r="J146" s="6"/>
-      <c r="K146"/>
-      <c r="L146"/>
-      <c r="M146"/>
-      <c r="N146"/>
-      <c r="O146"/>
-      <c r="P146"/>
-      <c r="Q146"/>
-      <c r="R146"/>
-      <c r="S146"/>
-      <c r="T146"/>
-      <c r="U146"/>
-      <c r="V146"/>
-      <c r="W146"/>
-      <c r="X146"/>
-      <c r="Y146"/>
-      <c r="Z146"/>
-      <c r="AA146"/>
-      <c r="AB146"/>
-      <c r="AC146"/>
-      <c r="AD146"/>
-      <c r="AE146"/>
-      <c r="AF146"/>
-      <c r="AG146"/>
-      <c r="AH146"/>
-      <c r="AI146"/>
-      <c r="AJ146"/>
-      <c r="AK146"/>
-      <c r="AL146"/>
-      <c r="AM146"/>
-      <c r="AN146"/>
-      <c r="AO146"/>
-      <c r="AP146"/>
-      <c r="AQ146"/>
-    </row>
-    <row r="147" ht="14.25">
-      <c r="A147" s="7" t="s">
-        <v>442</v>
-      </c>
-      <c r="B147" s="9" t="s">
-        <v>443</v>
-      </c>
-      <c r="C147" s="11" t="s">
-        <v>444</v>
-      </c>
-      <c r="D147" s="2" t="s">
-        <v>445</v>
-      </c>
-      <c r="E147" s="16" t="s">
-        <v>10</v>
-      </c>
       <c r="F147" s="4"/>
+      <c r="G147"/>
+      <c r="H147"/>
+      <c r="I147"/>
+      <c r="J147" s="6"/>
+      <c r="K147"/>
+      <c r="L147"/>
+      <c r="M147"/>
+      <c r="N147"/>
+      <c r="O147"/>
+      <c r="P147"/>
+      <c r="Q147"/>
+      <c r="R147"/>
+      <c r="S147"/>
+      <c r="T147"/>
+      <c r="U147"/>
+      <c r="V147"/>
+      <c r="W147"/>
+      <c r="X147"/>
+      <c r="Y147"/>
+      <c r="Z147"/>
+      <c r="AA147"/>
+      <c r="AB147"/>
+      <c r="AC147"/>
+      <c r="AD147"/>
+      <c r="AE147"/>
+      <c r="AF147"/>
+      <c r="AG147"/>
+      <c r="AH147"/>
+      <c r="AI147"/>
+      <c r="AJ147"/>
+      <c r="AK147"/>
+      <c r="AL147"/>
+      <c r="AM147"/>
+      <c r="AN147"/>
+      <c r="AO147"/>
+      <c r="AP147"/>
+      <c r="AQ147"/>
     </row>
     <row r="148" ht="14.25">
       <c r="A148" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="B148" s="9" t="s">
+        <v>445</v>
+      </c>
+      <c r="C148" s="11" t="s">
         <v>446</v>
       </c>
-      <c r="B148" s="9" t="s">
+      <c r="D148" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="C148" s="11" t="s">
-        <v>448</v>
-      </c>
-      <c r="D148" s="2" t="s">
-        <v>445</v>
-      </c>
-      <c r="E148" s="21" t="s">
+      <c r="E148" s="16" t="s">
         <v>10</v>
       </c>
       <c r="F148" s="4"/>
     </row>
     <row r="149" ht="14.25">
       <c r="A149" s="7" t="s">
+        <v>448</v>
+      </c>
+      <c r="B149" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="B149" s="9" t="s">
+      <c r="C149" s="11" t="s">
         <v>450</v>
       </c>
-      <c r="C149" s="11" t="s">
-        <v>451</v>
-      </c>
       <c r="D149" s="2" t="s">
-        <v>452</v>
-      </c>
-      <c r="E149" s="21" t="s">
+        <v>447</v>
+      </c>
+      <c r="E149" s="23" t="s">
         <v>10</v>
       </c>
       <c r="F149" s="4"/>
     </row>
     <row r="150" ht="14.25">
       <c r="A150" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="B150" s="9" t="s">
+        <v>452</v>
+      </c>
+      <c r="C150" s="11" t="s">
         <v>453</v>
       </c>
-      <c r="B150" s="9" t="s">
+      <c r="D150" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="C150" s="11" t="s">
+      <c r="E150" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F150" s="4"/>
+    </row>
+    <row r="151" ht="14.25">
+      <c r="A151" s="7" t="s">
         <v>455</v>
       </c>
-      <c r="D150" s="2" t="s">
+      <c r="B151" s="9" t="s">
         <v>456</v>
       </c>
-      <c r="E150" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F150" s="4"/>
-    </row>
-    <row r="151" ht="14.25">
-      <c r="A151" s="10" t="s">
+      <c r="C151" s="11" t="s">
         <v>457</v>
       </c>
-      <c r="B151" s="9" t="s">
+      <c r="D151" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="C151" s="11" t="s">
+      <c r="E151" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F151" s="4"/>
+    </row>
+    <row r="152" ht="14.25">
+      <c r="A152" s="10" t="s">
         <v>459</v>
       </c>
-      <c r="D151" s="2" t="s">
+      <c r="B152" s="9" t="s">
         <v>460</v>
       </c>
-      <c r="E151" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F151" s="4"/>
-    </row>
-    <row r="152" ht="14.25">
-      <c r="A152" t="s">
+      <c r="C152" s="11" t="s">
         <v>461</v>
       </c>
-      <c r="B152" s="9"/>
-      <c r="C152" s="1"/>
       <c r="D152" s="2" t="s">
         <v>462</v>
       </c>
-      <c r="E152" s="22" t="s">
-        <v>66</v>
+      <c r="E152" s="23" t="s">
+        <v>10</v>
       </c>
       <c r="F152" s="4"/>
     </row>
-    <row r="153" ht="14.25">
-      <c r="A153" t="s">
+    <row r="153" ht="15">
+      <c r="A153" s="10" t="s">
         <v>463</v>
       </c>
-      <c r="B153" s="9"/>
-      <c r="C153" s="1"/>
+      <c r="B153" s="24" t="s">
+        <v>464</v>
+      </c>
+      <c r="C153" s="11" t="s">
+        <v>465</v>
+      </c>
       <c r="D153" s="2" t="s">
-        <v>462</v>
-      </c>
-      <c r="E153" s="22" t="s">
+        <v>466</v>
+      </c>
+      <c r="E153" s="25" t="s">
         <v>66</v>
       </c>
       <c r="F153" s="4"/>
     </row>
     <row r="154" ht="14.25">
       <c r="A154" t="s">
-        <v>464</v>
-      </c>
-      <c r="B154" s="9"/>
+        <v>467</v>
+      </c>
+      <c r="B154" s="12" t="s">
+        <v>468</v>
+      </c>
       <c r="C154" s="1"/>
       <c r="D154" s="2" t="s">
-        <v>465</v>
-      </c>
-      <c r="E154" s="21" t="s">
-        <v>10</v>
+        <v>466</v>
+      </c>
+      <c r="E154" s="25" t="s">
+        <v>66</v>
       </c>
       <c r="F154" s="4"/>
     </row>
     <row r="155" ht="14.25">
       <c r="A155" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="B155" s="9"/>
       <c r="C155" s="1"/>
       <c r="D155" s="2" t="s">
-        <v>465</v>
-      </c>
-      <c r="E155" s="22" t="s">
-        <v>66</v>
+        <v>470</v>
+      </c>
+      <c r="E155" s="23" t="s">
+        <v>10</v>
       </c>
       <c r="F155" s="4"/>
     </row>
     <row r="156" ht="14.25">
       <c r="A156" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="B156" s="9"/>
       <c r="C156" s="1"/>
       <c r="D156" s="2" t="s">
-        <v>468</v>
-      </c>
-      <c r="E156" s="22" t="s">
+        <v>470</v>
+      </c>
+      <c r="E156" s="25" t="s">
         <v>66</v>
       </c>
       <c r="F156" s="4"/>
     </row>
     <row r="157" ht="14.25">
       <c r="A157" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="B157" s="9"/>
       <c r="C157" s="1"/>
       <c r="D157" s="2" t="s">
-        <v>470</v>
-      </c>
-      <c r="E157" s="22" t="s">
+        <v>473</v>
+      </c>
+      <c r="E157" s="25" t="s">
         <v>66</v>
       </c>
       <c r="F157" s="4"/>
     </row>
     <row r="158" ht="14.25">
       <c r="A158" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="B158" s="9"/>
       <c r="C158" s="1"/>
       <c r="D158" s="2" t="s">
-        <v>472</v>
-      </c>
-      <c r="E158" s="22" t="s">
+        <v>475</v>
+      </c>
+      <c r="E158" s="25" t="s">
         <v>66</v>
       </c>
       <c r="F158" s="4"/>
     </row>
     <row r="159" ht="14.25">
       <c r="A159" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="B159" s="9"/>
       <c r="C159" s="1"/>
       <c r="D159" s="2" t="s">
-        <v>474</v>
-      </c>
-      <c r="E159" s="22" t="s">
+        <v>477</v>
+      </c>
+      <c r="E159" s="25" t="s">
         <v>66</v>
       </c>
       <c r="F159" s="4"/>
-      <c r="L159" t="s">
-        <v>475</v>
-      </c>
     </row>
     <row r="160" ht="14.25">
       <c r="A160" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="B160" s="9"/>
       <c r="C160" s="1"/>
       <c r="D160" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="E160" s="21" t="s">
-        <v>10</v>
+        <v>479</v>
+      </c>
+      <c r="E160" s="25" t="s">
+        <v>66</v>
       </c>
       <c r="F160" s="4"/>
+      <c r="L160" t="s">
+        <v>480</v>
+      </c>
     </row>
     <row r="161" ht="14.25">
       <c r="A161" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="B161" s="9"/>
       <c r="C161" s="1"/>
       <c r="D161" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="E161" s="21" t="s">
+        <v>482</v>
+      </c>
+      <c r="E161" s="23" t="s">
         <v>10</v>
       </c>
       <c r="F161" s="4"/>
     </row>
     <row r="162" ht="14.25">
       <c r="A162" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="B162" s="9"/>
       <c r="C162" s="1"/>
       <c r="D162" s="2" t="s">
-        <v>481</v>
-      </c>
-      <c r="E162" s="22" t="s">
-        <v>66</v>
+        <v>484</v>
+      </c>
+      <c r="E162" s="23" t="s">
+        <v>10</v>
       </c>
       <c r="F162" s="4"/>
     </row>
     <row r="163" ht="14.25">
       <c r="A163" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="B163" s="9"/>
       <c r="C163" s="1"/>
       <c r="D163" s="2" t="s">
-        <v>483</v>
-      </c>
-      <c r="E163" s="21" t="s">
-        <v>10</v>
+        <v>486</v>
+      </c>
+      <c r="E163" s="25" t="s">
+        <v>66</v>
       </c>
       <c r="F163" s="4"/>
     </row>
     <row r="164" ht="14.25">
-      <c r="A164" t="s">
-        <v>484</v>
+      <c r="A164" s="26" t="s">
+        <v>487</v>
       </c>
       <c r="B164" s="9"/>
       <c r="C164" s="1"/>
       <c r="D164" s="2" t="s">
-        <v>485</v>
-      </c>
-      <c r="E164" s="21" t="s">
+        <v>488</v>
+      </c>
+      <c r="E164" s="23" t="s">
         <v>10</v>
       </c>
       <c r="F164" s="4"/>
     </row>
     <row r="165" ht="14.25">
       <c r="A165" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="B165" s="9"/>
       <c r="C165" s="1"/>
       <c r="D165" s="2" t="s">
-        <v>487</v>
-      </c>
-      <c r="E165" s="21" t="s">
+        <v>490</v>
+      </c>
+      <c r="E165" s="23" t="s">
         <v>10</v>
       </c>
       <c r="F165" s="4"/>
     </row>
     <row r="166" ht="14.25">
       <c r="A166" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="B166" s="9"/>
       <c r="C166" s="1"/>
       <c r="D166" s="2" t="s">
-        <v>489</v>
-      </c>
-      <c r="E166" s="22" t="s">
-        <v>66</v>
+        <v>492</v>
+      </c>
+      <c r="E166" s="23" t="s">
+        <v>10</v>
       </c>
       <c r="F166" s="4"/>
     </row>
     <row r="167" ht="14.25">
       <c r="A167" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="B167" s="9"/>
       <c r="C167" s="1"/>
       <c r="D167" s="2" t="s">
-        <v>491</v>
-      </c>
-      <c r="E167" s="22" t="s">
+        <v>494</v>
+      </c>
+      <c r="E167" s="25" t="s">
         <v>66</v>
       </c>
       <c r="F167" s="4"/>
     </row>
     <row r="168" ht="14.25">
       <c r="A168" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="B168" s="9"/>
       <c r="C168" s="1"/>
       <c r="D168" s="2" t="s">
-        <v>493</v>
-      </c>
-      <c r="E168" s="22" t="s">
+        <v>496</v>
+      </c>
+      <c r="E168" s="25" t="s">
         <v>66</v>
       </c>
       <c r="F168" s="4"/>
     </row>
     <row r="169" ht="14.25">
       <c r="A169" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
       <c r="B169" s="9"/>
       <c r="C169" s="1"/>
       <c r="D169" s="2" t="s">
-        <v>495</v>
-      </c>
-      <c r="E169" s="22" t="s">
+        <v>498</v>
+      </c>
+      <c r="E169" s="25" t="s">
         <v>66</v>
       </c>
       <c r="F169" s="4"/>
     </row>
     <row r="170" ht="14.25">
       <c r="A170" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="B170" s="9"/>
       <c r="C170" s="1"/>
       <c r="D170" s="2" t="s">
-        <v>497</v>
-      </c>
-      <c r="E170" s="22" t="s">
+        <v>500</v>
+      </c>
+      <c r="E170" s="25" t="s">
         <v>66</v>
       </c>
       <c r="F170" s="4"/>
     </row>
     <row r="171" ht="14.25">
       <c r="A171" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
       <c r="B171" s="9"/>
       <c r="C171" s="1"/>
       <c r="D171" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="E171" s="21" t="s">
-        <v>10</v>
+        <v>502</v>
+      </c>
+      <c r="E171" s="25" t="s">
+        <v>66</v>
       </c>
       <c r="F171" s="4"/>
     </row>
     <row r="172" ht="14.25">
       <c r="A172" t="s">
-        <v>500</v>
+        <v>503</v>
       </c>
       <c r="B172" s="9"/>
       <c r="C172" s="1"/>
       <c r="D172" s="2" t="s">
-        <v>501</v>
-      </c>
-      <c r="E172" s="21" t="s">
+        <v>504</v>
+      </c>
+      <c r="E172" s="23" t="s">
         <v>10</v>
       </c>
       <c r="F172" s="4"/>
     </row>
     <row r="173" ht="14.25">
       <c r="A173" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
       <c r="B173" s="9"/>
       <c r="C173" s="1"/>
       <c r="D173" s="2" t="s">
-        <v>503</v>
-      </c>
-      <c r="E173" s="21" t="s">
+        <v>506</v>
+      </c>
+      <c r="E173" s="23" t="s">
         <v>10</v>
       </c>
       <c r="F173" s="4"/>
     </row>
     <row r="174" ht="14.25">
       <c r="A174" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
       <c r="B174" s="9"/>
       <c r="C174" s="1"/>
       <c r="D174" s="2" t="s">
-        <v>505</v>
-      </c>
-      <c r="E174" s="22" t="s">
-        <v>66</v>
+        <v>508</v>
+      </c>
+      <c r="E174" s="23" t="s">
+        <v>10</v>
       </c>
       <c r="F174" s="4"/>
     </row>
     <row r="175" ht="14.25">
       <c r="A175" t="s">
-        <v>506</v>
+        <v>509</v>
       </c>
       <c r="B175" s="9"/>
       <c r="C175" s="1"/>
       <c r="D175" s="2" t="s">
-        <v>507</v>
-      </c>
-      <c r="E175" s="22" t="s">
+        <v>510</v>
+      </c>
+      <c r="E175" s="25" t="s">
         <v>66</v>
       </c>
       <c r="F175" s="4"/>
     </row>
     <row r="176" ht="14.25">
       <c r="A176" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="B176" s="9"/>
       <c r="C176" s="1"/>
       <c r="D176" s="2" t="s">
-        <v>509</v>
-      </c>
-      <c r="E176" s="22" t="s">
+        <v>512</v>
+      </c>
+      <c r="E176" s="25" t="s">
         <v>66</v>
       </c>
       <c r="F176" s="4"/>
     </row>
     <row r="177" ht="14.25">
       <c r="A177" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="B177" s="9"/>
       <c r="C177" s="1"/>
       <c r="D177" s="2" t="s">
-        <v>511</v>
-      </c>
-      <c r="E177" s="21" t="s">
-        <v>10</v>
+        <v>514</v>
+      </c>
+      <c r="E177" s="25" t="s">
+        <v>66</v>
       </c>
       <c r="F177" s="4"/>
     </row>
     <row r="178" ht="14.25">
       <c r="A178" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="B178" s="9"/>
       <c r="C178" s="1"/>
       <c r="D178" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E178" s="22" t="s">
-        <v>66</v>
+        <v>516</v>
+      </c>
+      <c r="E178" s="23" t="s">
+        <v>10</v>
       </c>
       <c r="F178" s="4"/>
     </row>
     <row r="179" ht="14.25">
       <c r="A179" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="B179" s="9"/>
       <c r="C179" s="1"/>
       <c r="D179" s="2" t="s">
-        <v>515</v>
-      </c>
-      <c r="E179" s="21" t="s">
-        <v>10</v>
+        <v>518</v>
+      </c>
+      <c r="E179" s="25" t="s">
+        <v>66</v>
       </c>
       <c r="F179" s="4"/>
     </row>
     <row r="180" ht="14.25">
       <c r="A180" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="B180" s="9"/>
       <c r="C180" s="1"/>
       <c r="D180" s="2" t="s">
-        <v>517</v>
-      </c>
-      <c r="E180" s="22" t="s">
-        <v>66</v>
+        <v>520</v>
+      </c>
+      <c r="E180" s="23" t="s">
+        <v>10</v>
       </c>
       <c r="F180" s="4"/>
     </row>
     <row r="181" ht="14.25">
       <c r="A181" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="B181" s="9"/>
       <c r="C181" s="1"/>
       <c r="D181" s="2" t="s">
-        <v>519</v>
-      </c>
-      <c r="E181" s="21" t="s">
-        <v>10</v>
+        <v>522</v>
+      </c>
+      <c r="E181" s="25" t="s">
+        <v>66</v>
       </c>
       <c r="F181" s="4"/>
     </row>
     <row r="182" ht="14.25">
       <c r="A182" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="B182" s="9"/>
       <c r="C182" s="1"/>
       <c r="D182" s="2" t="s">
-        <v>521</v>
-      </c>
-      <c r="E182" s="21" t="s">
+        <v>524</v>
+      </c>
+      <c r="E182" s="23" t="s">
         <v>10</v>
       </c>
       <c r="F182" s="4"/>
     </row>
     <row r="183" ht="14.25">
       <c r="A183" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="B183" s="9"/>
       <c r="C183" s="1"/>
       <c r="D183" s="2" t="s">
-        <v>523</v>
-      </c>
-      <c r="E183" s="22" t="s">
-        <v>66</v>
+        <v>526</v>
+      </c>
+      <c r="E183" s="23" t="s">
+        <v>10</v>
       </c>
       <c r="F183" s="4"/>
     </row>
     <row r="184" ht="14.25">
       <c r="A184" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="B184" s="9"/>
       <c r="C184" s="1"/>
       <c r="D184" s="2" t="s">
-        <v>525</v>
-      </c>
-      <c r="E184" s="22" t="s">
+        <v>528</v>
+      </c>
+      <c r="E184" s="25" t="s">
         <v>66</v>
       </c>
       <c r="F184" s="4"/>
     </row>
     <row r="185" ht="14.25">
       <c r="A185" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="B185" s="9"/>
       <c r="C185" s="1"/>
       <c r="D185" s="2" t="s">
-        <v>527</v>
-      </c>
-      <c r="E185" s="22" t="s">
+        <v>530</v>
+      </c>
+      <c r="E185" s="25" t="s">
         <v>66</v>
       </c>
       <c r="F185" s="4"/>
     </row>
     <row r="186" ht="14.25">
       <c r="A186" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="B186" s="9"/>
       <c r="C186" s="1"/>
       <c r="D186" s="2" t="s">
-        <v>529</v>
-      </c>
-      <c r="E186" s="22" t="s">
+        <v>532</v>
+      </c>
+      <c r="E186" s="25" t="s">
         <v>66</v>
       </c>
       <c r="F186" s="4"/>
     </row>
     <row r="187" ht="14.25">
       <c r="A187" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="B187" s="9"/>
       <c r="C187" s="1"/>
       <c r="D187" s="2" t="s">
-        <v>531</v>
-      </c>
-      <c r="E187" s="21" t="s">
-        <v>10</v>
+        <v>534</v>
+      </c>
+      <c r="E187" s="25" t="s">
+        <v>66</v>
       </c>
       <c r="F187" s="4"/>
     </row>
     <row r="188" ht="14.25">
       <c r="A188" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
       <c r="B188" s="9"/>
       <c r="C188" s="1"/>
       <c r="D188" s="2" t="s">
-        <v>533</v>
-      </c>
-      <c r="E188" s="22" t="s">
-        <v>66</v>
+        <v>536</v>
+      </c>
+      <c r="E188" s="23" t="s">
+        <v>10</v>
       </c>
       <c r="F188" s="4"/>
     </row>
     <row r="189" ht="14.25">
       <c r="A189" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="B189" s="9"/>
       <c r="C189" s="1"/>
       <c r="D189" s="2" t="s">
-        <v>535</v>
-      </c>
-      <c r="E189" s="21" t="s">
-        <v>10</v>
+        <v>538</v>
+      </c>
+      <c r="E189" s="25" t="s">
+        <v>66</v>
       </c>
       <c r="F189" s="4"/>
     </row>
     <row r="190" ht="14.25">
       <c r="A190" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="B190" s="9"/>
       <c r="C190" s="1"/>
       <c r="D190" s="2" t="s">
-        <v>537</v>
-      </c>
-      <c r="E190" s="22" t="s">
-        <v>66</v>
+        <v>540</v>
+      </c>
+      <c r="E190" s="23" t="s">
+        <v>10</v>
       </c>
       <c r="F190" s="4"/>
     </row>
     <row r="191" ht="14.25">
       <c r="A191" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
       <c r="B191" s="9"/>
       <c r="C191" s="1"/>
       <c r="D191" s="2" t="s">
-        <v>539</v>
-      </c>
-      <c r="E191" s="18" t="s">
+        <v>542</v>
+      </c>
+      <c r="E191" s="25" t="s">
         <v>66</v>
       </c>
       <c r="F191" s="4"/>
     </row>
     <row r="192" ht="14.25">
-      <c r="A192" s="4"/>
-      <c r="B192" s="4"/>
-      <c r="C192" s="4"/>
-      <c r="D192" s="4"/>
-      <c r="E192" s="4"/>
+      <c r="A192" t="s">
+        <v>543</v>
+      </c>
+      <c r="B192" s="9"/>
+      <c r="C192" s="1"/>
+      <c r="D192" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="E192" s="18" t="s">
+        <v>66</v>
+      </c>
       <c r="F192" s="4"/>
     </row>
     <row r="193" ht="14.25">
-      <c r="C193"/>
-      <c r="D193"/>
-      <c r="E193"/>
-      <c r="F193"/>
+      <c r="A193" s="4"/>
+      <c r="B193" s="4"/>
+      <c r="C193" s="4"/>
+      <c r="D193" s="4"/>
+      <c r="E193" s="4"/>
+      <c r="F193" s="4"/>
     </row>
     <row r="194" ht="14.25">
-      <c r="A194" s="5" t="s">
-        <v>540</v>
-      </c>
-      <c r="B194" s="5"/>
-      <c r="C194" s="5"/>
-      <c r="D194" s="5"/>
-      <c r="E194" s="5"/>
-      <c r="F194" s="5"/>
+      <c r="C194"/>
+      <c r="D194"/>
+      <c r="E194"/>
+      <c r="F194"/>
     </row>
     <row r="195" ht="14.25">
-      <c r="A195" s="4" t="s">
-        <v>541</v>
-      </c>
-      <c r="B195" s="4" t="s">
+      <c r="A195" s="5" t="s">
+        <v>545</v>
+      </c>
+      <c r="B195" s="5"/>
+      <c r="C195" s="5"/>
+      <c r="D195" s="5"/>
+      <c r="E195" s="5"/>
+      <c r="F195" s="5"/>
+    </row>
+    <row r="196" ht="14.25">
+      <c r="A196" s="4" t="s">
+        <v>546</v>
+      </c>
+      <c r="B196" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C195" s="4" t="s">
-        <v>542</v>
-      </c>
-      <c r="D195" s="4" t="s">
-        <v>543</v>
-      </c>
-      <c r="E195" s="4"/>
-      <c r="F195" s="4"/>
-    </row>
-    <row r="196" ht="14.25">
-      <c r="A196" s="20" t="s">
-        <v>544</v>
-      </c>
-      <c r="B196" s="9"/>
-      <c r="C196" s="1" t="s">
-        <v>545</v>
-      </c>
-      <c r="D196" s="2" t="s">
-        <v>546</v>
-      </c>
+      <c r="C196" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="D196" s="4" t="s">
+        <v>548</v>
+      </c>
+      <c r="E196" s="4"/>
       <c r="F196" s="4"/>
     </row>
     <row r="197" ht="14.25">
       <c r="A197" s="20" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="B197" s="9"/>
       <c r="C197" s="1" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>546</v>
+        <v>551</v>
       </c>
       <c r="F197" s="4"/>
-      <c r="H197" s="6"/>
     </row>
     <row r="198" ht="14.25">
       <c r="A198" s="20" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="B198" s="9"/>
       <c r="C198" s="1" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>546</v>
+        <v>551</v>
       </c>
       <c r="F198" s="4"/>
+      <c r="H198" s="6"/>
     </row>
     <row r="199" ht="14.25">
       <c r="A199" s="20" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="B199" s="9"/>
       <c r="C199" s="1" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
       <c r="D199" s="2" t="s">
-        <v>546</v>
+        <v>551</v>
       </c>
       <c r="F199" s="4"/>
     </row>
     <row r="200" ht="14.25">
       <c r="A200" s="20" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
       <c r="B200" s="9"/>
       <c r="C200" s="1" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>546</v>
+        <v>551</v>
       </c>
       <c r="F200" s="4"/>
     </row>
     <row r="201" ht="14.25">
       <c r="A201" s="20" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
       <c r="B201" s="9"/>
       <c r="C201" s="1" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
       <c r="F201" s="4"/>
     </row>
     <row r="202" ht="14.25">
       <c r="A202" s="20" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="B202" s="9"/>
       <c r="C202" s="1" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>557</v>
+        <v>562</v>
       </c>
       <c r="F202" s="4"/>
-      <c r="H202" s="6"/>
     </row>
     <row r="203" ht="14.25">
       <c r="A203" s="20" t="s">
-        <v>560</v>
+        <v>563</v>
       </c>
       <c r="B203" s="9"/>
       <c r="C203" s="1" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
       <c r="D203" s="2" t="s">
-        <v>557</v>
+        <v>562</v>
       </c>
       <c r="F203" s="4"/>
       <c r="H203" s="6"/>
     </row>
     <row r="204" ht="14.25">
       <c r="A204" s="20" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="B204" s="9"/>
       <c r="C204" s="1" t="s">
-        <v>563</v>
+        <v>566</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="F204" s="4"/>
       <c r="H204" s="6"/>
     </row>
     <row r="205" ht="14.25">
       <c r="A205" s="20" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="B205" s="9"/>
       <c r="C205" s="1" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="D205" s="2" t="s">
-        <v>564</v>
+        <v>569</v>
       </c>
       <c r="F205" s="4"/>
       <c r="H205" s="6"/>
     </row>
     <row r="206" ht="14.25">
       <c r="A206" s="20" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="B206" s="9"/>
       <c r="C206" s="1" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="D206" s="2" t="s">
-        <v>564</v>
+        <v>569</v>
       </c>
       <c r="F206" s="4"/>
       <c r="H206" s="6"/>
     </row>
     <row r="207" ht="14.25">
       <c r="A207" s="20" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="B207" s="9"/>
       <c r="C207" s="1" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="D207" s="2" t="s">
-        <v>564</v>
+        <v>569</v>
       </c>
       <c r="F207" s="4"/>
       <c r="H207" s="6"/>
     </row>
     <row r="208" ht="14.25">
       <c r="A208" s="20" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="B208" s="9"/>
       <c r="C208" s="1" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="D208" s="2" t="s">
-        <v>564</v>
+        <v>569</v>
       </c>
       <c r="F208" s="4"/>
       <c r="H208" s="6"/>
     </row>
     <row r="209" ht="14.25">
       <c r="A209" s="20" t="s">
-        <v>573</v>
+        <v>576</v>
       </c>
       <c r="B209" s="9"/>
       <c r="C209" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>564</v>
+        <v>569</v>
       </c>
       <c r="F209" s="4"/>
+      <c r="H209" s="6"/>
     </row>
     <row r="210" ht="14.25">
       <c r="A210" s="20" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
       <c r="B210" s="9"/>
       <c r="C210" s="1" t="s">
-        <v>576</v>
+        <v>579</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>564</v>
+        <v>569</v>
       </c>
       <c r="F210" s="4"/>
     </row>
     <row r="211" ht="14.25">
       <c r="A211" s="20" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="B211" s="9"/>
       <c r="C211" s="1" t="s">
-        <v>578</v>
+        <v>581</v>
       </c>
       <c r="D211" s="2" t="s">
-        <v>564</v>
+        <v>569</v>
       </c>
       <c r="F211" s="4"/>
     </row>
     <row r="212" ht="14.25">
       <c r="A212" s="20" t="s">
-        <v>579</v>
+        <v>582</v>
       </c>
       <c r="B212" s="9"/>
       <c r="C212" s="1" t="s">
-        <v>580</v>
+        <v>583</v>
       </c>
       <c r="D212" s="2" t="s">
-        <v>564</v>
+        <v>569</v>
       </c>
       <c r="F212" s="4"/>
     </row>
     <row r="213" ht="14.25">
       <c r="A213" s="20" t="s">
-        <v>581</v>
+        <v>584</v>
       </c>
       <c r="B213" s="9"/>
       <c r="C213" s="1" t="s">
-        <v>582</v>
+        <v>585</v>
       </c>
       <c r="D213" s="2" t="s">
-        <v>564</v>
+        <v>569</v>
       </c>
       <c r="F213" s="4"/>
     </row>
     <row r="214" ht="14.25">
       <c r="A214" s="20" t="s">
-        <v>583</v>
+        <v>586</v>
       </c>
       <c r="B214" s="9"/>
       <c r="C214" s="1" t="s">
-        <v>584</v>
+        <v>587</v>
       </c>
       <c r="D214" s="2" t="s">
-        <v>585</v>
+        <v>569</v>
       </c>
       <c r="F214" s="4"/>
     </row>
     <row r="215" ht="14.25">
       <c r="A215" s="20" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="B215" s="9"/>
       <c r="C215" s="1" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>585</v>
+        <v>590</v>
       </c>
       <c r="F215" s="4"/>
     </row>
     <row r="216" ht="14.25">
       <c r="A216" s="20" t="s">
-        <v>588</v>
+        <v>591</v>
       </c>
       <c r="B216" s="9"/>
       <c r="C216" s="1" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
       <c r="D216" s="2" t="s">
-        <v>585</v>
+        <v>590</v>
       </c>
       <c r="F216" s="4"/>
     </row>
     <row r="217" ht="14.25">
       <c r="A217" s="20" t="s">
-        <v>590</v>
+        <v>593</v>
       </c>
       <c r="B217" s="9"/>
       <c r="C217" s="1" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>585</v>
+        <v>590</v>
       </c>
       <c r="F217" s="4"/>
     </row>
     <row r="218" ht="14.25">
       <c r="A218" s="20" t="s">
-        <v>592</v>
+        <v>595</v>
       </c>
       <c r="B218" s="9"/>
       <c r="C218" s="1" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>585</v>
+        <v>590</v>
       </c>
       <c r="F218" s="4"/>
     </row>
     <row r="219" ht="14.25">
       <c r="A219" s="20" t="s">
-        <v>594</v>
+        <v>597</v>
       </c>
       <c r="B219" s="9"/>
       <c r="C219" s="1" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>596</v>
+        <v>590</v>
       </c>
       <c r="F219" s="4"/>
     </row>
     <row r="220" ht="14.25">
       <c r="A220" s="20" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="B220" s="9"/>
       <c r="C220" s="1" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="D220" s="2" t="s">
-        <v>596</v>
+        <v>601</v>
       </c>
       <c r="F220" s="4"/>
     </row>
     <row r="221" ht="14.25">
       <c r="A221" s="20" t="s">
-        <v>599</v>
+        <v>602</v>
       </c>
       <c r="B221" s="9"/>
       <c r="C221" s="1" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="D221" s="2" t="s">
-        <v>596</v>
+        <v>601</v>
       </c>
       <c r="F221" s="4"/>
     </row>
     <row r="222" ht="14.25">
       <c r="A222" s="20" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
       <c r="B222" s="9"/>
       <c r="C222" s="1" t="s">
-        <v>602</v>
+        <v>605</v>
       </c>
       <c r="D222" s="2" t="s">
-        <v>596</v>
+        <v>601</v>
       </c>
       <c r="F222" s="4"/>
     </row>
     <row r="223" ht="14.25">
       <c r="A223" s="20" t="s">
-        <v>603</v>
+        <v>606</v>
       </c>
       <c r="B223" s="9"/>
       <c r="C223" s="1" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
       <c r="D223" s="2" t="s">
-        <v>596</v>
+        <v>601</v>
       </c>
       <c r="F223" s="4"/>
     </row>
     <row r="224" ht="14.25">
       <c r="A224" s="20" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B224" s="9"/>
       <c r="C224" s="1" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
       <c r="D224" s="2" t="s">
-        <v>596</v>
+        <v>601</v>
       </c>
       <c r="F224" s="4"/>
     </row>
     <row r="225" ht="14.25">
       <c r="A225" s="20" t="s">
-        <v>607</v>
+        <v>610</v>
       </c>
       <c r="B225" s="9"/>
       <c r="C225" s="1" t="s">
-        <v>608</v>
+        <v>611</v>
       </c>
       <c r="D225" s="2" t="s">
-        <v>596</v>
+        <v>601</v>
       </c>
       <c r="F225" s="4"/>
     </row>
     <row r="226" ht="14.25">
       <c r="A226" s="20" t="s">
-        <v>609</v>
+        <v>612</v>
       </c>
       <c r="B226" s="9"/>
       <c r="C226" s="1" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="D226" s="2" t="s">
-        <v>611</v>
+        <v>601</v>
       </c>
       <c r="F226" s="4"/>
     </row>
     <row r="227" ht="14.25">
       <c r="A227" s="20" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="B227" s="9"/>
       <c r="C227" s="1" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="D227" s="2" t="s">
-        <v>611</v>
+        <v>616</v>
       </c>
       <c r="F227" s="4"/>
     </row>
     <row r="228" ht="14.25">
       <c r="A228" s="20" t="s">
-        <v>614</v>
+        <v>617</v>
       </c>
       <c r="B228" s="9"/>
       <c r="C228" s="1" t="s">
-        <v>615</v>
+        <v>618</v>
       </c>
       <c r="D228" s="2" t="s">
-        <v>611</v>
+        <v>616</v>
       </c>
       <c r="F228" s="4"/>
     </row>
     <row r="229" ht="14.25">
       <c r="A229" s="20" t="s">
-        <v>616</v>
+        <v>619</v>
       </c>
       <c r="B229" s="9"/>
       <c r="C229" s="1" t="s">
-        <v>617</v>
+        <v>620</v>
       </c>
       <c r="D229" s="2" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="F229" s="4"/>
     </row>
     <row r="230" ht="14.25">
       <c r="A230" s="20" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="B230" s="9"/>
       <c r="C230" s="1" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="D230" s="2" t="s">
-        <v>618</v>
+        <v>623</v>
       </c>
       <c r="F230" s="4"/>
     </row>
     <row r="231" ht="14.25">
-      <c r="A231" t="s">
-        <v>621</v>
+      <c r="A231" s="20" t="s">
+        <v>624</v>
       </c>
       <c r="B231" s="9"/>
       <c r="C231" s="1" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
       <c r="D231" s="2" t="s">
         <v>623</v>
       </c>
       <c r="F231" s="4"/>
-      <c r="H231" s="6"/>
     </row>
     <row r="232" ht="14.25">
       <c r="A232" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="B232" s="9"/>
       <c r="C232" s="1" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="D232" s="2" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="F232" s="4"/>
       <c r="H232" s="6"/>
     </row>
     <row r="233" ht="14.25">
       <c r="A233" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="B233" s="9"/>
       <c r="C233" s="1" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="D233" s="2" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
       <c r="F233" s="4"/>
       <c r="H233" s="6"/>
     </row>
     <row r="234" ht="14.25">
       <c r="A234" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="B234" s="9"/>
       <c r="C234" s="1" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
       <c r="D234" s="2" t="s">
-        <v>564</v>
+        <v>634</v>
       </c>
       <c r="F234" s="4"/>
       <c r="H234" s="6"/>
     </row>
     <row r="235" ht="14.25">
       <c r="A235" t="s">
-        <v>632</v>
+        <v>635</v>
       </c>
       <c r="B235" s="9"/>
       <c r="C235" s="1" t="s">
-        <v>633</v>
+        <v>636</v>
       </c>
       <c r="D235" s="2" t="s">
-        <v>634</v>
+        <v>569</v>
       </c>
       <c r="F235" s="4"/>
       <c r="H235" s="6"/>
     </row>
     <row r="236" ht="14.25">
       <c r="A236" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
       <c r="B236" s="9"/>
       <c r="C236" s="1" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="D236" s="2" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c r="F236" s="4"/>
       <c r="H236" s="6"/>
     </row>
     <row r="237" ht="14.25">
       <c r="A237" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="B237" s="9"/>
       <c r="C237" s="1" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="D237" s="2" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="F237" s="4"/>
       <c r="H237" s="6"/>
     </row>
     <row r="238" ht="14.25">
       <c r="A238" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="B238" s="9"/>
       <c r="C238" s="1" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="D238" s="2" t="s">
-        <v>640</v>
+        <v>645</v>
       </c>
       <c r="F238" s="4"/>
       <c r="H238" s="6"/>
     </row>
     <row r="239" ht="14.25">
       <c r="A239" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
       <c r="B239" s="9"/>
       <c r="C239" s="1" t="s">
-        <v>644</v>
+        <v>647</v>
       </c>
       <c r="D239" s="2" t="s">
-        <v>640</v>
+        <v>645</v>
       </c>
       <c r="F239" s="4"/>
       <c r="H239" s="6"/>
     </row>
     <row r="240" ht="14.25">
       <c r="A240" t="s">
-        <v>645</v>
+        <v>648</v>
       </c>
       <c r="B240" s="9"/>
       <c r="C240" s="1" t="s">
-        <v>646</v>
+        <v>649</v>
       </c>
       <c r="D240" s="2" t="s">
-        <v>647</v>
-      </c>
-      <c r="E240" s="3"/>
+        <v>645</v>
+      </c>
       <c r="F240" s="4"/>
       <c r="H240" s="6"/>
     </row>
     <row r="241" ht="14.25">
       <c r="A241" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B241" s="9"/>
       <c r="C241" s="1" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="D241" s="2" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c r="E241" s="3"/>
       <c r="F241" s="4"/>
@@ -7869,14 +7905,14 @@
     </row>
     <row r="242" ht="14.25">
       <c r="A242" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="B242" s="9"/>
       <c r="C242" s="1" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="D242" s="2" t="s">
-        <v>640</v>
+        <v>655</v>
       </c>
       <c r="E242" s="3"/>
       <c r="F242" s="4"/>
@@ -7884,14 +7920,14 @@
     </row>
     <row r="243" ht="14.25">
       <c r="A243" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="B243" s="9"/>
       <c r="C243" s="1" t="s">
-        <v>654</v>
+        <v>657</v>
       </c>
       <c r="D243" s="2" t="s">
-        <v>655</v>
+        <v>645</v>
       </c>
       <c r="E243" s="3"/>
       <c r="F243" s="4"/>
@@ -7899,14 +7935,14 @@
     </row>
     <row r="244" ht="14.25">
       <c r="A244" t="s">
-        <v>656</v>
+        <v>658</v>
       </c>
       <c r="B244" s="9"/>
       <c r="C244" s="1" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="D244" s="2" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="E244" s="3"/>
       <c r="F244" s="4"/>
@@ -7914,648 +7950,657 @@
     </row>
     <row r="245" ht="14.25">
       <c r="A245" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="B245" s="9"/>
       <c r="C245" s="1" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="D245" s="2" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="E245" s="3"/>
       <c r="F245" s="4"/>
       <c r="H245" s="6"/>
     </row>
     <row r="246" ht="14.25">
-      <c r="A246" s="4"/>
-      <c r="B246" s="4"/>
-      <c r="C246" s="4"/>
-      <c r="D246" s="4"/>
-      <c r="E246" s="4"/>
+      <c r="A246" t="s">
+        <v>664</v>
+      </c>
+      <c r="B246" s="9"/>
+      <c r="C246" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="D246" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="E246" s="3"/>
       <c r="F246" s="4"/>
+      <c r="H246" s="6"/>
     </row>
     <row r="247" ht="14.25">
-      <c r="C247" s="1"/>
-      <c r="D247" s="2"/>
-      <c r="E247" s="3"/>
+      <c r="A247" s="4"/>
+      <c r="B247" s="4"/>
+      <c r="C247" s="4"/>
+      <c r="D247" s="4"/>
+      <c r="E247" s="4"/>
       <c r="F247" s="4"/>
     </row>
     <row r="248" ht="14.25">
-      <c r="A248" s="5" t="s">
-        <v>662</v>
-      </c>
-      <c r="B248" s="5"/>
-      <c r="C248" s="5"/>
-      <c r="D248" s="5"/>
-      <c r="E248" s="5"/>
-      <c r="F248" s="5"/>
+      <c r="C248" s="1"/>
+      <c r="D248" s="2"/>
+      <c r="E248" s="3"/>
+      <c r="F248" s="4"/>
     </row>
     <row r="249" ht="14.25">
-      <c r="A249" s="19" t="s">
+      <c r="A249" s="5" t="s">
+        <v>667</v>
+      </c>
+      <c r="B249" s="5"/>
+      <c r="C249" s="5"/>
+      <c r="D249" s="5"/>
+      <c r="E249" s="5"/>
+      <c r="F249" s="5"/>
+    </row>
+    <row r="250" ht="14.25">
+      <c r="A250" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B249" s="19" t="s">
+      <c r="B250" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C249" s="19" t="s">
-        <v>441</v>
-      </c>
-      <c r="D249" s="19" t="s">
+      <c r="C250" s="19" t="s">
+        <v>443</v>
+      </c>
+      <c r="D250" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E249" s="4" t="s">
+      <c r="E250" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="F249" s="4"/>
-    </row>
-    <row r="250" ht="14.25">
-      <c r="A250" s="20" t="s">
-        <v>663</v>
-      </c>
-      <c r="B250" s="9"/>
-      <c r="C250" s="1"/>
-      <c r="D250" s="23" t="s">
-        <v>664</v>
-      </c>
-      <c r="E250" s="16" t="s">
-        <v>10</v>
       </c>
       <c r="F250" s="4"/>
     </row>
     <row r="251" ht="14.25">
       <c r="A251" s="20" t="s">
-        <v>665</v>
+        <v>668</v>
       </c>
       <c r="B251" s="9"/>
       <c r="C251" s="1"/>
-      <c r="D251" s="23" t="s">
-        <v>666</v>
-      </c>
-      <c r="E251" s="21" t="s">
+      <c r="D251" s="27" t="s">
+        <v>669</v>
+      </c>
+      <c r="E251" s="16" t="s">
         <v>10</v>
       </c>
       <c r="F251" s="4"/>
     </row>
     <row r="252" ht="14.25">
       <c r="A252" s="20" t="s">
-        <v>667</v>
+        <v>670</v>
       </c>
       <c r="B252" s="9"/>
       <c r="C252" s="1"/>
-      <c r="D252" s="23" t="s">
-        <v>668</v>
-      </c>
-      <c r="E252" s="21" t="s">
+      <c r="D252" s="27" t="s">
+        <v>671</v>
+      </c>
+      <c r="E252" s="23" t="s">
         <v>10</v>
       </c>
       <c r="F252" s="4"/>
     </row>
     <row r="253" ht="14.25">
       <c r="A253" s="20" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
       <c r="B253" s="9"/>
       <c r="C253" s="1"/>
-      <c r="D253" s="23" t="s">
-        <v>670</v>
-      </c>
-      <c r="E253" s="21" t="s">
+      <c r="D253" s="27" t="s">
+        <v>673</v>
+      </c>
+      <c r="E253" s="23" t="s">
         <v>10</v>
       </c>
       <c r="F253" s="4"/>
     </row>
     <row r="254" ht="14.25">
       <c r="A254" s="20" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
       <c r="B254" s="9"/>
       <c r="C254" s="1"/>
-      <c r="D254" s="23" t="s">
-        <v>672</v>
-      </c>
-      <c r="E254" s="21" t="s">
+      <c r="D254" s="27" t="s">
+        <v>675</v>
+      </c>
+      <c r="E254" s="23" t="s">
         <v>10</v>
       </c>
       <c r="F254" s="4"/>
     </row>
     <row r="255" ht="14.25">
       <c r="A255" s="20" t="s">
-        <v>673</v>
+        <v>676</v>
       </c>
       <c r="B255" s="9"/>
       <c r="C255" s="1"/>
-      <c r="D255" s="23" t="s">
-        <v>672</v>
-      </c>
-      <c r="E255" s="21" t="s">
+      <c r="D255" s="27" t="s">
+        <v>677</v>
+      </c>
+      <c r="E255" s="23" t="s">
         <v>10</v>
       </c>
       <c r="F255" s="4"/>
     </row>
     <row r="256" ht="14.25">
       <c r="A256" s="20" t="s">
-        <v>674</v>
+        <v>678</v>
       </c>
       <c r="B256" s="9"/>
       <c r="C256" s="1"/>
-      <c r="D256" s="23" t="s">
-        <v>666</v>
-      </c>
-      <c r="E256" s="21" t="s">
+      <c r="D256" s="27" t="s">
+        <v>677</v>
+      </c>
+      <c r="E256" s="23" t="s">
         <v>10</v>
       </c>
       <c r="F256" s="4"/>
     </row>
     <row r="257" ht="14.25">
       <c r="A257" s="20" t="s">
-        <v>675</v>
+        <v>679</v>
       </c>
       <c r="B257" s="9"/>
       <c r="C257" s="1"/>
-      <c r="D257" s="23" t="s">
-        <v>676</v>
-      </c>
-      <c r="E257" s="21" t="s">
+      <c r="D257" s="27" t="s">
+        <v>671</v>
+      </c>
+      <c r="E257" s="23" t="s">
         <v>10</v>
       </c>
       <c r="F257" s="4"/>
     </row>
     <row r="258" ht="14.25">
       <c r="A258" s="20" t="s">
-        <v>677</v>
+        <v>680</v>
       </c>
       <c r="B258" s="9"/>
       <c r="C258" s="1"/>
-      <c r="D258" s="23" t="s">
-        <v>676</v>
-      </c>
-      <c r="E258" s="21" t="s">
+      <c r="D258" s="27" t="s">
+        <v>681</v>
+      </c>
+      <c r="E258" s="23" t="s">
         <v>10</v>
       </c>
       <c r="F258" s="4"/>
     </row>
     <row r="259" ht="14.25">
       <c r="A259" s="20" t="s">
-        <v>678</v>
+        <v>682</v>
       </c>
       <c r="B259" s="9"/>
       <c r="C259" s="1"/>
-      <c r="D259" s="23" t="s">
-        <v>679</v>
-      </c>
-      <c r="E259" s="22" t="s">
-        <v>66</v>
+      <c r="D259" s="27" t="s">
+        <v>681</v>
+      </c>
+      <c r="E259" s="23" t="s">
+        <v>10</v>
       </c>
       <c r="F259" s="4"/>
     </row>
     <row r="260" ht="14.25">
       <c r="A260" s="20" t="s">
-        <v>680</v>
+        <v>683</v>
       </c>
       <c r="B260" s="9"/>
       <c r="C260" s="1"/>
-      <c r="D260" s="23" t="s">
-        <v>676</v>
-      </c>
-      <c r="E260" s="21" t="s">
-        <v>10</v>
+      <c r="D260" s="27" t="s">
+        <v>684</v>
+      </c>
+      <c r="E260" s="25" t="s">
+        <v>66</v>
       </c>
       <c r="F260" s="4"/>
     </row>
     <row r="261" ht="14.25">
       <c r="A261" s="20" t="s">
-        <v>681</v>
+        <v>685</v>
       </c>
       <c r="B261" s="9"/>
       <c r="C261" s="1"/>
-      <c r="D261" s="23" t="s">
-        <v>682</v>
-      </c>
-      <c r="E261" s="22" t="s">
-        <v>66</v>
+      <c r="D261" s="27" t="s">
+        <v>681</v>
+      </c>
+      <c r="E261" s="23" t="s">
+        <v>10</v>
       </c>
       <c r="F261" s="4"/>
     </row>
     <row r="262" ht="14.25">
       <c r="A262" s="20" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="B262" s="9"/>
       <c r="C262" s="1"/>
-      <c r="D262" s="23" t="s">
-        <v>684</v>
-      </c>
-      <c r="E262" s="21" t="s">
-        <v>10</v>
+      <c r="D262" s="27" t="s">
+        <v>687</v>
+      </c>
+      <c r="E262" s="25" t="s">
+        <v>66</v>
       </c>
       <c r="F262" s="4"/>
     </row>
     <row r="263" ht="14.25">
       <c r="A263" s="20" t="s">
-        <v>449</v>
+        <v>688</v>
       </c>
       <c r="B263" s="9"/>
       <c r="C263" s="1"/>
-      <c r="D263" s="23" t="s">
-        <v>685</v>
-      </c>
-      <c r="E263" s="22" t="s">
-        <v>66</v>
+      <c r="D263" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="E263" s="23" t="s">
+        <v>10</v>
       </c>
       <c r="F263" s="4"/>
     </row>
     <row r="264" ht="14.25">
       <c r="A264" s="20" t="s">
-        <v>442</v>
+        <v>451</v>
       </c>
       <c r="B264" s="9"/>
       <c r="C264" s="1"/>
-      <c r="D264" s="23" t="s">
-        <v>686</v>
-      </c>
-      <c r="E264" s="21" t="s">
-        <v>10</v>
+      <c r="D264" s="27" t="s">
+        <v>690</v>
+      </c>
+      <c r="E264" s="25" t="s">
+        <v>66</v>
       </c>
       <c r="F264" s="4"/>
     </row>
     <row r="265" ht="14.25">
       <c r="A265" s="20" t="s">
-        <v>687</v>
+        <v>444</v>
       </c>
       <c r="B265" s="9"/>
       <c r="C265" s="1"/>
-      <c r="D265" s="23" t="s">
-        <v>688</v>
-      </c>
-      <c r="E265" s="22" t="s">
-        <v>66</v>
+      <c r="D265" s="27" t="s">
+        <v>691</v>
+      </c>
+      <c r="E265" s="23" t="s">
+        <v>10</v>
       </c>
       <c r="F265" s="4"/>
     </row>
     <row r="266" ht="14.25">
       <c r="A266" s="20" t="s">
-        <v>689</v>
+        <v>692</v>
       </c>
       <c r="B266" s="9"/>
       <c r="C266" s="1"/>
-      <c r="D266" s="23" t="s">
-        <v>690</v>
-      </c>
-      <c r="E266" s="21" t="s">
-        <v>10</v>
+      <c r="D266" s="27" t="s">
+        <v>693</v>
+      </c>
+      <c r="E266" s="25" t="s">
+        <v>66</v>
       </c>
       <c r="F266" s="4"/>
     </row>
     <row r="267" ht="14.25">
       <c r="A267" s="20" t="s">
-        <v>691</v>
+        <v>694</v>
       </c>
       <c r="B267" s="9"/>
       <c r="C267" s="1"/>
-      <c r="D267" s="23" t="s">
-        <v>692</v>
-      </c>
-      <c r="E267" s="21" t="s">
+      <c r="D267" s="27" t="s">
+        <v>695</v>
+      </c>
+      <c r="E267" s="23" t="s">
         <v>10</v>
       </c>
       <c r="F267" s="4"/>
     </row>
     <row r="268" ht="14.25">
       <c r="A268" s="20" t="s">
-        <v>693</v>
+        <v>696</v>
       </c>
       <c r="B268" s="9"/>
       <c r="C268" s="1"/>
-      <c r="D268" s="23" t="s">
-        <v>694</v>
-      </c>
-      <c r="E268" s="22" t="s">
-        <v>66</v>
+      <c r="D268" s="27" t="s">
+        <v>697</v>
+      </c>
+      <c r="E268" s="23" t="s">
+        <v>10</v>
       </c>
       <c r="F268" s="4"/>
     </row>
     <row r="269" ht="14.25">
       <c r="A269" s="20" t="s">
-        <v>695</v>
+        <v>698</v>
       </c>
       <c r="B269" s="9"/>
       <c r="C269" s="1"/>
-      <c r="D269" s="23" t="s">
-        <v>672</v>
-      </c>
-      <c r="E269" s="21" t="s">
-        <v>10</v>
+      <c r="D269" s="27" t="s">
+        <v>699</v>
+      </c>
+      <c r="E269" s="25" t="s">
+        <v>66</v>
       </c>
       <c r="F269" s="4"/>
     </row>
     <row r="270" ht="14.25">
       <c r="A270" s="20" t="s">
-        <v>696</v>
+        <v>700</v>
       </c>
       <c r="B270" s="9"/>
       <c r="C270" s="1"/>
-      <c r="D270" s="23" t="s">
-        <v>697</v>
-      </c>
-      <c r="E270" s="21" t="s">
+      <c r="D270" s="27" t="s">
+        <v>677</v>
+      </c>
+      <c r="E270" s="23" t="s">
         <v>10</v>
       </c>
       <c r="F270" s="4"/>
     </row>
     <row r="271" ht="14.25">
       <c r="A271" s="20" t="s">
-        <v>698</v>
+        <v>701</v>
       </c>
       <c r="B271" s="9"/>
       <c r="C271" s="1"/>
-      <c r="D271" s="23" t="s">
-        <v>672</v>
-      </c>
-      <c r="E271" s="21" t="s">
+      <c r="D271" s="27" t="s">
+        <v>702</v>
+      </c>
+      <c r="E271" s="23" t="s">
         <v>10</v>
       </c>
       <c r="F271" s="4"/>
     </row>
     <row r="272" ht="14.25">
       <c r="A272" s="20" t="s">
-        <v>699</v>
+        <v>703</v>
       </c>
       <c r="B272" s="9"/>
       <c r="C272" s="1"/>
-      <c r="D272" s="23" t="s">
-        <v>700</v>
-      </c>
-      <c r="E272" s="22" t="s">
-        <v>66</v>
+      <c r="D272" s="27" t="s">
+        <v>677</v>
+      </c>
+      <c r="E272" s="23" t="s">
+        <v>10</v>
       </c>
       <c r="F272" s="4"/>
     </row>
     <row r="273" ht="14.25">
       <c r="A273" s="20" t="s">
-        <v>701</v>
+        <v>704</v>
       </c>
       <c r="B273" s="9"/>
       <c r="C273" s="1"/>
-      <c r="D273" s="23" t="s">
-        <v>702</v>
-      </c>
-      <c r="E273" s="21" t="s">
-        <v>10</v>
+      <c r="D273" s="27" t="s">
+        <v>705</v>
+      </c>
+      <c r="E273" s="25" t="s">
+        <v>66</v>
       </c>
       <c r="F273" s="4"/>
     </row>
     <row r="274" ht="14.25">
       <c r="A274" s="20" t="s">
-        <v>703</v>
+        <v>706</v>
       </c>
       <c r="B274" s="9"/>
       <c r="C274" s="1"/>
-      <c r="D274" s="23" t="s">
-        <v>690</v>
-      </c>
-      <c r="E274" s="22" t="s">
-        <v>66</v>
+      <c r="D274" s="27" t="s">
+        <v>707</v>
+      </c>
+      <c r="E274" s="23" t="s">
+        <v>10</v>
       </c>
       <c r="F274" s="4"/>
     </row>
     <row r="275" ht="14.25">
       <c r="A275" s="20" t="s">
-        <v>704</v>
+        <v>708</v>
       </c>
       <c r="B275" s="9"/>
       <c r="C275" s="1"/>
-      <c r="D275" s="23" t="s">
-        <v>705</v>
-      </c>
-      <c r="E275" s="21" t="s">
-        <v>10</v>
+      <c r="D275" s="27" t="s">
+        <v>695</v>
+      </c>
+      <c r="E275" s="25" t="s">
+        <v>66</v>
       </c>
       <c r="F275" s="4"/>
     </row>
     <row r="276" ht="14.25">
       <c r="A276" s="20" t="s">
-        <v>706</v>
+        <v>709</v>
       </c>
       <c r="B276" s="9"/>
       <c r="C276" s="1"/>
-      <c r="D276" s="23" t="s">
-        <v>664</v>
-      </c>
-      <c r="E276" s="21" t="s">
+      <c r="D276" s="27" t="s">
+        <v>710</v>
+      </c>
+      <c r="E276" s="23" t="s">
         <v>10</v>
       </c>
       <c r="F276" s="4"/>
     </row>
     <row r="277" ht="14.25">
       <c r="A277" s="20" t="s">
-        <v>707</v>
+        <v>711</v>
       </c>
       <c r="B277" s="9"/>
       <c r="C277" s="1"/>
-      <c r="D277" s="23" t="s">
-        <v>708</v>
-      </c>
-      <c r="E277" s="22" t="s">
-        <v>66</v>
+      <c r="D277" s="27" t="s">
+        <v>669</v>
+      </c>
+      <c r="E277" s="23" t="s">
+        <v>10</v>
       </c>
       <c r="F277" s="4"/>
     </row>
     <row r="278" ht="14.25">
       <c r="A278" s="20" t="s">
-        <v>709</v>
+        <v>712</v>
       </c>
       <c r="B278" s="9"/>
       <c r="C278" s="1"/>
-      <c r="D278" s="23" t="s">
-        <v>710</v>
-      </c>
-      <c r="E278" s="22" t="s">
+      <c r="D278" s="27" t="s">
+        <v>713</v>
+      </c>
+      <c r="E278" s="25" t="s">
         <v>66</v>
       </c>
       <c r="F278" s="4"/>
     </row>
     <row r="279" ht="14.25">
       <c r="A279" s="20" t="s">
-        <v>711</v>
+        <v>714</v>
       </c>
       <c r="B279" s="9"/>
       <c r="C279" s="1"/>
-      <c r="D279" s="23" t="s">
-        <v>712</v>
-      </c>
-      <c r="E279" s="21" t="s">
-        <v>10</v>
+      <c r="D279" s="27" t="s">
+        <v>715</v>
+      </c>
+      <c r="E279" s="25" t="s">
+        <v>66</v>
       </c>
       <c r="F279" s="4"/>
     </row>
     <row r="280" ht="14.25">
       <c r="A280" s="20" t="s">
-        <v>713</v>
+        <v>716</v>
       </c>
       <c r="B280" s="9"/>
       <c r="C280" s="1"/>
-      <c r="D280" s="23" t="s">
-        <v>714</v>
-      </c>
-      <c r="E280" s="22" t="s">
-        <v>66</v>
+      <c r="D280" s="27" t="s">
+        <v>717</v>
+      </c>
+      <c r="E280" s="23" t="s">
+        <v>10</v>
       </c>
       <c r="F280" s="4"/>
     </row>
     <row r="281" ht="14.25">
       <c r="A281" s="20" t="s">
-        <v>715</v>
+        <v>718</v>
       </c>
       <c r="B281" s="9"/>
       <c r="C281" s="1"/>
-      <c r="D281" s="23" t="s">
-        <v>716</v>
-      </c>
-      <c r="E281" s="21" t="s">
-        <v>10</v>
+      <c r="D281" s="27" t="s">
+        <v>719</v>
+      </c>
+      <c r="E281" s="25" t="s">
+        <v>66</v>
       </c>
       <c r="F281" s="4"/>
     </row>
     <row r="282" ht="14.25">
       <c r="A282" s="20" t="s">
-        <v>717</v>
+        <v>720</v>
       </c>
       <c r="B282" s="9"/>
       <c r="C282" s="1"/>
-      <c r="D282" s="23" t="s">
-        <v>672</v>
-      </c>
-      <c r="E282" s="21" t="s">
+      <c r="D282" s="27" t="s">
+        <v>721</v>
+      </c>
+      <c r="E282" s="23" t="s">
         <v>10</v>
       </c>
       <c r="F282" s="4"/>
     </row>
     <row r="283" ht="14.25">
       <c r="A283" s="20" t="s">
-        <v>718</v>
+        <v>722</v>
       </c>
       <c r="B283" s="9"/>
       <c r="C283" s="1"/>
-      <c r="D283" s="23" t="s">
-        <v>719</v>
-      </c>
-      <c r="E283" s="21" t="s">
+      <c r="D283" s="27" t="s">
+        <v>677</v>
+      </c>
+      <c r="E283" s="23" t="s">
         <v>10</v>
       </c>
       <c r="F283" s="4"/>
     </row>
     <row r="284" ht="14.25">
       <c r="A284" s="20" t="s">
-        <v>502</v>
+        <v>723</v>
       </c>
       <c r="B284" s="9"/>
       <c r="C284" s="1"/>
-      <c r="D284" s="23" t="s">
-        <v>720</v>
-      </c>
-      <c r="E284" s="21" t="s">
+      <c r="D284" s="27" t="s">
+        <v>724</v>
+      </c>
+      <c r="E284" s="23" t="s">
         <v>10</v>
       </c>
       <c r="F284" s="4"/>
     </row>
     <row r="285" ht="14.25">
       <c r="A285" s="20" t="s">
-        <v>721</v>
+        <v>507</v>
       </c>
       <c r="B285" s="9"/>
       <c r="C285" s="1"/>
-      <c r="D285" s="23" t="s">
-        <v>722</v>
-      </c>
-      <c r="E285" s="22" t="s">
-        <v>66</v>
+      <c r="D285" s="27" t="s">
+        <v>725</v>
+      </c>
+      <c r="E285" s="23" t="s">
+        <v>10</v>
       </c>
       <c r="F285" s="4"/>
     </row>
     <row r="286" ht="14.25">
       <c r="A286" s="20" t="s">
-        <v>723</v>
+        <v>726</v>
       </c>
       <c r="B286" s="9"/>
       <c r="C286" s="1"/>
-      <c r="D286" s="23" t="s">
-        <v>724</v>
-      </c>
-      <c r="E286" s="21" t="s">
-        <v>10</v>
+      <c r="D286" s="27" t="s">
+        <v>727</v>
+      </c>
+      <c r="E286" s="25" t="s">
+        <v>66</v>
       </c>
       <c r="F286" s="4"/>
     </row>
     <row r="287" ht="14.25">
       <c r="A287" s="20" t="s">
-        <v>725</v>
+        <v>728</v>
       </c>
       <c r="B287" s="9"/>
       <c r="C287" s="1"/>
-      <c r="D287" s="23" t="s">
-        <v>726</v>
-      </c>
-      <c r="E287" s="21" t="s">
+      <c r="D287" s="27" t="s">
+        <v>729</v>
+      </c>
+      <c r="E287" s="23" t="s">
         <v>10</v>
       </c>
       <c r="F287" s="4"/>
     </row>
     <row r="288" ht="14.25">
       <c r="A288" s="20" t="s">
-        <v>727</v>
+        <v>730</v>
       </c>
       <c r="B288" s="9"/>
       <c r="C288" s="1"/>
-      <c r="D288" s="23" t="s">
-        <v>672</v>
-      </c>
-      <c r="E288" s="21" t="s">
+      <c r="D288" s="27" t="s">
+        <v>731</v>
+      </c>
+      <c r="E288" s="23" t="s">
         <v>10</v>
       </c>
       <c r="F288" s="4"/>
     </row>
     <row r="289" ht="14.25">
       <c r="A289" s="20" t="s">
-        <v>728</v>
+        <v>732</v>
       </c>
       <c r="B289" s="9"/>
       <c r="C289" s="1"/>
-      <c r="D289" s="23" t="s">
-        <v>692</v>
-      </c>
-      <c r="E289" s="22" t="s">
-        <v>66</v>
+      <c r="D289" s="27" t="s">
+        <v>677</v>
+      </c>
+      <c r="E289" s="23" t="s">
+        <v>10</v>
       </c>
       <c r="F289" s="4"/>
     </row>
     <row r="290" ht="14.25">
       <c r="A290" s="20" t="s">
-        <v>729</v>
+        <v>733</v>
       </c>
       <c r="B290" s="9"/>
       <c r="C290" s="1"/>
-      <c r="D290" s="23" t="s">
-        <v>730</v>
-      </c>
-      <c r="E290" s="16" t="s">
-        <v>10</v>
+      <c r="D290" s="27" t="s">
+        <v>697</v>
+      </c>
+      <c r="E290" s="25" t="s">
+        <v>66</v>
       </c>
       <c r="F290" s="4"/>
     </row>
     <row r="291" ht="14.25">
-      <c r="A291" s="4"/>
-      <c r="B291" s="4"/>
-      <c r="C291" s="4"/>
-      <c r="D291" s="4"/>
-      <c r="E291" s="4"/>
+      <c r="A291" s="20" t="s">
+        <v>734</v>
+      </c>
+      <c r="B291" s="9"/>
+      <c r="C291" s="1"/>
+      <c r="D291" s="27" t="s">
+        <v>735</v>
+      </c>
+      <c r="E291" s="16" t="s">
+        <v>10</v>
+      </c>
       <c r="F291" s="4"/>
     </row>
     <row r="292" ht="14.25">
-      <c r="C292"/>
-      <c r="D292"/>
-      <c r="E292"/>
-      <c r="F292"/>
+      <c r="A292" s="4"/>
+      <c r="B292" s="4"/>
+      <c r="C292" s="4"/>
+      <c r="D292" s="4"/>
+      <c r="E292" s="4"/>
+      <c r="F292" s="4"/>
     </row>
     <row r="293" ht="14.25">
       <c r="C293"/>
@@ -8648,7 +8693,7 @@
       <c r="F307"/>
     </row>
     <row r="308" ht="14.25">
-      <c r="C308" s="1"/>
+      <c r="C308"/>
       <c r="D308"/>
       <c r="E308"/>
       <c r="F308"/>
@@ -8726,6 +8771,7 @@
       <c r="F320"/>
     </row>
     <row r="321" ht="14.25">
+      <c r="C321" s="1"/>
       <c r="D321"/>
       <c r="E321"/>
       <c r="F321"/>
@@ -8785,7 +8831,11 @@
       <c r="E332"/>
       <c r="F332"/>
     </row>
-    <row r="333" ht="14.25"/>
+    <row r="333" ht="14.25">
+      <c r="D333"/>
+      <c r="E333"/>
+      <c r="F333"/>
+    </row>
     <row r="334" ht="14.25"/>
     <row r="335" ht="14.25"/>
     <row r="336" ht="14.25"/>
@@ -8795,6 +8845,7 @@
     <row r="340" ht="14.25"/>
     <row r="341" ht="14.25"/>
     <row r="342" ht="14.25"/>
+    <row r="343" ht="14.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="C5"/>
@@ -8913,11 +8964,12 @@
     <hyperlink r:id="rId114" ref="C130"/>
     <hyperlink r:id="rId115" ref="C131"/>
     <hyperlink r:id="rId116" ref="C132"/>
-    <hyperlink r:id="rId117" ref="C147"/>
-    <hyperlink r:id="rId118" ref="C148"/>
-    <hyperlink r:id="rId119" ref="C149"/>
-    <hyperlink r:id="rId120" ref="C150"/>
-    <hyperlink r:id="rId121" ref="C151"/>
+    <hyperlink r:id="rId117" ref="C148"/>
+    <hyperlink r:id="rId118" ref="C149"/>
+    <hyperlink r:id="rId119" ref="C150"/>
+    <hyperlink r:id="rId120" ref="C151"/>
+    <hyperlink r:id="rId121" ref="C152"/>
+    <hyperlink r:id="rId122" ref="C153"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
vault backup: 2026-01-07 21:13:28
</commit_message>
<xml_diff>
--- a/Excalidraw/switch.xlsx
+++ b/Excalidraw/switch.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="736">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="737">
   <si>
     <t>DSA</t>
   </si>
@@ -1430,11 +1430,10 @@
     <t xml:space="preserve">Design a Distributed Cache (Redis)</t>
   </si>
   <si>
-    <t xml:space="preserve">Lets take the assumptions - 
-functional requirements - 
-1. Users should be able to store the value (string) via keys (string), get them, overwride them
-2. Each key value pair should have a time to live, eviction can be based of LRU or LFU algorithms
-3. </t>
+    <t xml:space="preserve">decentralized, highly available, low-latency distributed in-memory cache using consistent hashing, quorum-based replication, gossip-based membership, and local eviction strategies, prioritizing availability and performance over strong consistency</t>
+  </si>
+  <si>
+    <t>https://github.com/yashaggarwal85d/Neural-Vault/blob/main/Excalidraw/Design%20a%20Distributed%20Cache%20(Redis).md</t>
   </si>
   <si>
     <t xml:space="preserve">Design a Notification Service</t>
@@ -2439,7 +2438,7 @@
     <xf fontId="6" fillId="12" borderId="2" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="3" fillId="13" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="3" fillId="8" borderId="0" numFmtId="0" xfId="7" applyFont="1" applyFill="1"/>
     <xf fontId="3" fillId="7" borderId="0" numFmtId="0" xfId="6" applyFont="1" applyFill="1"/>
@@ -2479,8 +2478,6 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="4" fillId="9" borderId="0" numFmtId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2977,7 +2974,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A140" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A131" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -6502,17 +6499,17 @@
       <c r="E141"/>
       <c r="F141"/>
     </row>
-    <row r="142" ht="71.25">
-      <c r="A142" s="21" t="s">
+    <row r="142" ht="28.5">
+      <c r="A142" s="7" t="s">
         <v>440</v>
       </c>
       <c r="B142" s="12" t="s">
         <v>441</v>
       </c>
-      <c r="C142" s="22"/>
-      <c r="D142" s="22"/>
-      <c r="E142" s="22"/>
-      <c r="F142" s="22"/>
+      <c r="C142" s="6"/>
+      <c r="D142" s="6"/>
+      <c r="E142" s="6"/>
+      <c r="F142" s="6"/>
     </row>
     <row r="143" ht="14.25">
       <c r="B143" s="9"/>
@@ -6631,7 +6628,7 @@
       <c r="D149" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="E149" s="23" t="s">
+      <c r="E149" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F149" s="4"/>
@@ -6649,7 +6646,7 @@
       <c r="D150" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="E150" s="23" t="s">
+      <c r="E150" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F150" s="4"/>
@@ -6667,7 +6664,7 @@
       <c r="D151" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="E151" s="23" t="s">
+      <c r="E151" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F151" s="4"/>
@@ -6685,7 +6682,7 @@
       <c r="D152" s="2" t="s">
         <v>462</v>
       </c>
-      <c r="E152" s="23" t="s">
+      <c r="E152" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F152" s="4"/>
@@ -6694,7 +6691,7 @@
       <c r="A153" s="10" t="s">
         <v>463</v>
       </c>
-      <c r="B153" s="24" t="s">
+      <c r="B153" s="22" t="s">
         <v>464</v>
       </c>
       <c r="C153" s="11" t="s">
@@ -6703,556 +6700,558 @@
       <c r="D153" s="2" t="s">
         <v>466</v>
       </c>
-      <c r="E153" s="25" t="s">
+      <c r="E153" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F153" s="4"/>
     </row>
-    <row r="154" ht="14.25">
-      <c r="A154" t="s">
+    <row r="154" ht="42.75">
+      <c r="A154" s="7" t="s">
         <v>467</v>
       </c>
       <c r="B154" s="12" t="s">
         <v>468</v>
       </c>
-      <c r="C154" s="1"/>
+      <c r="C154" s="11" t="s">
+        <v>469</v>
+      </c>
       <c r="D154" s="2" t="s">
         <v>466</v>
       </c>
-      <c r="E154" s="25" t="s">
+      <c r="E154" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F154" s="4"/>
     </row>
     <row r="155" ht="14.25">
       <c r="A155" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B155" s="9"/>
       <c r="C155" s="1"/>
       <c r="D155" s="2" t="s">
-        <v>470</v>
-      </c>
-      <c r="E155" s="23" t="s">
+        <v>471</v>
+      </c>
+      <c r="E155" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F155" s="4"/>
     </row>
     <row r="156" ht="14.25">
       <c r="A156" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B156" s="9"/>
       <c r="C156" s="1"/>
       <c r="D156" s="2" t="s">
-        <v>470</v>
-      </c>
-      <c r="E156" s="25" t="s">
+        <v>471</v>
+      </c>
+      <c r="E156" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F156" s="4"/>
     </row>
     <row r="157" ht="14.25">
       <c r="A157" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="B157" s="9"/>
       <c r="C157" s="1"/>
       <c r="D157" s="2" t="s">
-        <v>473</v>
-      </c>
-      <c r="E157" s="25" t="s">
+        <v>474</v>
+      </c>
+      <c r="E157" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F157" s="4"/>
     </row>
     <row r="158" ht="14.25">
       <c r="A158" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B158" s="9"/>
       <c r="C158" s="1"/>
       <c r="D158" s="2" t="s">
-        <v>475</v>
-      </c>
-      <c r="E158" s="25" t="s">
+        <v>476</v>
+      </c>
+      <c r="E158" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F158" s="4"/>
     </row>
     <row r="159" ht="14.25">
       <c r="A159" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B159" s="9"/>
       <c r="C159" s="1"/>
       <c r="D159" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="E159" s="25" t="s">
+        <v>478</v>
+      </c>
+      <c r="E159" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F159" s="4"/>
     </row>
     <row r="160" ht="14.25">
       <c r="A160" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B160" s="9"/>
       <c r="C160" s="1"/>
       <c r="D160" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="E160" s="25" t="s">
+        <v>480</v>
+      </c>
+      <c r="E160" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F160" s="4"/>
       <c r="L160" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="161" ht="14.25">
       <c r="A161" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B161" s="9"/>
       <c r="C161" s="1"/>
       <c r="D161" s="2" t="s">
-        <v>482</v>
-      </c>
-      <c r="E161" s="23" t="s">
+        <v>483</v>
+      </c>
+      <c r="E161" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F161" s="4"/>
     </row>
     <row r="162" ht="14.25">
       <c r="A162" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B162" s="9"/>
       <c r="C162" s="1"/>
       <c r="D162" s="2" t="s">
-        <v>484</v>
-      </c>
-      <c r="E162" s="23" t="s">
+        <v>485</v>
+      </c>
+      <c r="E162" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F162" s="4"/>
     </row>
     <row r="163" ht="14.25">
       <c r="A163" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="B163" s="9"/>
       <c r="C163" s="1"/>
       <c r="D163" s="2" t="s">
-        <v>486</v>
-      </c>
-      <c r="E163" s="25" t="s">
+        <v>487</v>
+      </c>
+      <c r="E163" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F163" s="4"/>
     </row>
     <row r="164" ht="14.25">
-      <c r="A164" s="26" t="s">
-        <v>487</v>
+      <c r="A164" s="24" t="s">
+        <v>488</v>
       </c>
       <c r="B164" s="9"/>
       <c r="C164" s="1"/>
       <c r="D164" s="2" t="s">
-        <v>488</v>
-      </c>
-      <c r="E164" s="23" t="s">
+        <v>489</v>
+      </c>
+      <c r="E164" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F164" s="4"/>
     </row>
     <row r="165" ht="14.25">
       <c r="A165" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B165" s="9"/>
       <c r="C165" s="1"/>
       <c r="D165" s="2" t="s">
-        <v>490</v>
-      </c>
-      <c r="E165" s="23" t="s">
+        <v>491</v>
+      </c>
+      <c r="E165" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F165" s="4"/>
     </row>
     <row r="166" ht="14.25">
       <c r="A166" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B166" s="9"/>
       <c r="C166" s="1"/>
       <c r="D166" s="2" t="s">
-        <v>492</v>
-      </c>
-      <c r="E166" s="23" t="s">
+        <v>493</v>
+      </c>
+      <c r="E166" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F166" s="4"/>
     </row>
     <row r="167" ht="14.25">
       <c r="A167" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B167" s="9"/>
       <c r="C167" s="1"/>
       <c r="D167" s="2" t="s">
-        <v>494</v>
-      </c>
-      <c r="E167" s="25" t="s">
+        <v>495</v>
+      </c>
+      <c r="E167" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F167" s="4"/>
     </row>
     <row r="168" ht="14.25">
       <c r="A168" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B168" s="9"/>
       <c r="C168" s="1"/>
       <c r="D168" s="2" t="s">
-        <v>496</v>
-      </c>
-      <c r="E168" s="25" t="s">
+        <v>497</v>
+      </c>
+      <c r="E168" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F168" s="4"/>
     </row>
     <row r="169" ht="14.25">
       <c r="A169" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B169" s="9"/>
       <c r="C169" s="1"/>
       <c r="D169" s="2" t="s">
-        <v>498</v>
-      </c>
-      <c r="E169" s="25" t="s">
+        <v>499</v>
+      </c>
+      <c r="E169" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F169" s="4"/>
     </row>
     <row r="170" ht="14.25">
       <c r="A170" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B170" s="9"/>
       <c r="C170" s="1"/>
       <c r="D170" s="2" t="s">
-        <v>500</v>
-      </c>
-      <c r="E170" s="25" t="s">
+        <v>501</v>
+      </c>
+      <c r="E170" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F170" s="4"/>
     </row>
     <row r="171" ht="14.25">
       <c r="A171" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="B171" s="9"/>
       <c r="C171" s="1"/>
       <c r="D171" s="2" t="s">
-        <v>502</v>
-      </c>
-      <c r="E171" s="25" t="s">
+        <v>503</v>
+      </c>
+      <c r="E171" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F171" s="4"/>
     </row>
     <row r="172" ht="14.25">
       <c r="A172" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B172" s="9"/>
       <c r="C172" s="1"/>
       <c r="D172" s="2" t="s">
-        <v>504</v>
-      </c>
-      <c r="E172" s="23" t="s">
+        <v>505</v>
+      </c>
+      <c r="E172" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F172" s="4"/>
     </row>
     <row r="173" ht="14.25">
       <c r="A173" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="B173" s="9"/>
       <c r="C173" s="1"/>
       <c r="D173" s="2" t="s">
-        <v>506</v>
-      </c>
-      <c r="E173" s="23" t="s">
+        <v>507</v>
+      </c>
+      <c r="E173" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F173" s="4"/>
     </row>
     <row r="174" ht="14.25">
       <c r="A174" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="B174" s="9"/>
       <c r="C174" s="1"/>
       <c r="D174" s="2" t="s">
-        <v>508</v>
-      </c>
-      <c r="E174" s="23" t="s">
+        <v>509</v>
+      </c>
+      <c r="E174" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F174" s="4"/>
     </row>
     <row r="175" ht="14.25">
       <c r="A175" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B175" s="9"/>
       <c r="C175" s="1"/>
       <c r="D175" s="2" t="s">
-        <v>510</v>
-      </c>
-      <c r="E175" s="25" t="s">
+        <v>511</v>
+      </c>
+      <c r="E175" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F175" s="4"/>
     </row>
     <row r="176" ht="14.25">
       <c r="A176" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B176" s="9"/>
       <c r="C176" s="1"/>
       <c r="D176" s="2" t="s">
-        <v>512</v>
-      </c>
-      <c r="E176" s="25" t="s">
+        <v>513</v>
+      </c>
+      <c r="E176" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F176" s="4"/>
     </row>
     <row r="177" ht="14.25">
       <c r="A177" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B177" s="9"/>
       <c r="C177" s="1"/>
       <c r="D177" s="2" t="s">
-        <v>514</v>
-      </c>
-      <c r="E177" s="25" t="s">
+        <v>515</v>
+      </c>
+      <c r="E177" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F177" s="4"/>
     </row>
     <row r="178" ht="14.25">
       <c r="A178" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B178" s="9"/>
       <c r="C178" s="1"/>
       <c r="D178" s="2" t="s">
-        <v>516</v>
-      </c>
-      <c r="E178" s="23" t="s">
+        <v>517</v>
+      </c>
+      <c r="E178" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F178" s="4"/>
     </row>
     <row r="179" ht="14.25">
       <c r="A179" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B179" s="9"/>
       <c r="C179" s="1"/>
       <c r="D179" s="2" t="s">
-        <v>518</v>
-      </c>
-      <c r="E179" s="25" t="s">
+        <v>519</v>
+      </c>
+      <c r="E179" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F179" s="4"/>
     </row>
     <row r="180" ht="14.25">
       <c r="A180" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="B180" s="9"/>
       <c r="C180" s="1"/>
       <c r="D180" s="2" t="s">
-        <v>520</v>
-      </c>
-      <c r="E180" s="23" t="s">
+        <v>521</v>
+      </c>
+      <c r="E180" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F180" s="4"/>
     </row>
     <row r="181" ht="14.25">
       <c r="A181" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B181" s="9"/>
       <c r="C181" s="1"/>
       <c r="D181" s="2" t="s">
-        <v>522</v>
-      </c>
-      <c r="E181" s="25" t="s">
+        <v>523</v>
+      </c>
+      <c r="E181" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F181" s="4"/>
     </row>
     <row r="182" ht="14.25">
       <c r="A182" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B182" s="9"/>
       <c r="C182" s="1"/>
       <c r="D182" s="2" t="s">
-        <v>524</v>
-      </c>
-      <c r="E182" s="23" t="s">
+        <v>525</v>
+      </c>
+      <c r="E182" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F182" s="4"/>
     </row>
     <row r="183" ht="14.25">
       <c r="A183" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="B183" s="9"/>
       <c r="C183" s="1"/>
       <c r="D183" s="2" t="s">
-        <v>526</v>
-      </c>
-      <c r="E183" s="23" t="s">
+        <v>527</v>
+      </c>
+      <c r="E183" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F183" s="4"/>
     </row>
     <row r="184" ht="14.25">
       <c r="A184" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B184" s="9"/>
       <c r="C184" s="1"/>
       <c r="D184" s="2" t="s">
-        <v>528</v>
-      </c>
-      <c r="E184" s="25" t="s">
+        <v>529</v>
+      </c>
+      <c r="E184" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F184" s="4"/>
     </row>
     <row r="185" ht="14.25">
       <c r="A185" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B185" s="9"/>
       <c r="C185" s="1"/>
       <c r="D185" s="2" t="s">
-        <v>530</v>
-      </c>
-      <c r="E185" s="25" t="s">
+        <v>531</v>
+      </c>
+      <c r="E185" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F185" s="4"/>
     </row>
     <row r="186" ht="14.25">
       <c r="A186" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="B186" s="9"/>
       <c r="C186" s="1"/>
       <c r="D186" s="2" t="s">
-        <v>532</v>
-      </c>
-      <c r="E186" s="25" t="s">
+        <v>533</v>
+      </c>
+      <c r="E186" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F186" s="4"/>
     </row>
     <row r="187" ht="14.25">
       <c r="A187" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="B187" s="9"/>
       <c r="C187" s="1"/>
       <c r="D187" s="2" t="s">
-        <v>534</v>
-      </c>
-      <c r="E187" s="25" t="s">
+        <v>535</v>
+      </c>
+      <c r="E187" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F187" s="4"/>
     </row>
     <row r="188" ht="14.25">
       <c r="A188" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="B188" s="9"/>
       <c r="C188" s="1"/>
       <c r="D188" s="2" t="s">
-        <v>536</v>
-      </c>
-      <c r="E188" s="23" t="s">
+        <v>537</v>
+      </c>
+      <c r="E188" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F188" s="4"/>
     </row>
     <row r="189" ht="14.25">
       <c r="A189" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="B189" s="9"/>
       <c r="C189" s="1"/>
       <c r="D189" s="2" t="s">
-        <v>538</v>
-      </c>
-      <c r="E189" s="25" t="s">
+        <v>539</v>
+      </c>
+      <c r="E189" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F189" s="4"/>
     </row>
     <row r="190" ht="14.25">
       <c r="A190" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="B190" s="9"/>
       <c r="C190" s="1"/>
       <c r="D190" s="2" t="s">
-        <v>540</v>
-      </c>
-      <c r="E190" s="23" t="s">
+        <v>541</v>
+      </c>
+      <c r="E190" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F190" s="4"/>
     </row>
     <row r="191" ht="14.25">
       <c r="A191" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="B191" s="9"/>
       <c r="C191" s="1"/>
       <c r="D191" s="2" t="s">
-        <v>542</v>
-      </c>
-      <c r="E191" s="25" t="s">
+        <v>543</v>
+      </c>
+      <c r="E191" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F191" s="4"/>
     </row>
     <row r="192" ht="14.25">
       <c r="A192" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="B192" s="9"/>
       <c r="C192" s="1"/>
       <c r="D192" s="2" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="E192" s="18" t="s">
         <v>66</v>
@@ -7275,7 +7274,7 @@
     </row>
     <row r="195" ht="14.25">
       <c r="A195" s="5" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B195" s="5"/>
       <c r="C195" s="5"/>
@@ -7285,619 +7284,619 @@
     </row>
     <row r="196" ht="14.25">
       <c r="A196" s="4" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="B196" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C196" s="4" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="D196" s="4" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="E196" s="4"/>
       <c r="F196" s="4"/>
     </row>
     <row r="197" ht="14.25">
       <c r="A197" s="20" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="B197" s="9"/>
       <c r="C197" s="1" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="F197" s="4"/>
     </row>
     <row r="198" ht="14.25">
       <c r="A198" s="20" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B198" s="9"/>
       <c r="C198" s="1" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="F198" s="4"/>
       <c r="H198" s="6"/>
     </row>
     <row r="199" ht="14.25">
       <c r="A199" s="20" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="B199" s="9"/>
       <c r="C199" s="1" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="D199" s="2" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="F199" s="4"/>
     </row>
     <row r="200" ht="14.25">
       <c r="A200" s="20" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="B200" s="9"/>
       <c r="C200" s="1" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="F200" s="4"/>
     </row>
     <row r="201" ht="14.25">
       <c r="A201" s="20" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B201" s="9"/>
       <c r="C201" s="1" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="F201" s="4"/>
     </row>
     <row r="202" ht="14.25">
       <c r="A202" s="20" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="B202" s="9"/>
       <c r="C202" s="1" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="F202" s="4"/>
     </row>
     <row r="203" ht="14.25">
       <c r="A203" s="20" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="B203" s="9"/>
       <c r="C203" s="1" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="D203" s="2" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="F203" s="4"/>
       <c r="H203" s="6"/>
     </row>
     <row r="204" ht="14.25">
       <c r="A204" s="20" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="B204" s="9"/>
       <c r="C204" s="1" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="F204" s="4"/>
       <c r="H204" s="6"/>
     </row>
     <row r="205" ht="14.25">
       <c r="A205" s="20" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="B205" s="9"/>
       <c r="C205" s="1" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="D205" s="2" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="F205" s="4"/>
       <c r="H205" s="6"/>
     </row>
     <row r="206" ht="14.25">
       <c r="A206" s="20" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="B206" s="9"/>
       <c r="C206" s="1" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="D206" s="2" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="F206" s="4"/>
       <c r="H206" s="6"/>
     </row>
     <row r="207" ht="14.25">
       <c r="A207" s="20" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="B207" s="9"/>
       <c r="C207" s="1" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="D207" s="2" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="F207" s="4"/>
       <c r="H207" s="6"/>
     </row>
     <row r="208" ht="14.25">
       <c r="A208" s="20" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="B208" s="9"/>
       <c r="C208" s="1" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="D208" s="2" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="F208" s="4"/>
       <c r="H208" s="6"/>
     </row>
     <row r="209" ht="14.25">
       <c r="A209" s="20" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="B209" s="9"/>
       <c r="C209" s="1" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="F209" s="4"/>
       <c r="H209" s="6"/>
     </row>
     <row r="210" ht="14.25">
       <c r="A210" s="20" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="B210" s="9"/>
       <c r="C210" s="1" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="F210" s="4"/>
     </row>
     <row r="211" ht="14.25">
       <c r="A211" s="20" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="B211" s="9"/>
       <c r="C211" s="1" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D211" s="2" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="F211" s="4"/>
     </row>
     <row r="212" ht="14.25">
       <c r="A212" s="20" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="B212" s="9"/>
       <c r="C212" s="1" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="D212" s="2" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="F212" s="4"/>
     </row>
     <row r="213" ht="14.25">
       <c r="A213" s="20" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="B213" s="9"/>
       <c r="C213" s="1" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="D213" s="2" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="F213" s="4"/>
     </row>
     <row r="214" ht="14.25">
       <c r="A214" s="20" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="B214" s="9"/>
       <c r="C214" s="1" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="D214" s="2" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="F214" s="4"/>
     </row>
     <row r="215" ht="14.25">
       <c r="A215" s="20" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="B215" s="9"/>
       <c r="C215" s="1" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="F215" s="4"/>
     </row>
     <row r="216" ht="14.25">
       <c r="A216" s="20" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="B216" s="9"/>
       <c r="C216" s="1" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="D216" s="2" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="F216" s="4"/>
     </row>
     <row r="217" ht="14.25">
       <c r="A217" s="20" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="B217" s="9"/>
       <c r="C217" s="1" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="F217" s="4"/>
     </row>
     <row r="218" ht="14.25">
       <c r="A218" s="20" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="B218" s="9"/>
       <c r="C218" s="1" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="F218" s="4"/>
     </row>
     <row r="219" ht="14.25">
       <c r="A219" s="20" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="B219" s="9"/>
       <c r="C219" s="1" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="F219" s="4"/>
     </row>
     <row r="220" ht="14.25">
       <c r="A220" s="20" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="B220" s="9"/>
       <c r="C220" s="1" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="D220" s="2" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="F220" s="4"/>
     </row>
     <row r="221" ht="14.25">
       <c r="A221" s="20" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="B221" s="9"/>
       <c r="C221" s="1" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="D221" s="2" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="F221" s="4"/>
     </row>
     <row r="222" ht="14.25">
       <c r="A222" s="20" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="B222" s="9"/>
       <c r="C222" s="1" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="D222" s="2" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="F222" s="4"/>
     </row>
     <row r="223" ht="14.25">
       <c r="A223" s="20" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="B223" s="9"/>
       <c r="C223" s="1" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="D223" s="2" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="F223" s="4"/>
     </row>
     <row r="224" ht="14.25">
       <c r="A224" s="20" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="B224" s="9"/>
       <c r="C224" s="1" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="D224" s="2" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="F224" s="4"/>
     </row>
     <row r="225" ht="14.25">
       <c r="A225" s="20" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="B225" s="9"/>
       <c r="C225" s="1" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="D225" s="2" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="F225" s="4"/>
     </row>
     <row r="226" ht="14.25">
       <c r="A226" s="20" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="B226" s="9"/>
       <c r="C226" s="1" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="D226" s="2" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="F226" s="4"/>
     </row>
     <row r="227" ht="14.25">
       <c r="A227" s="20" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="B227" s="9"/>
       <c r="C227" s="1" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="D227" s="2" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="F227" s="4"/>
     </row>
     <row r="228" ht="14.25">
       <c r="A228" s="20" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="B228" s="9"/>
       <c r="C228" s="1" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D228" s="2" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="F228" s="4"/>
     </row>
     <row r="229" ht="14.25">
       <c r="A229" s="20" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="B229" s="9"/>
       <c r="C229" s="1" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="D229" s="2" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="F229" s="4"/>
     </row>
     <row r="230" ht="14.25">
       <c r="A230" s="20" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="B230" s="9"/>
       <c r="C230" s="1" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="D230" s="2" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="F230" s="4"/>
     </row>
     <row r="231" ht="14.25">
       <c r="A231" s="20" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="B231" s="9"/>
       <c r="C231" s="1" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="D231" s="2" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="F231" s="4"/>
     </row>
     <row r="232" ht="14.25">
       <c r="A232" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="B232" s="9"/>
       <c r="C232" s="1" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="D232" s="2" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="F232" s="4"/>
       <c r="H232" s="6"/>
     </row>
     <row r="233" ht="14.25">
       <c r="A233" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="B233" s="9"/>
       <c r="C233" s="1" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="D233" s="2" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="F233" s="4"/>
       <c r="H233" s="6"/>
     </row>
     <row r="234" ht="14.25">
       <c r="A234" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="B234" s="9"/>
       <c r="C234" s="1" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="D234" s="2" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="F234" s="4"/>
       <c r="H234" s="6"/>
     </row>
     <row r="235" ht="14.25">
       <c r="A235" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="B235" s="9"/>
       <c r="C235" s="1" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="D235" s="2" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="F235" s="4"/>
       <c r="H235" s="6"/>
     </row>
     <row r="236" ht="14.25">
       <c r="A236" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="B236" s="9"/>
       <c r="C236" s="1" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="D236" s="2" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="F236" s="4"/>
       <c r="H236" s="6"/>
     </row>
     <row r="237" ht="14.25">
       <c r="A237" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="B237" s="9"/>
       <c r="C237" s="1" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="D237" s="2" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="F237" s="4"/>
       <c r="H237" s="6"/>
     </row>
     <row r="238" ht="14.25">
       <c r="A238" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="B238" s="9"/>
       <c r="C238" s="1" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="D238" s="2" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="F238" s="4"/>
       <c r="H238" s="6"/>
     </row>
     <row r="239" ht="14.25">
       <c r="A239" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="B239" s="9"/>
       <c r="C239" s="1" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="D239" s="2" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="F239" s="4"/>
       <c r="H239" s="6"/>
     </row>
     <row r="240" ht="14.25">
       <c r="A240" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="B240" s="9"/>
       <c r="C240" s="1" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="D240" s="2" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="F240" s="4"/>
       <c r="H240" s="6"/>
     </row>
     <row r="241" ht="14.25">
       <c r="A241" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="B241" s="9"/>
       <c r="C241" s="1" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="D241" s="2" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="E241" s="3"/>
       <c r="F241" s="4"/>
@@ -7905,14 +7904,14 @@
     </row>
     <row r="242" ht="14.25">
       <c r="A242" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="B242" s="9"/>
       <c r="C242" s="1" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="D242" s="2" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="E242" s="3"/>
       <c r="F242" s="4"/>
@@ -7920,14 +7919,14 @@
     </row>
     <row r="243" ht="14.25">
       <c r="A243" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="B243" s="9"/>
       <c r="C243" s="1" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="D243" s="2" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="E243" s="3"/>
       <c r="F243" s="4"/>
@@ -7935,14 +7934,14 @@
     </row>
     <row r="244" ht="14.25">
       <c r="A244" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="B244" s="9"/>
       <c r="C244" s="1" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="D244" s="2" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="E244" s="3"/>
       <c r="F244" s="4"/>
@@ -7950,14 +7949,14 @@
     </row>
     <row r="245" ht="14.25">
       <c r="A245" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="B245" s="9"/>
       <c r="C245" s="1" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="D245" s="2" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="E245" s="3"/>
       <c r="F245" s="4"/>
@@ -7965,14 +7964,14 @@
     </row>
     <row r="246" ht="14.25">
       <c r="A246" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="B246" s="9"/>
       <c r="C246" s="1" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="D246" s="2" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="E246" s="3"/>
       <c r="F246" s="4"/>
@@ -7994,7 +7993,7 @@
     </row>
     <row r="249" ht="14.25">
       <c r="A249" s="5" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="B249" s="5"/>
       <c r="C249" s="5"/>
@@ -8022,12 +8021,12 @@
     </row>
     <row r="251" ht="14.25">
       <c r="A251" s="20" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="B251" s="9"/>
       <c r="C251" s="1"/>
-      <c r="D251" s="27" t="s">
-        <v>669</v>
+      <c r="D251" s="25" t="s">
+        <v>670</v>
       </c>
       <c r="E251" s="16" t="s">
         <v>10</v>
@@ -8036,168 +8035,168 @@
     </row>
     <row r="252" ht="14.25">
       <c r="A252" s="20" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="B252" s="9"/>
       <c r="C252" s="1"/>
-      <c r="D252" s="27" t="s">
-        <v>671</v>
-      </c>
-      <c r="E252" s="23" t="s">
+      <c r="D252" s="25" t="s">
+        <v>672</v>
+      </c>
+      <c r="E252" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F252" s="4"/>
     </row>
     <row r="253" ht="14.25">
       <c r="A253" s="20" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="B253" s="9"/>
       <c r="C253" s="1"/>
-      <c r="D253" s="27" t="s">
-        <v>673</v>
-      </c>
-      <c r="E253" s="23" t="s">
+      <c r="D253" s="25" t="s">
+        <v>674</v>
+      </c>
+      <c r="E253" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F253" s="4"/>
     </row>
     <row r="254" ht="14.25">
       <c r="A254" s="20" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="B254" s="9"/>
       <c r="C254" s="1"/>
-      <c r="D254" s="27" t="s">
-        <v>675</v>
-      </c>
-      <c r="E254" s="23" t="s">
+      <c r="D254" s="25" t="s">
+        <v>676</v>
+      </c>
+      <c r="E254" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F254" s="4"/>
     </row>
     <row r="255" ht="14.25">
       <c r="A255" s="20" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="B255" s="9"/>
       <c r="C255" s="1"/>
-      <c r="D255" s="27" t="s">
-        <v>677</v>
-      </c>
-      <c r="E255" s="23" t="s">
+      <c r="D255" s="25" t="s">
+        <v>678</v>
+      </c>
+      <c r="E255" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F255" s="4"/>
     </row>
     <row r="256" ht="14.25">
       <c r="A256" s="20" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="B256" s="9"/>
       <c r="C256" s="1"/>
-      <c r="D256" s="27" t="s">
-        <v>677</v>
-      </c>
-      <c r="E256" s="23" t="s">
+      <c r="D256" s="25" t="s">
+        <v>678</v>
+      </c>
+      <c r="E256" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F256" s="4"/>
     </row>
     <row r="257" ht="14.25">
       <c r="A257" s="20" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="B257" s="9"/>
       <c r="C257" s="1"/>
-      <c r="D257" s="27" t="s">
-        <v>671</v>
-      </c>
-      <c r="E257" s="23" t="s">
+      <c r="D257" s="25" t="s">
+        <v>672</v>
+      </c>
+      <c r="E257" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F257" s="4"/>
     </row>
     <row r="258" ht="14.25">
       <c r="A258" s="20" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="B258" s="9"/>
       <c r="C258" s="1"/>
-      <c r="D258" s="27" t="s">
-        <v>681</v>
-      </c>
-      <c r="E258" s="23" t="s">
+      <c r="D258" s="25" t="s">
+        <v>682</v>
+      </c>
+      <c r="E258" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F258" s="4"/>
     </row>
     <row r="259" ht="14.25">
       <c r="A259" s="20" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="B259" s="9"/>
       <c r="C259" s="1"/>
-      <c r="D259" s="27" t="s">
-        <v>681</v>
-      </c>
-      <c r="E259" s="23" t="s">
+      <c r="D259" s="25" t="s">
+        <v>682</v>
+      </c>
+      <c r="E259" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F259" s="4"/>
     </row>
     <row r="260" ht="14.25">
       <c r="A260" s="20" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="B260" s="9"/>
       <c r="C260" s="1"/>
-      <c r="D260" s="27" t="s">
-        <v>684</v>
-      </c>
-      <c r="E260" s="25" t="s">
+      <c r="D260" s="25" t="s">
+        <v>685</v>
+      </c>
+      <c r="E260" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F260" s="4"/>
     </row>
     <row r="261" ht="14.25">
       <c r="A261" s="20" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="B261" s="9"/>
       <c r="C261" s="1"/>
-      <c r="D261" s="27" t="s">
-        <v>681</v>
-      </c>
-      <c r="E261" s="23" t="s">
+      <c r="D261" s="25" t="s">
+        <v>682</v>
+      </c>
+      <c r="E261" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F261" s="4"/>
     </row>
     <row r="262" ht="14.25">
       <c r="A262" s="20" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="B262" s="9"/>
       <c r="C262" s="1"/>
-      <c r="D262" s="27" t="s">
-        <v>687</v>
-      </c>
-      <c r="E262" s="25" t="s">
+      <c r="D262" s="25" t="s">
+        <v>688</v>
+      </c>
+      <c r="E262" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F262" s="4"/>
     </row>
     <row r="263" ht="14.25">
       <c r="A263" s="20" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="B263" s="9"/>
       <c r="C263" s="1"/>
-      <c r="D263" s="27" t="s">
-        <v>689</v>
-      </c>
-      <c r="E263" s="23" t="s">
+      <c r="D263" s="25" t="s">
+        <v>690</v>
+      </c>
+      <c r="E263" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F263" s="4"/>
@@ -8208,10 +8207,10 @@
       </c>
       <c r="B264" s="9"/>
       <c r="C264" s="1"/>
-      <c r="D264" s="27" t="s">
-        <v>690</v>
-      </c>
-      <c r="E264" s="25" t="s">
+      <c r="D264" s="25" t="s">
+        <v>691</v>
+      </c>
+      <c r="E264" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F264" s="4"/>
@@ -8222,372 +8221,372 @@
       </c>
       <c r="B265" s="9"/>
       <c r="C265" s="1"/>
-      <c r="D265" s="27" t="s">
-        <v>691</v>
-      </c>
-      <c r="E265" s="23" t="s">
+      <c r="D265" s="25" t="s">
+        <v>692</v>
+      </c>
+      <c r="E265" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F265" s="4"/>
     </row>
     <row r="266" ht="14.25">
       <c r="A266" s="20" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="B266" s="9"/>
       <c r="C266" s="1"/>
-      <c r="D266" s="27" t="s">
-        <v>693</v>
-      </c>
-      <c r="E266" s="25" t="s">
+      <c r="D266" s="25" t="s">
+        <v>694</v>
+      </c>
+      <c r="E266" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F266" s="4"/>
     </row>
     <row r="267" ht="14.25">
       <c r="A267" s="20" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="B267" s="9"/>
       <c r="C267" s="1"/>
-      <c r="D267" s="27" t="s">
-        <v>695</v>
-      </c>
-      <c r="E267" s="23" t="s">
+      <c r="D267" s="25" t="s">
+        <v>696</v>
+      </c>
+      <c r="E267" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F267" s="4"/>
     </row>
     <row r="268" ht="14.25">
       <c r="A268" s="20" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="B268" s="9"/>
       <c r="C268" s="1"/>
-      <c r="D268" s="27" t="s">
-        <v>697</v>
-      </c>
-      <c r="E268" s="23" t="s">
+      <c r="D268" s="25" t="s">
+        <v>698</v>
+      </c>
+      <c r="E268" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F268" s="4"/>
     </row>
     <row r="269" ht="14.25">
       <c r="A269" s="20" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="B269" s="9"/>
       <c r="C269" s="1"/>
-      <c r="D269" s="27" t="s">
-        <v>699</v>
-      </c>
-      <c r="E269" s="25" t="s">
+      <c r="D269" s="25" t="s">
+        <v>700</v>
+      </c>
+      <c r="E269" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F269" s="4"/>
     </row>
     <row r="270" ht="14.25">
       <c r="A270" s="20" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="B270" s="9"/>
       <c r="C270" s="1"/>
-      <c r="D270" s="27" t="s">
-        <v>677</v>
-      </c>
-      <c r="E270" s="23" t="s">
+      <c r="D270" s="25" t="s">
+        <v>678</v>
+      </c>
+      <c r="E270" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F270" s="4"/>
     </row>
     <row r="271" ht="14.25">
       <c r="A271" s="20" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="B271" s="9"/>
       <c r="C271" s="1"/>
-      <c r="D271" s="27" t="s">
-        <v>702</v>
-      </c>
-      <c r="E271" s="23" t="s">
+      <c r="D271" s="25" t="s">
+        <v>703</v>
+      </c>
+      <c r="E271" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F271" s="4"/>
     </row>
     <row r="272" ht="14.25">
       <c r="A272" s="20" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="B272" s="9"/>
       <c r="C272" s="1"/>
-      <c r="D272" s="27" t="s">
-        <v>677</v>
-      </c>
-      <c r="E272" s="23" t="s">
+      <c r="D272" s="25" t="s">
+        <v>678</v>
+      </c>
+      <c r="E272" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F272" s="4"/>
     </row>
     <row r="273" ht="14.25">
       <c r="A273" s="20" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B273" s="9"/>
       <c r="C273" s="1"/>
-      <c r="D273" s="27" t="s">
-        <v>705</v>
-      </c>
-      <c r="E273" s="25" t="s">
+      <c r="D273" s="25" t="s">
+        <v>706</v>
+      </c>
+      <c r="E273" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F273" s="4"/>
     </row>
     <row r="274" ht="14.25">
       <c r="A274" s="20" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="B274" s="9"/>
       <c r="C274" s="1"/>
-      <c r="D274" s="27" t="s">
-        <v>707</v>
-      </c>
-      <c r="E274" s="23" t="s">
+      <c r="D274" s="25" t="s">
+        <v>708</v>
+      </c>
+      <c r="E274" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F274" s="4"/>
     </row>
     <row r="275" ht="14.25">
       <c r="A275" s="20" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="B275" s="9"/>
       <c r="C275" s="1"/>
-      <c r="D275" s="27" t="s">
-        <v>695</v>
-      </c>
-      <c r="E275" s="25" t="s">
+      <c r="D275" s="25" t="s">
+        <v>696</v>
+      </c>
+      <c r="E275" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F275" s="4"/>
     </row>
     <row r="276" ht="14.25">
       <c r="A276" s="20" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="B276" s="9"/>
       <c r="C276" s="1"/>
-      <c r="D276" s="27" t="s">
-        <v>710</v>
-      </c>
-      <c r="E276" s="23" t="s">
+      <c r="D276" s="25" t="s">
+        <v>711</v>
+      </c>
+      <c r="E276" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F276" s="4"/>
     </row>
     <row r="277" ht="14.25">
       <c r="A277" s="20" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="B277" s="9"/>
       <c r="C277" s="1"/>
-      <c r="D277" s="27" t="s">
-        <v>669</v>
-      </c>
-      <c r="E277" s="23" t="s">
+      <c r="D277" s="25" t="s">
+        <v>670</v>
+      </c>
+      <c r="E277" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F277" s="4"/>
     </row>
     <row r="278" ht="14.25">
       <c r="A278" s="20" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="B278" s="9"/>
       <c r="C278" s="1"/>
-      <c r="D278" s="27" t="s">
-        <v>713</v>
-      </c>
-      <c r="E278" s="25" t="s">
+      <c r="D278" s="25" t="s">
+        <v>714</v>
+      </c>
+      <c r="E278" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F278" s="4"/>
     </row>
     <row r="279" ht="14.25">
       <c r="A279" s="20" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B279" s="9"/>
       <c r="C279" s="1"/>
-      <c r="D279" s="27" t="s">
-        <v>715</v>
-      </c>
-      <c r="E279" s="25" t="s">
+      <c r="D279" s="25" t="s">
+        <v>716</v>
+      </c>
+      <c r="E279" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F279" s="4"/>
     </row>
     <row r="280" ht="14.25">
       <c r="A280" s="20" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="B280" s="9"/>
       <c r="C280" s="1"/>
-      <c r="D280" s="27" t="s">
-        <v>717</v>
-      </c>
-      <c r="E280" s="23" t="s">
+      <c r="D280" s="25" t="s">
+        <v>718</v>
+      </c>
+      <c r="E280" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F280" s="4"/>
     </row>
     <row r="281" ht="14.25">
       <c r="A281" s="20" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="B281" s="9"/>
       <c r="C281" s="1"/>
-      <c r="D281" s="27" t="s">
-        <v>719</v>
-      </c>
-      <c r="E281" s="25" t="s">
+      <c r="D281" s="25" t="s">
+        <v>720</v>
+      </c>
+      <c r="E281" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F281" s="4"/>
     </row>
     <row r="282" ht="14.25">
       <c r="A282" s="20" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="B282" s="9"/>
       <c r="C282" s="1"/>
-      <c r="D282" s="27" t="s">
-        <v>721</v>
-      </c>
-      <c r="E282" s="23" t="s">
+      <c r="D282" s="25" t="s">
+        <v>722</v>
+      </c>
+      <c r="E282" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F282" s="4"/>
     </row>
     <row r="283" ht="14.25">
       <c r="A283" s="20" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="B283" s="9"/>
       <c r="C283" s="1"/>
-      <c r="D283" s="27" t="s">
-        <v>677</v>
-      </c>
-      <c r="E283" s="23" t="s">
+      <c r="D283" s="25" t="s">
+        <v>678</v>
+      </c>
+      <c r="E283" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F283" s="4"/>
     </row>
     <row r="284" ht="14.25">
       <c r="A284" s="20" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="B284" s="9"/>
       <c r="C284" s="1"/>
-      <c r="D284" s="27" t="s">
-        <v>724</v>
-      </c>
-      <c r="E284" s="23" t="s">
+      <c r="D284" s="25" t="s">
+        <v>725</v>
+      </c>
+      <c r="E284" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F284" s="4"/>
     </row>
     <row r="285" ht="14.25">
       <c r="A285" s="20" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="B285" s="9"/>
       <c r="C285" s="1"/>
-      <c r="D285" s="27" t="s">
-        <v>725</v>
-      </c>
-      <c r="E285" s="23" t="s">
+      <c r="D285" s="25" t="s">
+        <v>726</v>
+      </c>
+      <c r="E285" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F285" s="4"/>
     </row>
     <row r="286" ht="14.25">
       <c r="A286" s="20" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="B286" s="9"/>
       <c r="C286" s="1"/>
-      <c r="D286" s="27" t="s">
-        <v>727</v>
-      </c>
-      <c r="E286" s="25" t="s">
+      <c r="D286" s="25" t="s">
+        <v>728</v>
+      </c>
+      <c r="E286" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F286" s="4"/>
     </row>
     <row r="287" ht="14.25">
       <c r="A287" s="20" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="B287" s="9"/>
       <c r="C287" s="1"/>
-      <c r="D287" s="27" t="s">
-        <v>729</v>
-      </c>
-      <c r="E287" s="23" t="s">
+      <c r="D287" s="25" t="s">
+        <v>730</v>
+      </c>
+      <c r="E287" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F287" s="4"/>
     </row>
     <row r="288" ht="14.25">
       <c r="A288" s="20" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="B288" s="9"/>
       <c r="C288" s="1"/>
-      <c r="D288" s="27" t="s">
-        <v>731</v>
-      </c>
-      <c r="E288" s="23" t="s">
+      <c r="D288" s="25" t="s">
+        <v>732</v>
+      </c>
+      <c r="E288" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F288" s="4"/>
     </row>
     <row r="289" ht="14.25">
       <c r="A289" s="20" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="B289" s="9"/>
       <c r="C289" s="1"/>
-      <c r="D289" s="27" t="s">
-        <v>677</v>
-      </c>
-      <c r="E289" s="23" t="s">
+      <c r="D289" s="25" t="s">
+        <v>678</v>
+      </c>
+      <c r="E289" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F289" s="4"/>
     </row>
     <row r="290" ht="14.25">
       <c r="A290" s="20" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="B290" s="9"/>
       <c r="C290" s="1"/>
-      <c r="D290" s="27" t="s">
-        <v>697</v>
-      </c>
-      <c r="E290" s="25" t="s">
+      <c r="D290" s="25" t="s">
+        <v>698</v>
+      </c>
+      <c r="E290" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F290" s="4"/>
     </row>
     <row r="291" ht="14.25">
       <c r="A291" s="20" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="B291" s="9"/>
       <c r="C291" s="1"/>
-      <c r="D291" s="27" t="s">
-        <v>735</v>
+      <c r="D291" s="25" t="s">
+        <v>736</v>
       </c>
       <c r="E291" s="16" t="s">
         <v>10</v>
@@ -8970,6 +8969,7 @@
     <hyperlink r:id="rId120" ref="C151"/>
     <hyperlink r:id="rId121" ref="C152"/>
     <hyperlink r:id="rId122" ref="C153"/>
+    <hyperlink r:id="rId123" ref="C154"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
vault backup: 2026-01-09 00:18:36
</commit_message>
<xml_diff>
--- a/Excalidraw/switch.xlsx
+++ b/Excalidraw/switch.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="737">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="739">
   <si>
     <t>DSA</t>
   </si>
@@ -1437,6 +1437,12 @@
   </si>
   <si>
     <t xml:space="preserve">Design a Notification Service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Highly scalable, production ready rate limited notification service with messaging queues and rate limited notifications, handles retries, deduplication, atleast once delivery</t>
+  </si>
+  <si>
+    <t>https://github.com/yashaggarwal85d/Neural-Vault/blob/main/Excalidraw/Design%20a%20Notification%20Service.md</t>
   </si>
   <si>
     <t xml:space="preserve">Distributed Systems</t>
@@ -6724,13 +6730,17 @@
       <c r="F154" s="4"/>
     </row>
     <row r="155" ht="14.25">
-      <c r="A155" t="s">
+      <c r="A155" s="7" t="s">
         <v>470</v>
       </c>
-      <c r="B155" s="9"/>
-      <c r="C155" s="1"/>
+      <c r="B155" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="C155" s="11" t="s">
+        <v>472</v>
+      </c>
       <c r="D155" s="2" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="E155" s="21" t="s">
         <v>10</v>
@@ -6739,12 +6749,12 @@
     </row>
     <row r="156" ht="14.25">
       <c r="A156" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="B156" s="9"/>
       <c r="C156" s="1"/>
       <c r="D156" s="2" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="E156" s="23" t="s">
         <v>66</v>
@@ -6753,12 +6763,12 @@
     </row>
     <row r="157" ht="14.25">
       <c r="A157" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="B157" s="9"/>
       <c r="C157" s="1"/>
       <c r="D157" s="2" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="E157" s="23" t="s">
         <v>66</v>
@@ -6767,12 +6777,12 @@
     </row>
     <row r="158" ht="14.25">
       <c r="A158" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="B158" s="9"/>
       <c r="C158" s="1"/>
       <c r="D158" s="2" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="E158" s="23" t="s">
         <v>66</v>
@@ -6781,12 +6791,12 @@
     </row>
     <row r="159" ht="14.25">
       <c r="A159" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="B159" s="9"/>
       <c r="C159" s="1"/>
       <c r="D159" s="2" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="E159" s="23" t="s">
         <v>66</v>
@@ -6795,29 +6805,29 @@
     </row>
     <row r="160" ht="14.25">
       <c r="A160" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="B160" s="9"/>
       <c r="C160" s="1"/>
       <c r="D160" s="2" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="E160" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F160" s="4"/>
       <c r="L160" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
     </row>
     <row r="161" ht="14.25">
       <c r="A161" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="B161" s="9"/>
       <c r="C161" s="1"/>
       <c r="D161" s="2" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="E161" s="21" t="s">
         <v>10</v>
@@ -6826,12 +6836,12 @@
     </row>
     <row r="162" ht="14.25">
       <c r="A162" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="B162" s="9"/>
       <c r="C162" s="1"/>
       <c r="D162" s="2" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="E162" s="21" t="s">
         <v>10</v>
@@ -6840,12 +6850,12 @@
     </row>
     <row r="163" ht="14.25">
       <c r="A163" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="B163" s="9"/>
       <c r="C163" s="1"/>
       <c r="D163" s="2" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="E163" s="23" t="s">
         <v>66</v>
@@ -6854,12 +6864,12 @@
     </row>
     <row r="164" ht="14.25">
       <c r="A164" s="24" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="B164" s="9"/>
       <c r="C164" s="1"/>
       <c r="D164" s="2" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="E164" s="21" t="s">
         <v>10</v>
@@ -6868,12 +6878,12 @@
     </row>
     <row r="165" ht="14.25">
       <c r="A165" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="B165" s="9"/>
       <c r="C165" s="1"/>
       <c r="D165" s="2" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="E165" s="21" t="s">
         <v>10</v>
@@ -6882,12 +6892,12 @@
     </row>
     <row r="166" ht="14.25">
       <c r="A166" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="B166" s="9"/>
       <c r="C166" s="1"/>
       <c r="D166" s="2" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="E166" s="21" t="s">
         <v>10</v>
@@ -6896,12 +6906,12 @@
     </row>
     <row r="167" ht="14.25">
       <c r="A167" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="B167" s="9"/>
       <c r="C167" s="1"/>
       <c r="D167" s="2" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="E167" s="23" t="s">
         <v>66</v>
@@ -6910,12 +6920,12 @@
     </row>
     <row r="168" ht="14.25">
       <c r="A168" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="B168" s="9"/>
       <c r="C168" s="1"/>
       <c r="D168" s="2" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="E168" s="23" t="s">
         <v>66</v>
@@ -6924,12 +6934,12 @@
     </row>
     <row r="169" ht="14.25">
       <c r="A169" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="B169" s="9"/>
       <c r="C169" s="1"/>
       <c r="D169" s="2" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="E169" s="23" t="s">
         <v>66</v>
@@ -6938,12 +6948,12 @@
     </row>
     <row r="170" ht="14.25">
       <c r="A170" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="B170" s="9"/>
       <c r="C170" s="1"/>
       <c r="D170" s="2" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="E170" s="23" t="s">
         <v>66</v>
@@ -6952,12 +6962,12 @@
     </row>
     <row r="171" ht="14.25">
       <c r="A171" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="B171" s="9"/>
       <c r="C171" s="1"/>
       <c r="D171" s="2" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="E171" s="23" t="s">
         <v>66</v>
@@ -6966,12 +6976,12 @@
     </row>
     <row r="172" ht="14.25">
       <c r="A172" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="B172" s="9"/>
       <c r="C172" s="1"/>
       <c r="D172" s="2" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="E172" s="21" t="s">
         <v>10</v>
@@ -6980,12 +6990,12 @@
     </row>
     <row r="173" ht="14.25">
       <c r="A173" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="B173" s="9"/>
       <c r="C173" s="1"/>
       <c r="D173" s="2" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="E173" s="21" t="s">
         <v>10</v>
@@ -6994,12 +7004,12 @@
     </row>
     <row r="174" ht="14.25">
       <c r="A174" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="B174" s="9"/>
       <c r="C174" s="1"/>
       <c r="D174" s="2" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="E174" s="21" t="s">
         <v>10</v>
@@ -7008,12 +7018,12 @@
     </row>
     <row r="175" ht="14.25">
       <c r="A175" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="B175" s="9"/>
       <c r="C175" s="1"/>
       <c r="D175" s="2" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="E175" s="23" t="s">
         <v>66</v>
@@ -7022,12 +7032,12 @@
     </row>
     <row r="176" ht="14.25">
       <c r="A176" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="B176" s="9"/>
       <c r="C176" s="1"/>
       <c r="D176" s="2" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="E176" s="23" t="s">
         <v>66</v>
@@ -7036,12 +7046,12 @@
     </row>
     <row r="177" ht="14.25">
       <c r="A177" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="B177" s="9"/>
       <c r="C177" s="1"/>
       <c r="D177" s="2" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="E177" s="23" t="s">
         <v>66</v>
@@ -7050,12 +7060,12 @@
     </row>
     <row r="178" ht="14.25">
       <c r="A178" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="B178" s="9"/>
       <c r="C178" s="1"/>
       <c r="D178" s="2" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="E178" s="21" t="s">
         <v>10</v>
@@ -7064,12 +7074,12 @@
     </row>
     <row r="179" ht="14.25">
       <c r="A179" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="B179" s="9"/>
       <c r="C179" s="1"/>
       <c r="D179" s="2" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="E179" s="23" t="s">
         <v>66</v>
@@ -7078,12 +7088,12 @@
     </row>
     <row r="180" ht="14.25">
       <c r="A180" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="B180" s="9"/>
       <c r="C180" s="1"/>
       <c r="D180" s="2" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="E180" s="21" t="s">
         <v>10</v>
@@ -7092,12 +7102,12 @@
     </row>
     <row r="181" ht="14.25">
       <c r="A181" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="B181" s="9"/>
       <c r="C181" s="1"/>
       <c r="D181" s="2" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="E181" s="23" t="s">
         <v>66</v>
@@ -7106,12 +7116,12 @@
     </row>
     <row r="182" ht="14.25">
       <c r="A182" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="B182" s="9"/>
       <c r="C182" s="1"/>
       <c r="D182" s="2" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="E182" s="21" t="s">
         <v>10</v>
@@ -7120,12 +7130,12 @@
     </row>
     <row r="183" ht="14.25">
       <c r="A183" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="B183" s="9"/>
       <c r="C183" s="1"/>
       <c r="D183" s="2" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="E183" s="21" t="s">
         <v>10</v>
@@ -7134,12 +7144,12 @@
     </row>
     <row r="184" ht="14.25">
       <c r="A184" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="B184" s="9"/>
       <c r="C184" s="1"/>
       <c r="D184" s="2" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="E184" s="23" t="s">
         <v>66</v>
@@ -7148,12 +7158,12 @@
     </row>
     <row r="185" ht="14.25">
       <c r="A185" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="B185" s="9"/>
       <c r="C185" s="1"/>
       <c r="D185" s="2" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="E185" s="23" t="s">
         <v>66</v>
@@ -7162,12 +7172,12 @@
     </row>
     <row r="186" ht="14.25">
       <c r="A186" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="B186" s="9"/>
       <c r="C186" s="1"/>
       <c r="D186" s="2" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="E186" s="23" t="s">
         <v>66</v>
@@ -7176,12 +7186,12 @@
     </row>
     <row r="187" ht="14.25">
       <c r="A187" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="B187" s="9"/>
       <c r="C187" s="1"/>
       <c r="D187" s="2" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="E187" s="23" t="s">
         <v>66</v>
@@ -7190,12 +7200,12 @@
     </row>
     <row r="188" ht="14.25">
       <c r="A188" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="B188" s="9"/>
       <c r="C188" s="1"/>
       <c r="D188" s="2" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="E188" s="21" t="s">
         <v>10</v>
@@ -7204,12 +7214,12 @@
     </row>
     <row r="189" ht="14.25">
       <c r="A189" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="B189" s="9"/>
       <c r="C189" s="1"/>
       <c r="D189" s="2" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="E189" s="23" t="s">
         <v>66</v>
@@ -7218,12 +7228,12 @@
     </row>
     <row r="190" ht="14.25">
       <c r="A190" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="B190" s="9"/>
       <c r="C190" s="1"/>
       <c r="D190" s="2" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="E190" s="21" t="s">
         <v>10</v>
@@ -7232,12 +7242,12 @@
     </row>
     <row r="191" ht="14.25">
       <c r="A191" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="B191" s="9"/>
       <c r="C191" s="1"/>
       <c r="D191" s="2" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="E191" s="23" t="s">
         <v>66</v>
@@ -7246,12 +7256,12 @@
     </row>
     <row r="192" ht="14.25">
       <c r="A192" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="B192" s="9"/>
       <c r="C192" s="1"/>
       <c r="D192" s="2" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="E192" s="18" t="s">
         <v>66</v>
@@ -7274,7 +7284,7 @@
     </row>
     <row r="195" ht="14.25">
       <c r="A195" s="5" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="B195" s="5"/>
       <c r="C195" s="5"/>
@@ -7284,619 +7294,619 @@
     </row>
     <row r="196" ht="14.25">
       <c r="A196" s="4" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="B196" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C196" s="4" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="D196" s="4" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="E196" s="4"/>
       <c r="F196" s="4"/>
     </row>
     <row r="197" ht="14.25">
       <c r="A197" s="20" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="B197" s="9"/>
       <c r="C197" s="1" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="F197" s="4"/>
     </row>
     <row r="198" ht="14.25">
       <c r="A198" s="20" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="B198" s="9"/>
       <c r="C198" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="D198" s="2" t="s">
         <v>554</v>
-      </c>
-      <c r="D198" s="2" t="s">
-        <v>552</v>
       </c>
       <c r="F198" s="4"/>
       <c r="H198" s="6"/>
     </row>
     <row r="199" ht="14.25">
       <c r="A199" s="20" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="B199" s="9"/>
       <c r="C199" s="1" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="D199" s="2" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="F199" s="4"/>
     </row>
     <row r="200" ht="14.25">
       <c r="A200" s="20" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="B200" s="9"/>
       <c r="C200" s="1" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="F200" s="4"/>
     </row>
     <row r="201" ht="14.25">
       <c r="A201" s="20" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="B201" s="9"/>
       <c r="C201" s="1" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="F201" s="4"/>
     </row>
     <row r="202" ht="14.25">
       <c r="A202" s="20" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="B202" s="9"/>
       <c r="C202" s="1" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="F202" s="4"/>
     </row>
     <row r="203" ht="14.25">
       <c r="A203" s="20" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="B203" s="9"/>
       <c r="C203" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="D203" s="2" t="s">
         <v>565</v>
-      </c>
-      <c r="D203" s="2" t="s">
-        <v>563</v>
       </c>
       <c r="F203" s="4"/>
       <c r="H203" s="6"/>
     </row>
     <row r="204" ht="14.25">
       <c r="A204" s="20" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="B204" s="9"/>
       <c r="C204" s="1" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="F204" s="4"/>
       <c r="H204" s="6"/>
     </row>
     <row r="205" ht="14.25">
       <c r="A205" s="20" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="B205" s="9"/>
       <c r="C205" s="1" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="D205" s="2" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="F205" s="4"/>
       <c r="H205" s="6"/>
     </row>
     <row r="206" ht="14.25">
       <c r="A206" s="20" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="B206" s="9"/>
       <c r="C206" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="D206" s="2" t="s">
         <v>572</v>
-      </c>
-      <c r="D206" s="2" t="s">
-        <v>570</v>
       </c>
       <c r="F206" s="4"/>
       <c r="H206" s="6"/>
     </row>
     <row r="207" ht="14.25">
       <c r="A207" s="20" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="B207" s="9"/>
       <c r="C207" s="1" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="D207" s="2" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="F207" s="4"/>
       <c r="H207" s="6"/>
     </row>
     <row r="208" ht="14.25">
       <c r="A208" s="20" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="B208" s="9"/>
       <c r="C208" s="1" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="D208" s="2" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="F208" s="4"/>
       <c r="H208" s="6"/>
     </row>
     <row r="209" ht="14.25">
       <c r="A209" s="20" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c r="B209" s="9"/>
       <c r="C209" s="1" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="F209" s="4"/>
       <c r="H209" s="6"/>
     </row>
     <row r="210" ht="14.25">
       <c r="A210" s="20" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="B210" s="9"/>
       <c r="C210" s="1" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="F210" s="4"/>
     </row>
     <row r="211" ht="14.25">
       <c r="A211" s="20" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="B211" s="9"/>
       <c r="C211" s="1" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="D211" s="2" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="F211" s="4"/>
     </row>
     <row r="212" ht="14.25">
       <c r="A212" s="20" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="B212" s="9"/>
       <c r="C212" s="1" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="D212" s="2" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="F212" s="4"/>
     </row>
     <row r="213" ht="14.25">
       <c r="A213" s="20" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="B213" s="9"/>
       <c r="C213" s="1" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="D213" s="2" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="F213" s="4"/>
     </row>
     <row r="214" ht="14.25">
       <c r="A214" s="20" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="B214" s="9"/>
       <c r="C214" s="1" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="D214" s="2" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="F214" s="4"/>
     </row>
     <row r="215" ht="14.25">
       <c r="A215" s="20" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="B215" s="9"/>
       <c r="C215" s="1" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="F215" s="4"/>
     </row>
     <row r="216" ht="14.25">
       <c r="A216" s="20" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="B216" s="9"/>
       <c r="C216" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="D216" s="2" t="s">
         <v>593</v>
-      </c>
-      <c r="D216" s="2" t="s">
-        <v>591</v>
       </c>
       <c r="F216" s="4"/>
     </row>
     <row r="217" ht="14.25">
       <c r="A217" s="20" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="B217" s="9"/>
       <c r="C217" s="1" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="F217" s="4"/>
     </row>
     <row r="218" ht="14.25">
       <c r="A218" s="20" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="B218" s="9"/>
       <c r="C218" s="1" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="F218" s="4"/>
     </row>
     <row r="219" ht="14.25">
       <c r="A219" s="20" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="B219" s="9"/>
       <c r="C219" s="1" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="F219" s="4"/>
     </row>
     <row r="220" ht="14.25">
       <c r="A220" s="20" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="B220" s="9"/>
       <c r="C220" s="1" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="D220" s="2" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="F220" s="4"/>
     </row>
     <row r="221" ht="14.25">
       <c r="A221" s="20" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="B221" s="9"/>
       <c r="C221" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="D221" s="2" t="s">
         <v>604</v>
-      </c>
-      <c r="D221" s="2" t="s">
-        <v>602</v>
       </c>
       <c r="F221" s="4"/>
     </row>
     <row r="222" ht="14.25">
       <c r="A222" s="20" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="B222" s="9"/>
       <c r="C222" s="1" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="D222" s="2" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="F222" s="4"/>
     </row>
     <row r="223" ht="14.25">
       <c r="A223" s="20" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="B223" s="9"/>
       <c r="C223" s="1" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="D223" s="2" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="F223" s="4"/>
     </row>
     <row r="224" ht="14.25">
       <c r="A224" s="20" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="B224" s="9"/>
       <c r="C224" s="1" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="D224" s="2" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="F224" s="4"/>
     </row>
     <row r="225" ht="14.25">
       <c r="A225" s="20" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="B225" s="9"/>
       <c r="C225" s="1" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="D225" s="2" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="F225" s="4"/>
     </row>
     <row r="226" ht="14.25">
       <c r="A226" s="20" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="B226" s="9"/>
       <c r="C226" s="1" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="D226" s="2" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="F226" s="4"/>
     </row>
     <row r="227" ht="14.25">
       <c r="A227" s="20" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="B227" s="9"/>
       <c r="C227" s="1" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="D227" s="2" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="F227" s="4"/>
     </row>
     <row r="228" ht="14.25">
       <c r="A228" s="20" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="B228" s="9"/>
       <c r="C228" s="1" t="s">
+        <v>621</v>
+      </c>
+      <c r="D228" s="2" t="s">
         <v>619</v>
-      </c>
-      <c r="D228" s="2" t="s">
-        <v>617</v>
       </c>
       <c r="F228" s="4"/>
     </row>
     <row r="229" ht="14.25">
       <c r="A229" s="20" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="B229" s="9"/>
       <c r="C229" s="1" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c r="D229" s="2" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="F229" s="4"/>
     </row>
     <row r="230" ht="14.25">
       <c r="A230" s="20" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
       <c r="B230" s="9"/>
       <c r="C230" s="1" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c r="D230" s="2" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="F230" s="4"/>
     </row>
     <row r="231" ht="14.25">
       <c r="A231" s="20" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="B231" s="9"/>
       <c r="C231" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="D231" s="2" t="s">
         <v>626</v>
-      </c>
-      <c r="D231" s="2" t="s">
-        <v>624</v>
       </c>
       <c r="F231" s="4"/>
     </row>
     <row r="232" ht="14.25">
       <c r="A232" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="B232" s="9"/>
       <c r="C232" s="1" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="D232" s="2" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
       <c r="F232" s="4"/>
       <c r="H232" s="6"/>
     </row>
     <row r="233" ht="14.25">
       <c r="A233" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="B233" s="9"/>
       <c r="C233" s="1" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
       <c r="D233" s="2" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
       <c r="F233" s="4"/>
       <c r="H233" s="6"/>
     </row>
     <row r="234" ht="14.25">
       <c r="A234" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="B234" s="9"/>
       <c r="C234" s="1" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="D234" s="2" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
       <c r="F234" s="4"/>
       <c r="H234" s="6"/>
     </row>
     <row r="235" ht="14.25">
       <c r="A235" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="B235" s="9"/>
       <c r="C235" s="1" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c r="D235" s="2" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="F235" s="4"/>
       <c r="H235" s="6"/>
     </row>
     <row r="236" ht="14.25">
       <c r="A236" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="B236" s="9"/>
       <c r="C236" s="1" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="D236" s="2" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="F236" s="4"/>
       <c r="H236" s="6"/>
     </row>
     <row r="237" ht="14.25">
       <c r="A237" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="B237" s="9"/>
       <c r="C237" s="1" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="D237" s="2" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="F237" s="4"/>
       <c r="H237" s="6"/>
     </row>
     <row r="238" ht="14.25">
       <c r="A238" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="B238" s="9"/>
       <c r="C238" s="1" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="D238" s="2" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="F238" s="4"/>
       <c r="H238" s="6"/>
     </row>
     <row r="239" ht="14.25">
       <c r="A239" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="B239" s="9"/>
       <c r="C239" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="D239" s="2" t="s">
         <v>648</v>
-      </c>
-      <c r="D239" s="2" t="s">
-        <v>646</v>
       </c>
       <c r="F239" s="4"/>
       <c r="H239" s="6"/>
     </row>
     <row r="240" ht="14.25">
       <c r="A240" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="B240" s="9"/>
       <c r="C240" s="1" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c r="D240" s="2" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="F240" s="4"/>
       <c r="H240" s="6"/>
     </row>
     <row r="241" ht="14.25">
       <c r="A241" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="B241" s="9"/>
       <c r="C241" s="1" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="D241" s="2" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c r="E241" s="3"/>
       <c r="F241" s="4"/>
@@ -7904,14 +7914,14 @@
     </row>
     <row r="242" ht="14.25">
       <c r="A242" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c r="B242" s="9"/>
       <c r="C242" s="1" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c r="D242" s="2" t="s">
-        <v>656</v>
+        <v>658</v>
       </c>
       <c r="E242" s="3"/>
       <c r="F242" s="4"/>
@@ -7919,14 +7929,14 @@
     </row>
     <row r="243" ht="14.25">
       <c r="A243" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="B243" s="9"/>
       <c r="C243" s="1" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="D243" s="2" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="E243" s="3"/>
       <c r="F243" s="4"/>
@@ -7934,14 +7944,14 @@
     </row>
     <row r="244" ht="14.25">
       <c r="A244" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="B244" s="9"/>
       <c r="C244" s="1" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="D244" s="2" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="E244" s="3"/>
       <c r="F244" s="4"/>
@@ -7949,14 +7959,14 @@
     </row>
     <row r="245" ht="14.25">
       <c r="A245" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="B245" s="9"/>
       <c r="C245" s="1" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c r="D245" s="2" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c r="E245" s="3"/>
       <c r="F245" s="4"/>
@@ -7964,14 +7974,14 @@
     </row>
     <row r="246" ht="14.25">
       <c r="A246" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="B246" s="9"/>
       <c r="C246" s="1" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="D246" s="2" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c r="E246" s="3"/>
       <c r="F246" s="4"/>
@@ -7993,7 +8003,7 @@
     </row>
     <row r="249" ht="14.25">
       <c r="A249" s="5" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c r="B249" s="5"/>
       <c r="C249" s="5"/>
@@ -8021,12 +8031,12 @@
     </row>
     <row r="251" ht="14.25">
       <c r="A251" s="20" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="B251" s="9"/>
       <c r="C251" s="1"/>
       <c r="D251" s="25" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="E251" s="16" t="s">
         <v>10</v>
@@ -8035,12 +8045,12 @@
     </row>
     <row r="252" ht="14.25">
       <c r="A252" s="20" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="B252" s="9"/>
       <c r="C252" s="1"/>
       <c r="D252" s="25" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="E252" s="21" t="s">
         <v>10</v>
@@ -8049,12 +8059,12 @@
     </row>
     <row r="253" ht="14.25">
       <c r="A253" s="20" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="B253" s="9"/>
       <c r="C253" s="1"/>
       <c r="D253" s="25" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="E253" s="21" t="s">
         <v>10</v>
@@ -8063,12 +8073,12 @@
     </row>
     <row r="254" ht="14.25">
       <c r="A254" s="20" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c r="B254" s="9"/>
       <c r="C254" s="1"/>
       <c r="D254" s="25" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="E254" s="21" t="s">
         <v>10</v>
@@ -8077,12 +8087,12 @@
     </row>
     <row r="255" ht="14.25">
       <c r="A255" s="20" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="B255" s="9"/>
       <c r="C255" s="1"/>
       <c r="D255" s="25" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="E255" s="21" t="s">
         <v>10</v>
@@ -8091,12 +8101,12 @@
     </row>
     <row r="256" ht="14.25">
       <c r="A256" s="20" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="B256" s="9"/>
       <c r="C256" s="1"/>
       <c r="D256" s="25" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="E256" s="21" t="s">
         <v>10</v>
@@ -8105,12 +8115,12 @@
     </row>
     <row r="257" ht="14.25">
       <c r="A257" s="20" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="B257" s="9"/>
       <c r="C257" s="1"/>
       <c r="D257" s="25" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="E257" s="21" t="s">
         <v>10</v>
@@ -8119,12 +8129,12 @@
     </row>
     <row r="258" ht="14.25">
       <c r="A258" s="20" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="B258" s="9"/>
       <c r="C258" s="1"/>
       <c r="D258" s="25" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="E258" s="21" t="s">
         <v>10</v>
@@ -8133,12 +8143,12 @@
     </row>
     <row r="259" ht="14.25">
       <c r="A259" s="20" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="B259" s="9"/>
       <c r="C259" s="1"/>
       <c r="D259" s="25" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="E259" s="21" t="s">
         <v>10</v>
@@ -8147,12 +8157,12 @@
     </row>
     <row r="260" ht="14.25">
       <c r="A260" s="20" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="B260" s="9"/>
       <c r="C260" s="1"/>
       <c r="D260" s="25" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="E260" s="23" t="s">
         <v>66</v>
@@ -8161,12 +8171,12 @@
     </row>
     <row r="261" ht="14.25">
       <c r="A261" s="20" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="B261" s="9"/>
       <c r="C261" s="1"/>
       <c r="D261" s="25" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="E261" s="21" t="s">
         <v>10</v>
@@ -8175,12 +8185,12 @@
     </row>
     <row r="262" ht="14.25">
       <c r="A262" s="20" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="B262" s="9"/>
       <c r="C262" s="1"/>
       <c r="D262" s="25" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="E262" s="23" t="s">
         <v>66</v>
@@ -8189,12 +8199,12 @@
     </row>
     <row r="263" ht="14.25">
       <c r="A263" s="20" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="B263" s="9"/>
       <c r="C263" s="1"/>
       <c r="D263" s="25" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="E263" s="21" t="s">
         <v>10</v>
@@ -8208,7 +8218,7 @@
       <c r="B264" s="9"/>
       <c r="C264" s="1"/>
       <c r="D264" s="25" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="E264" s="23" t="s">
         <v>66</v>
@@ -8222,7 +8232,7 @@
       <c r="B265" s="9"/>
       <c r="C265" s="1"/>
       <c r="D265" s="25" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c r="E265" s="21" t="s">
         <v>10</v>
@@ -8231,12 +8241,12 @@
     </row>
     <row r="266" ht="14.25">
       <c r="A266" s="20" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="B266" s="9"/>
       <c r="C266" s="1"/>
       <c r="D266" s="25" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="E266" s="23" t="s">
         <v>66</v>
@@ -8245,12 +8255,12 @@
     </row>
     <row r="267" ht="14.25">
       <c r="A267" s="20" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="B267" s="9"/>
       <c r="C267" s="1"/>
       <c r="D267" s="25" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
       <c r="E267" s="21" t="s">
         <v>10</v>
@@ -8259,12 +8269,12 @@
     </row>
     <row r="268" ht="14.25">
       <c r="A268" s="20" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="B268" s="9"/>
       <c r="C268" s="1"/>
       <c r="D268" s="25" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="E268" s="21" t="s">
         <v>10</v>
@@ -8273,12 +8283,12 @@
     </row>
     <row r="269" ht="14.25">
       <c r="A269" s="20" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="B269" s="9"/>
       <c r="C269" s="1"/>
       <c r="D269" s="25" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="E269" s="23" t="s">
         <v>66</v>
@@ -8287,12 +8297,12 @@
     </row>
     <row r="270" ht="14.25">
       <c r="A270" s="20" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="B270" s="9"/>
       <c r="C270" s="1"/>
       <c r="D270" s="25" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="E270" s="21" t="s">
         <v>10</v>
@@ -8301,12 +8311,12 @@
     </row>
     <row r="271" ht="14.25">
       <c r="A271" s="20" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="B271" s="9"/>
       <c r="C271" s="1"/>
       <c r="D271" s="25" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="E271" s="21" t="s">
         <v>10</v>
@@ -8315,12 +8325,12 @@
     </row>
     <row r="272" ht="14.25">
       <c r="A272" s="20" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="B272" s="9"/>
       <c r="C272" s="1"/>
       <c r="D272" s="25" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="E272" s="21" t="s">
         <v>10</v>
@@ -8329,12 +8339,12 @@
     </row>
     <row r="273" ht="14.25">
       <c r="A273" s="20" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="B273" s="9"/>
       <c r="C273" s="1"/>
       <c r="D273" s="25" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="E273" s="23" t="s">
         <v>66</v>
@@ -8343,12 +8353,12 @@
     </row>
     <row r="274" ht="14.25">
       <c r="A274" s="20" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="B274" s="9"/>
       <c r="C274" s="1"/>
       <c r="D274" s="25" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="E274" s="21" t="s">
         <v>10</v>
@@ -8357,12 +8367,12 @@
     </row>
     <row r="275" ht="14.25">
       <c r="A275" s="20" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="B275" s="9"/>
       <c r="C275" s="1"/>
       <c r="D275" s="25" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
       <c r="E275" s="23" t="s">
         <v>66</v>
@@ -8371,12 +8381,12 @@
     </row>
     <row r="276" ht="14.25">
       <c r="A276" s="20" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="B276" s="9"/>
       <c r="C276" s="1"/>
       <c r="D276" s="25" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="E276" s="21" t="s">
         <v>10</v>
@@ -8385,12 +8395,12 @@
     </row>
     <row r="277" ht="14.25">
       <c r="A277" s="20" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="B277" s="9"/>
       <c r="C277" s="1"/>
       <c r="D277" s="25" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="E277" s="21" t="s">
         <v>10</v>
@@ -8399,12 +8409,12 @@
     </row>
     <row r="278" ht="14.25">
       <c r="A278" s="20" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="B278" s="9"/>
       <c r="C278" s="1"/>
       <c r="D278" s="25" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="E278" s="23" t="s">
         <v>66</v>
@@ -8413,12 +8423,12 @@
     </row>
     <row r="279" ht="14.25">
       <c r="A279" s="20" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="B279" s="9"/>
       <c r="C279" s="1"/>
       <c r="D279" s="25" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="E279" s="23" t="s">
         <v>66</v>
@@ -8427,12 +8437,12 @@
     </row>
     <row r="280" ht="14.25">
       <c r="A280" s="20" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="B280" s="9"/>
       <c r="C280" s="1"/>
       <c r="D280" s="25" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="E280" s="21" t="s">
         <v>10</v>
@@ -8441,12 +8451,12 @@
     </row>
     <row r="281" ht="14.25">
       <c r="A281" s="20" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="B281" s="9"/>
       <c r="C281" s="1"/>
       <c r="D281" s="25" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c r="E281" s="23" t="s">
         <v>66</v>
@@ -8455,12 +8465,12 @@
     </row>
     <row r="282" ht="14.25">
       <c r="A282" s="20" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="B282" s="9"/>
       <c r="C282" s="1"/>
       <c r="D282" s="25" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="E282" s="21" t="s">
         <v>10</v>
@@ -8469,12 +8479,12 @@
     </row>
     <row r="283" ht="14.25">
       <c r="A283" s="20" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="B283" s="9"/>
       <c r="C283" s="1"/>
       <c r="D283" s="25" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="E283" s="21" t="s">
         <v>10</v>
@@ -8483,12 +8493,12 @@
     </row>
     <row r="284" ht="14.25">
       <c r="A284" s="20" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="B284" s="9"/>
       <c r="C284" s="1"/>
       <c r="D284" s="25" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="E284" s="21" t="s">
         <v>10</v>
@@ -8497,12 +8507,12 @@
     </row>
     <row r="285" ht="14.25">
       <c r="A285" s="20" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="B285" s="9"/>
       <c r="C285" s="1"/>
       <c r="D285" s="25" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="E285" s="21" t="s">
         <v>10</v>
@@ -8511,12 +8521,12 @@
     </row>
     <row r="286" ht="14.25">
       <c r="A286" s="20" t="s">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c r="B286" s="9"/>
       <c r="C286" s="1"/>
       <c r="D286" s="25" t="s">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c r="E286" s="23" t="s">
         <v>66</v>
@@ -8525,12 +8535,12 @@
     </row>
     <row r="287" ht="14.25">
       <c r="A287" s="20" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="B287" s="9"/>
       <c r="C287" s="1"/>
       <c r="D287" s="25" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="E287" s="21" t="s">
         <v>10</v>
@@ -8539,12 +8549,12 @@
     </row>
     <row r="288" ht="14.25">
       <c r="A288" s="20" t="s">
-        <v>731</v>
+        <v>733</v>
       </c>
       <c r="B288" s="9"/>
       <c r="C288" s="1"/>
       <c r="D288" s="25" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="E288" s="21" t="s">
         <v>10</v>
@@ -8553,12 +8563,12 @@
     </row>
     <row r="289" ht="14.25">
       <c r="A289" s="20" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="B289" s="9"/>
       <c r="C289" s="1"/>
       <c r="D289" s="25" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="E289" s="21" t="s">
         <v>10</v>
@@ -8567,12 +8577,12 @@
     </row>
     <row r="290" ht="14.25">
       <c r="A290" s="20" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c r="B290" s="9"/>
       <c r="C290" s="1"/>
       <c r="D290" s="25" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="E290" s="23" t="s">
         <v>66</v>
@@ -8581,12 +8591,12 @@
     </row>
     <row r="291" ht="14.25">
       <c r="A291" s="20" t="s">
-        <v>735</v>
+        <v>737</v>
       </c>
       <c r="B291" s="9"/>
       <c r="C291" s="1"/>
       <c r="D291" s="25" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="E291" s="16" t="s">
         <v>10</v>
@@ -8970,6 +8980,7 @@
     <hyperlink r:id="rId121" ref="C152"/>
     <hyperlink r:id="rId122" ref="C153"/>
     <hyperlink r:id="rId123" ref="C154"/>
+    <hyperlink r:id="rId124" ref="C155"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
vault backup: 2026-01-09 21:00:13
</commit_message>
<xml_diff>
--- a/Excalidraw/switch.xlsx
+++ b/Excalidraw/switch.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="741">
   <si>
     <t>DSA</t>
   </si>
@@ -1449,6 +1449,12 @@
   </si>
   <si>
     <t xml:space="preserve">Design a Distributed Job Scheduler (Cron)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">horizontally scalable, fault-tolerant distributed job scheduler that guarantees exactly-once triggering using shard ownership, time-bucketed scheduling, and queue-based execution decoupling</t>
+  </si>
+  <si>
+    <t>https://github.com/yashaggarwal85d/Neural-Vault/blob/main/Excalidraw/Design%20a%20Distributed%20Job%20Scheduler%20(Cron).md</t>
   </si>
   <si>
     <t xml:space="preserve">Design a Metrics / Monitoring System</t>
@@ -6748,11 +6754,15 @@
       <c r="F155" s="4"/>
     </row>
     <row r="156" ht="14.25">
-      <c r="A156" t="s">
+      <c r="A156" s="7" t="s">
         <v>474</v>
       </c>
-      <c r="B156" s="9"/>
-      <c r="C156" s="1"/>
+      <c r="B156" s="9" t="s">
+        <v>475</v>
+      </c>
+      <c r="C156" s="11" t="s">
+        <v>476</v>
+      </c>
       <c r="D156" s="2" t="s">
         <v>473</v>
       </c>
@@ -6763,12 +6773,12 @@
     </row>
     <row r="157" ht="14.25">
       <c r="A157" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="B157" s="9"/>
       <c r="C157" s="1"/>
       <c r="D157" s="2" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="E157" s="23" t="s">
         <v>66</v>
@@ -6777,12 +6787,12 @@
     </row>
     <row r="158" ht="14.25">
       <c r="A158" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="B158" s="9"/>
       <c r="C158" s="1"/>
       <c r="D158" s="2" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="E158" s="23" t="s">
         <v>66</v>
@@ -6791,12 +6801,12 @@
     </row>
     <row r="159" ht="14.25">
       <c r="A159" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="B159" s="9"/>
       <c r="C159" s="1"/>
       <c r="D159" s="2" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="E159" s="23" t="s">
         <v>66</v>
@@ -6805,29 +6815,29 @@
     </row>
     <row r="160" ht="14.25">
       <c r="A160" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="B160" s="9"/>
       <c r="C160" s="1"/>
       <c r="D160" s="2" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="E160" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F160" s="4"/>
       <c r="L160" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
     </row>
     <row r="161" ht="14.25">
       <c r="A161" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="B161" s="9"/>
       <c r="C161" s="1"/>
       <c r="D161" s="2" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="E161" s="21" t="s">
         <v>10</v>
@@ -6836,12 +6846,12 @@
     </row>
     <row r="162" ht="14.25">
       <c r="A162" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="B162" s="9"/>
       <c r="C162" s="1"/>
       <c r="D162" s="2" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="E162" s="21" t="s">
         <v>10</v>
@@ -6850,12 +6860,12 @@
     </row>
     <row r="163" ht="14.25">
       <c r="A163" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="B163" s="9"/>
       <c r="C163" s="1"/>
       <c r="D163" s="2" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="E163" s="23" t="s">
         <v>66</v>
@@ -6864,12 +6874,12 @@
     </row>
     <row r="164" ht="14.25">
       <c r="A164" s="24" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="B164" s="9"/>
       <c r="C164" s="1"/>
       <c r="D164" s="2" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="E164" s="21" t="s">
         <v>10</v>
@@ -6878,12 +6888,12 @@
     </row>
     <row r="165" ht="14.25">
       <c r="A165" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="B165" s="9"/>
       <c r="C165" s="1"/>
       <c r="D165" s="2" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="E165" s="21" t="s">
         <v>10</v>
@@ -6892,12 +6902,12 @@
     </row>
     <row r="166" ht="14.25">
       <c r="A166" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="B166" s="9"/>
       <c r="C166" s="1"/>
       <c r="D166" s="2" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="E166" s="21" t="s">
         <v>10</v>
@@ -6906,12 +6916,12 @@
     </row>
     <row r="167" ht="14.25">
       <c r="A167" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="B167" s="9"/>
       <c r="C167" s="1"/>
       <c r="D167" s="2" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="E167" s="23" t="s">
         <v>66</v>
@@ -6920,12 +6930,12 @@
     </row>
     <row r="168" ht="14.25">
       <c r="A168" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="B168" s="9"/>
       <c r="C168" s="1"/>
       <c r="D168" s="2" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="E168" s="23" t="s">
         <v>66</v>
@@ -6934,12 +6944,12 @@
     </row>
     <row r="169" ht="14.25">
       <c r="A169" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="B169" s="9"/>
       <c r="C169" s="1"/>
       <c r="D169" s="2" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="E169" s="23" t="s">
         <v>66</v>
@@ -6948,12 +6958,12 @@
     </row>
     <row r="170" ht="14.25">
       <c r="A170" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="B170" s="9"/>
       <c r="C170" s="1"/>
       <c r="D170" s="2" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="E170" s="23" t="s">
         <v>66</v>
@@ -6962,12 +6972,12 @@
     </row>
     <row r="171" ht="14.25">
       <c r="A171" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="B171" s="9"/>
       <c r="C171" s="1"/>
       <c r="D171" s="2" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="E171" s="23" t="s">
         <v>66</v>
@@ -6976,12 +6986,12 @@
     </row>
     <row r="172" ht="14.25">
       <c r="A172" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="B172" s="9"/>
       <c r="C172" s="1"/>
       <c r="D172" s="2" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="E172" s="21" t="s">
         <v>10</v>
@@ -6990,12 +7000,12 @@
     </row>
     <row r="173" ht="14.25">
       <c r="A173" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="B173" s="9"/>
       <c r="C173" s="1"/>
       <c r="D173" s="2" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="E173" s="21" t="s">
         <v>10</v>
@@ -7004,12 +7014,12 @@
     </row>
     <row r="174" ht="14.25">
       <c r="A174" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="B174" s="9"/>
       <c r="C174" s="1"/>
       <c r="D174" s="2" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="E174" s="21" t="s">
         <v>10</v>
@@ -7018,12 +7028,12 @@
     </row>
     <row r="175" ht="14.25">
       <c r="A175" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="B175" s="9"/>
       <c r="C175" s="1"/>
       <c r="D175" s="2" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="E175" s="23" t="s">
         <v>66</v>
@@ -7032,12 +7042,12 @@
     </row>
     <row r="176" ht="14.25">
       <c r="A176" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="B176" s="9"/>
       <c r="C176" s="1"/>
       <c r="D176" s="2" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="E176" s="23" t="s">
         <v>66</v>
@@ -7046,12 +7056,12 @@
     </row>
     <row r="177" ht="14.25">
       <c r="A177" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="B177" s="9"/>
       <c r="C177" s="1"/>
       <c r="D177" s="2" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="E177" s="23" t="s">
         <v>66</v>
@@ -7060,12 +7070,12 @@
     </row>
     <row r="178" ht="14.25">
       <c r="A178" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="B178" s="9"/>
       <c r="C178" s="1"/>
       <c r="D178" s="2" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="E178" s="21" t="s">
         <v>10</v>
@@ -7074,12 +7084,12 @@
     </row>
     <row r="179" ht="14.25">
       <c r="A179" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="B179" s="9"/>
       <c r="C179" s="1"/>
       <c r="D179" s="2" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="E179" s="23" t="s">
         <v>66</v>
@@ -7088,12 +7098,12 @@
     </row>
     <row r="180" ht="14.25">
       <c r="A180" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="B180" s="9"/>
       <c r="C180" s="1"/>
       <c r="D180" s="2" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="E180" s="21" t="s">
         <v>10</v>
@@ -7102,12 +7112,12 @@
     </row>
     <row r="181" ht="14.25">
       <c r="A181" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="B181" s="9"/>
       <c r="C181" s="1"/>
       <c r="D181" s="2" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="E181" s="23" t="s">
         <v>66</v>
@@ -7116,12 +7126,12 @@
     </row>
     <row r="182" ht="14.25">
       <c r="A182" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="B182" s="9"/>
       <c r="C182" s="1"/>
       <c r="D182" s="2" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="E182" s="21" t="s">
         <v>10</v>
@@ -7130,12 +7140,12 @@
     </row>
     <row r="183" ht="14.25">
       <c r="A183" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="B183" s="9"/>
       <c r="C183" s="1"/>
       <c r="D183" s="2" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="E183" s="21" t="s">
         <v>10</v>
@@ -7144,12 +7154,12 @@
     </row>
     <row r="184" ht="14.25">
       <c r="A184" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="B184" s="9"/>
       <c r="C184" s="1"/>
       <c r="D184" s="2" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="E184" s="23" t="s">
         <v>66</v>
@@ -7158,12 +7168,12 @@
     </row>
     <row r="185" ht="14.25">
       <c r="A185" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="B185" s="9"/>
       <c r="C185" s="1"/>
       <c r="D185" s="2" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="E185" s="23" t="s">
         <v>66</v>
@@ -7172,12 +7182,12 @@
     </row>
     <row r="186" ht="14.25">
       <c r="A186" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="B186" s="9"/>
       <c r="C186" s="1"/>
       <c r="D186" s="2" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="E186" s="23" t="s">
         <v>66</v>
@@ -7186,12 +7196,12 @@
     </row>
     <row r="187" ht="14.25">
       <c r="A187" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="B187" s="9"/>
       <c r="C187" s="1"/>
       <c r="D187" s="2" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="E187" s="23" t="s">
         <v>66</v>
@@ -7200,12 +7210,12 @@
     </row>
     <row r="188" ht="14.25">
       <c r="A188" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="B188" s="9"/>
       <c r="C188" s="1"/>
       <c r="D188" s="2" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="E188" s="21" t="s">
         <v>10</v>
@@ -7214,12 +7224,12 @@
     </row>
     <row r="189" ht="14.25">
       <c r="A189" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="B189" s="9"/>
       <c r="C189" s="1"/>
       <c r="D189" s="2" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="E189" s="23" t="s">
         <v>66</v>
@@ -7228,12 +7238,12 @@
     </row>
     <row r="190" ht="14.25">
       <c r="A190" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="B190" s="9"/>
       <c r="C190" s="1"/>
       <c r="D190" s="2" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="E190" s="21" t="s">
         <v>10</v>
@@ -7242,12 +7252,12 @@
     </row>
     <row r="191" ht="14.25">
       <c r="A191" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="B191" s="9"/>
       <c r="C191" s="1"/>
       <c r="D191" s="2" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="E191" s="23" t="s">
         <v>66</v>
@@ -7256,12 +7266,12 @@
     </row>
     <row r="192" ht="14.25">
       <c r="A192" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="B192" s="9"/>
       <c r="C192" s="1"/>
       <c r="D192" s="2" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="E192" s="18" t="s">
         <v>66</v>
@@ -7284,7 +7294,7 @@
     </row>
     <row r="195" ht="14.25">
       <c r="A195" s="5" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="B195" s="5"/>
       <c r="C195" s="5"/>
@@ -7294,619 +7304,619 @@
     </row>
     <row r="196" ht="14.25">
       <c r="A196" s="4" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="B196" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C196" s="4" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="D196" s="4" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="E196" s="4"/>
       <c r="F196" s="4"/>
     </row>
     <row r="197" ht="14.25">
       <c r="A197" s="20" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="B197" s="9"/>
       <c r="C197" s="1" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="F197" s="4"/>
     </row>
     <row r="198" ht="14.25">
       <c r="A198" s="20" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="B198" s="9"/>
       <c r="C198" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="D198" s="2" t="s">
         <v>556</v>
-      </c>
-      <c r="D198" s="2" t="s">
-        <v>554</v>
       </c>
       <c r="F198" s="4"/>
       <c r="H198" s="6"/>
     </row>
     <row r="199" ht="14.25">
       <c r="A199" s="20" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="B199" s="9"/>
       <c r="C199" s="1" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="D199" s="2" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="F199" s="4"/>
     </row>
     <row r="200" ht="14.25">
       <c r="A200" s="20" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="B200" s="9"/>
       <c r="C200" s="1" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="F200" s="4"/>
     </row>
     <row r="201" ht="14.25">
       <c r="A201" s="20" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="B201" s="9"/>
       <c r="C201" s="1" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="F201" s="4"/>
     </row>
     <row r="202" ht="14.25">
       <c r="A202" s="20" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="B202" s="9"/>
       <c r="C202" s="1" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="F202" s="4"/>
     </row>
     <row r="203" ht="14.25">
       <c r="A203" s="20" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="B203" s="9"/>
       <c r="C203" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="D203" s="2" t="s">
         <v>567</v>
-      </c>
-      <c r="D203" s="2" t="s">
-        <v>565</v>
       </c>
       <c r="F203" s="4"/>
       <c r="H203" s="6"/>
     </row>
     <row r="204" ht="14.25">
       <c r="A204" s="20" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="B204" s="9"/>
       <c r="C204" s="1" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="F204" s="4"/>
       <c r="H204" s="6"/>
     </row>
     <row r="205" ht="14.25">
       <c r="A205" s="20" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="B205" s="9"/>
       <c r="C205" s="1" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="D205" s="2" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="F205" s="4"/>
       <c r="H205" s="6"/>
     </row>
     <row r="206" ht="14.25">
       <c r="A206" s="20" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="B206" s="9"/>
       <c r="C206" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="D206" s="2" t="s">
         <v>574</v>
-      </c>
-      <c r="D206" s="2" t="s">
-        <v>572</v>
       </c>
       <c r="F206" s="4"/>
       <c r="H206" s="6"/>
     </row>
     <row r="207" ht="14.25">
       <c r="A207" s="20" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="B207" s="9"/>
       <c r="C207" s="1" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="D207" s="2" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="F207" s="4"/>
       <c r="H207" s="6"/>
     </row>
     <row r="208" ht="14.25">
       <c r="A208" s="20" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c r="B208" s="9"/>
       <c r="C208" s="1" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="D208" s="2" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="F208" s="4"/>
       <c r="H208" s="6"/>
     </row>
     <row r="209" ht="14.25">
       <c r="A209" s="20" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="B209" s="9"/>
       <c r="C209" s="1" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="F209" s="4"/>
       <c r="H209" s="6"/>
     </row>
     <row r="210" ht="14.25">
       <c r="A210" s="20" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="B210" s="9"/>
       <c r="C210" s="1" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="F210" s="4"/>
     </row>
     <row r="211" ht="14.25">
       <c r="A211" s="20" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="B211" s="9"/>
       <c r="C211" s="1" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="D211" s="2" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="F211" s="4"/>
     </row>
     <row r="212" ht="14.25">
       <c r="A212" s="20" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="B212" s="9"/>
       <c r="C212" s="1" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="D212" s="2" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="F212" s="4"/>
     </row>
     <row r="213" ht="14.25">
       <c r="A213" s="20" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="B213" s="9"/>
       <c r="C213" s="1" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="D213" s="2" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="F213" s="4"/>
     </row>
     <row r="214" ht="14.25">
       <c r="A214" s="20" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="B214" s="9"/>
       <c r="C214" s="1" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="D214" s="2" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="F214" s="4"/>
     </row>
     <row r="215" ht="14.25">
       <c r="A215" s="20" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="B215" s="9"/>
       <c r="C215" s="1" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="F215" s="4"/>
     </row>
     <row r="216" ht="14.25">
       <c r="A216" s="20" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="B216" s="9"/>
       <c r="C216" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="D216" s="2" t="s">
         <v>595</v>
-      </c>
-      <c r="D216" s="2" t="s">
-        <v>593</v>
       </c>
       <c r="F216" s="4"/>
     </row>
     <row r="217" ht="14.25">
       <c r="A217" s="20" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="B217" s="9"/>
       <c r="C217" s="1" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="F217" s="4"/>
     </row>
     <row r="218" ht="14.25">
       <c r="A218" s="20" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="B218" s="9"/>
       <c r="C218" s="1" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="F218" s="4"/>
     </row>
     <row r="219" ht="14.25">
       <c r="A219" s="20" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="B219" s="9"/>
       <c r="C219" s="1" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="F219" s="4"/>
     </row>
     <row r="220" ht="14.25">
       <c r="A220" s="20" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="B220" s="9"/>
       <c r="C220" s="1" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="D220" s="2" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="F220" s="4"/>
     </row>
     <row r="221" ht="14.25">
       <c r="A221" s="20" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="B221" s="9"/>
       <c r="C221" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="D221" s="2" t="s">
         <v>606</v>
-      </c>
-      <c r="D221" s="2" t="s">
-        <v>604</v>
       </c>
       <c r="F221" s="4"/>
     </row>
     <row r="222" ht="14.25">
       <c r="A222" s="20" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="B222" s="9"/>
       <c r="C222" s="1" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="D222" s="2" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="F222" s="4"/>
     </row>
     <row r="223" ht="14.25">
       <c r="A223" s="20" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="B223" s="9"/>
       <c r="C223" s="1" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="D223" s="2" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="F223" s="4"/>
     </row>
     <row r="224" ht="14.25">
       <c r="A224" s="20" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="B224" s="9"/>
       <c r="C224" s="1" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="D224" s="2" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="F224" s="4"/>
     </row>
     <row r="225" ht="14.25">
       <c r="A225" s="20" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="B225" s="9"/>
       <c r="C225" s="1" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="D225" s="2" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="F225" s="4"/>
     </row>
     <row r="226" ht="14.25">
       <c r="A226" s="20" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="B226" s="9"/>
       <c r="C226" s="1" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="D226" s="2" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="F226" s="4"/>
     </row>
     <row r="227" ht="14.25">
       <c r="A227" s="20" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="B227" s="9"/>
       <c r="C227" s="1" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="D227" s="2" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="F227" s="4"/>
     </row>
     <row r="228" ht="14.25">
       <c r="A228" s="20" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="B228" s="9"/>
       <c r="C228" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="D228" s="2" t="s">
         <v>621</v>
-      </c>
-      <c r="D228" s="2" t="s">
-        <v>619</v>
       </c>
       <c r="F228" s="4"/>
     </row>
     <row r="229" ht="14.25">
       <c r="A229" s="20" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
       <c r="B229" s="9"/>
       <c r="C229" s="1" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c r="D229" s="2" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="F229" s="4"/>
     </row>
     <row r="230" ht="14.25">
       <c r="A230" s="20" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="B230" s="9"/>
       <c r="C230" s="1" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="D230" s="2" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="F230" s="4"/>
     </row>
     <row r="231" ht="14.25">
       <c r="A231" s="20" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="B231" s="9"/>
       <c r="C231" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="D231" s="2" t="s">
         <v>628</v>
-      </c>
-      <c r="D231" s="2" t="s">
-        <v>626</v>
       </c>
       <c r="F231" s="4"/>
     </row>
     <row r="232" ht="14.25">
       <c r="A232" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
       <c r="B232" s="9"/>
       <c r="C232" s="1" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="D232" s="2" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
       <c r="F232" s="4"/>
       <c r="H232" s="6"/>
     </row>
     <row r="233" ht="14.25">
       <c r="A233" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
       <c r="B233" s="9"/>
       <c r="C233" s="1" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="D233" s="2" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="F233" s="4"/>
       <c r="H233" s="6"/>
     </row>
     <row r="234" ht="14.25">
       <c r="A234" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
       <c r="B234" s="9"/>
       <c r="C234" s="1" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="D234" s="2" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c r="F234" s="4"/>
       <c r="H234" s="6"/>
     </row>
     <row r="235" ht="14.25">
       <c r="A235" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="B235" s="9"/>
       <c r="C235" s="1" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="D235" s="2" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="F235" s="4"/>
       <c r="H235" s="6"/>
     </row>
     <row r="236" ht="14.25">
       <c r="A236" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="B236" s="9"/>
       <c r="C236" s="1" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="D236" s="2" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="F236" s="4"/>
       <c r="H236" s="6"/>
     </row>
     <row r="237" ht="14.25">
       <c r="A237" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="B237" s="9"/>
       <c r="C237" s="1" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="D237" s="2" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="F237" s="4"/>
       <c r="H237" s="6"/>
     </row>
     <row r="238" ht="14.25">
       <c r="A238" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="B238" s="9"/>
       <c r="C238" s="1" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="D238" s="2" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="F238" s="4"/>
       <c r="H238" s="6"/>
     </row>
     <row r="239" ht="14.25">
       <c r="A239" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="B239" s="9"/>
       <c r="C239" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="D239" s="2" t="s">
         <v>650</v>
-      </c>
-      <c r="D239" s="2" t="s">
-        <v>648</v>
       </c>
       <c r="F239" s="4"/>
       <c r="H239" s="6"/>
     </row>
     <row r="240" ht="14.25">
       <c r="A240" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="B240" s="9"/>
       <c r="C240" s="1" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="D240" s="2" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="F240" s="4"/>
       <c r="H240" s="6"/>
     </row>
     <row r="241" ht="14.25">
       <c r="A241" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c r="B241" s="9"/>
       <c r="C241" s="1" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c r="D241" s="2" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c r="E241" s="3"/>
       <c r="F241" s="4"/>
@@ -7914,14 +7924,14 @@
     </row>
     <row r="242" ht="14.25">
       <c r="A242" t="s">
-        <v>656</v>
+        <v>658</v>
       </c>
       <c r="B242" s="9"/>
       <c r="C242" s="1" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="D242" s="2" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="E242" s="3"/>
       <c r="F242" s="4"/>
@@ -7929,14 +7939,14 @@
     </row>
     <row r="243" ht="14.25">
       <c r="A243" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="B243" s="9"/>
       <c r="C243" s="1" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="D243" s="2" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="E243" s="3"/>
       <c r="F243" s="4"/>
@@ -7944,14 +7954,14 @@
     </row>
     <row r="244" ht="14.25">
       <c r="A244" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="B244" s="9"/>
       <c r="C244" s="1" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="D244" s="2" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c r="E244" s="3"/>
       <c r="F244" s="4"/>
@@ -7959,14 +7969,14 @@
     </row>
     <row r="245" ht="14.25">
       <c r="A245" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c r="B245" s="9"/>
       <c r="C245" s="1" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="D245" s="2" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="E245" s="3"/>
       <c r="F245" s="4"/>
@@ -7974,14 +7984,14 @@
     </row>
     <row r="246" ht="14.25">
       <c r="A246" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c r="B246" s="9"/>
       <c r="C246" s="1" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c r="D246" s="2" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="E246" s="3"/>
       <c r="F246" s="4"/>
@@ -8003,7 +8013,7 @@
     </row>
     <row r="249" ht="14.25">
       <c r="A249" s="5" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="B249" s="5"/>
       <c r="C249" s="5"/>
@@ -8031,12 +8041,12 @@
     </row>
     <row r="251" ht="14.25">
       <c r="A251" s="20" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="B251" s="9"/>
       <c r="C251" s="1"/>
       <c r="D251" s="25" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="E251" s="16" t="s">
         <v>10</v>
@@ -8045,12 +8055,12 @@
     </row>
     <row r="252" ht="14.25">
       <c r="A252" s="20" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="B252" s="9"/>
       <c r="C252" s="1"/>
       <c r="D252" s="25" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="E252" s="21" t="s">
         <v>10</v>
@@ -8059,12 +8069,12 @@
     </row>
     <row r="253" ht="14.25">
       <c r="A253" s="20" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c r="B253" s="9"/>
       <c r="C253" s="1"/>
       <c r="D253" s="25" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="E253" s="21" t="s">
         <v>10</v>
@@ -8073,12 +8083,12 @@
     </row>
     <row r="254" ht="14.25">
       <c r="A254" s="20" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="B254" s="9"/>
       <c r="C254" s="1"/>
       <c r="D254" s="25" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="E254" s="21" t="s">
         <v>10</v>
@@ -8087,12 +8097,12 @@
     </row>
     <row r="255" ht="14.25">
       <c r="A255" s="20" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="B255" s="9"/>
       <c r="C255" s="1"/>
       <c r="D255" s="25" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="E255" s="21" t="s">
         <v>10</v>
@@ -8101,12 +8111,12 @@
     </row>
     <row r="256" ht="14.25">
       <c r="A256" s="20" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="B256" s="9"/>
       <c r="C256" s="1"/>
       <c r="D256" s="25" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="E256" s="21" t="s">
         <v>10</v>
@@ -8115,12 +8125,12 @@
     </row>
     <row r="257" ht="14.25">
       <c r="A257" s="20" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="B257" s="9"/>
       <c r="C257" s="1"/>
       <c r="D257" s="25" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="E257" s="21" t="s">
         <v>10</v>
@@ -8129,12 +8139,12 @@
     </row>
     <row r="258" ht="14.25">
       <c r="A258" s="20" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="B258" s="9"/>
       <c r="C258" s="1"/>
       <c r="D258" s="25" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="E258" s="21" t="s">
         <v>10</v>
@@ -8143,12 +8153,12 @@
     </row>
     <row r="259" ht="14.25">
       <c r="A259" s="20" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="B259" s="9"/>
       <c r="C259" s="1"/>
       <c r="D259" s="25" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="E259" s="21" t="s">
         <v>10</v>
@@ -8157,12 +8167,12 @@
     </row>
     <row r="260" ht="14.25">
       <c r="A260" s="20" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="B260" s="9"/>
       <c r="C260" s="1"/>
       <c r="D260" s="25" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="E260" s="23" t="s">
         <v>66</v>
@@ -8171,12 +8181,12 @@
     </row>
     <row r="261" ht="14.25">
       <c r="A261" s="20" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="B261" s="9"/>
       <c r="C261" s="1"/>
       <c r="D261" s="25" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="E261" s="21" t="s">
         <v>10</v>
@@ -8185,12 +8195,12 @@
     </row>
     <row r="262" ht="14.25">
       <c r="A262" s="20" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="B262" s="9"/>
       <c r="C262" s="1"/>
       <c r="D262" s="25" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="E262" s="23" t="s">
         <v>66</v>
@@ -8199,12 +8209,12 @@
     </row>
     <row r="263" ht="14.25">
       <c r="A263" s="20" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="B263" s="9"/>
       <c r="C263" s="1"/>
       <c r="D263" s="25" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c r="E263" s="21" t="s">
         <v>10</v>
@@ -8218,7 +8228,7 @@
       <c r="B264" s="9"/>
       <c r="C264" s="1"/>
       <c r="D264" s="25" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="E264" s="23" t="s">
         <v>66</v>
@@ -8232,7 +8242,7 @@
       <c r="B265" s="9"/>
       <c r="C265" s="1"/>
       <c r="D265" s="25" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="E265" s="21" t="s">
         <v>10</v>
@@ -8241,12 +8251,12 @@
     </row>
     <row r="266" ht="14.25">
       <c r="A266" s="20" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="B266" s="9"/>
       <c r="C266" s="1"/>
       <c r="D266" s="25" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
       <c r="E266" s="23" t="s">
         <v>66</v>
@@ -8255,12 +8265,12 @@
     </row>
     <row r="267" ht="14.25">
       <c r="A267" s="20" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="B267" s="9"/>
       <c r="C267" s="1"/>
       <c r="D267" s="25" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="E267" s="21" t="s">
         <v>10</v>
@@ -8269,12 +8279,12 @@
     </row>
     <row r="268" ht="14.25">
       <c r="A268" s="20" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="B268" s="9"/>
       <c r="C268" s="1"/>
       <c r="D268" s="25" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="E268" s="21" t="s">
         <v>10</v>
@@ -8283,12 +8293,12 @@
     </row>
     <row r="269" ht="14.25">
       <c r="A269" s="20" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="B269" s="9"/>
       <c r="C269" s="1"/>
       <c r="D269" s="25" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="E269" s="23" t="s">
         <v>66</v>
@@ -8297,12 +8307,12 @@
     </row>
     <row r="270" ht="14.25">
       <c r="A270" s="20" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="B270" s="9"/>
       <c r="C270" s="1"/>
       <c r="D270" s="25" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="E270" s="21" t="s">
         <v>10</v>
@@ -8311,12 +8321,12 @@
     </row>
     <row r="271" ht="14.25">
       <c r="A271" s="20" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="B271" s="9"/>
       <c r="C271" s="1"/>
       <c r="D271" s="25" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="E271" s="21" t="s">
         <v>10</v>
@@ -8325,12 +8335,12 @@
     </row>
     <row r="272" ht="14.25">
       <c r="A272" s="20" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="B272" s="9"/>
       <c r="C272" s="1"/>
       <c r="D272" s="25" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="E272" s="21" t="s">
         <v>10</v>
@@ -8339,12 +8349,12 @@
     </row>
     <row r="273" ht="14.25">
       <c r="A273" s="20" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="B273" s="9"/>
       <c r="C273" s="1"/>
       <c r="D273" s="25" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="E273" s="23" t="s">
         <v>66</v>
@@ -8353,12 +8363,12 @@
     </row>
     <row r="274" ht="14.25">
       <c r="A274" s="20" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="B274" s="9"/>
       <c r="C274" s="1"/>
       <c r="D274" s="25" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="E274" s="21" t="s">
         <v>10</v>
@@ -8367,12 +8377,12 @@
     </row>
     <row r="275" ht="14.25">
       <c r="A275" s="20" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="B275" s="9"/>
       <c r="C275" s="1"/>
       <c r="D275" s="25" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="E275" s="23" t="s">
         <v>66</v>
@@ -8381,12 +8391,12 @@
     </row>
     <row r="276" ht="14.25">
       <c r="A276" s="20" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="B276" s="9"/>
       <c r="C276" s="1"/>
       <c r="D276" s="25" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="E276" s="21" t="s">
         <v>10</v>
@@ -8395,12 +8405,12 @@
     </row>
     <row r="277" ht="14.25">
       <c r="A277" s="20" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="B277" s="9"/>
       <c r="C277" s="1"/>
       <c r="D277" s="25" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="E277" s="21" t="s">
         <v>10</v>
@@ -8409,12 +8419,12 @@
     </row>
     <row r="278" ht="14.25">
       <c r="A278" s="20" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="B278" s="9"/>
       <c r="C278" s="1"/>
       <c r="D278" s="25" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="E278" s="23" t="s">
         <v>66</v>
@@ -8423,12 +8433,12 @@
     </row>
     <row r="279" ht="14.25">
       <c r="A279" s="20" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="B279" s="9"/>
       <c r="C279" s="1"/>
       <c r="D279" s="25" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="E279" s="23" t="s">
         <v>66</v>
@@ -8437,12 +8447,12 @@
     </row>
     <row r="280" ht="14.25">
       <c r="A280" s="20" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="B280" s="9"/>
       <c r="C280" s="1"/>
       <c r="D280" s="25" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c r="E280" s="21" t="s">
         <v>10</v>
@@ -8451,12 +8461,12 @@
     </row>
     <row r="281" ht="14.25">
       <c r="A281" s="20" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="B281" s="9"/>
       <c r="C281" s="1"/>
       <c r="D281" s="25" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="E281" s="23" t="s">
         <v>66</v>
@@ -8465,12 +8475,12 @@
     </row>
     <row r="282" ht="14.25">
       <c r="A282" s="20" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="B282" s="9"/>
       <c r="C282" s="1"/>
       <c r="D282" s="25" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="E282" s="21" t="s">
         <v>10</v>
@@ -8479,12 +8489,12 @@
     </row>
     <row r="283" ht="14.25">
       <c r="A283" s="20" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="B283" s="9"/>
       <c r="C283" s="1"/>
       <c r="D283" s="25" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="E283" s="21" t="s">
         <v>10</v>
@@ -8493,12 +8503,12 @@
     </row>
     <row r="284" ht="14.25">
       <c r="A284" s="20" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="B284" s="9"/>
       <c r="C284" s="1"/>
       <c r="D284" s="25" t="s">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c r="E284" s="21" t="s">
         <v>10</v>
@@ -8507,12 +8517,12 @@
     </row>
     <row r="285" ht="14.25">
       <c r="A285" s="20" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="B285" s="9"/>
       <c r="C285" s="1"/>
       <c r="D285" s="25" t="s">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c r="E285" s="21" t="s">
         <v>10</v>
@@ -8521,12 +8531,12 @@
     </row>
     <row r="286" ht="14.25">
       <c r="A286" s="20" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="B286" s="9"/>
       <c r="C286" s="1"/>
       <c r="D286" s="25" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="E286" s="23" t="s">
         <v>66</v>
@@ -8535,12 +8545,12 @@
     </row>
     <row r="287" ht="14.25">
       <c r="A287" s="20" t="s">
-        <v>731</v>
+        <v>733</v>
       </c>
       <c r="B287" s="9"/>
       <c r="C287" s="1"/>
       <c r="D287" s="25" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="E287" s="21" t="s">
         <v>10</v>
@@ -8549,12 +8559,12 @@
     </row>
     <row r="288" ht="14.25">
       <c r="A288" s="20" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="B288" s="9"/>
       <c r="C288" s="1"/>
       <c r="D288" s="25" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c r="E288" s="21" t="s">
         <v>10</v>
@@ -8563,12 +8573,12 @@
     </row>
     <row r="289" ht="14.25">
       <c r="A289" s="20" t="s">
-        <v>735</v>
+        <v>737</v>
       </c>
       <c r="B289" s="9"/>
       <c r="C289" s="1"/>
       <c r="D289" s="25" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="E289" s="21" t="s">
         <v>10</v>
@@ -8577,12 +8587,12 @@
     </row>
     <row r="290" ht="14.25">
       <c r="A290" s="20" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="B290" s="9"/>
       <c r="C290" s="1"/>
       <c r="D290" s="25" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="E290" s="23" t="s">
         <v>66</v>
@@ -8591,12 +8601,12 @@
     </row>
     <row r="291" ht="14.25">
       <c r="A291" s="20" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="B291" s="9"/>
       <c r="C291" s="1"/>
       <c r="D291" s="25" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="E291" s="16" t="s">
         <v>10</v>
@@ -8981,6 +8991,7 @@
     <hyperlink r:id="rId122" ref="C153"/>
     <hyperlink r:id="rId123" ref="C154"/>
     <hyperlink r:id="rId124" ref="C155"/>
+    <hyperlink r:id="rId125" ref="C156"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
vault backup: 2026-01-11 15:50:21
</commit_message>
<xml_diff>
--- a/Excalidraw/switch.xlsx
+++ b/Excalidraw/switch.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="741">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="744">
   <si>
     <t>DSA</t>
   </si>
@@ -1460,10 +1460,19 @@
     <t xml:space="preserve">Design a Metrics / Monitoring System</t>
   </si>
   <si>
+    <t xml:space="preserve">horizontally scalable, multi-tenant metrics and monitoring system that ingests millions of time-series data points per second using buffered, asynchronous pipelines and stores them efficiently for low-latency querying, visualization, and alerting.</t>
+  </si>
+  <si>
+    <t>https://github.com/yashaggarwal85d/Neural-Vault/blob/main/Excalidraw/Design%20a%20Metrics%20Monitoring%20System.md</t>
+  </si>
+  <si>
     <t xml:space="preserve">Observability (Time Series DB)</t>
   </si>
   <si>
     <t xml:space="preserve">Design a Distributed Message Queue (Kafka)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">distributed message queue using partitioned, replicated append-only logs with leader-follower replication, pull-based consumers, ISR-backed durability, and transactional guarantees to achieve high throughput, fault tolerance, and exactly-once processing at scale.</t>
   </si>
   <si>
     <t xml:space="preserve">Streaming / Log Data</t>
@@ -2986,7 +2995,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A131" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A141" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -6772,13 +6781,17 @@
       <c r="F156" s="4"/>
     </row>
     <row r="157" ht="14.25">
-      <c r="A157" t="s">
+      <c r="A157" s="10" t="s">
         <v>477</v>
       </c>
-      <c r="B157" s="9"/>
-      <c r="C157" s="1"/>
+      <c r="B157" s="9" t="s">
+        <v>478</v>
+      </c>
+      <c r="C157" s="11" t="s">
+        <v>479</v>
+      </c>
       <c r="D157" s="2" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="E157" s="23" t="s">
         <v>66</v>
@@ -6787,12 +6800,14 @@
     </row>
     <row r="158" ht="14.25">
       <c r="A158" t="s">
-        <v>479</v>
-      </c>
-      <c r="B158" s="9"/>
+        <v>481</v>
+      </c>
+      <c r="B158" s="9" t="s">
+        <v>482</v>
+      </c>
       <c r="C158" s="1"/>
       <c r="D158" s="2" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="E158" s="23" t="s">
         <v>66</v>
@@ -6801,12 +6816,12 @@
     </row>
     <row r="159" ht="14.25">
       <c r="A159" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
       <c r="B159" s="9"/>
       <c r="C159" s="1"/>
       <c r="D159" s="2" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="E159" s="23" t="s">
         <v>66</v>
@@ -6815,29 +6830,29 @@
     </row>
     <row r="160" ht="14.25">
       <c r="A160" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="B160" s="9"/>
       <c r="C160" s="1"/>
       <c r="D160" s="2" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="E160" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F160" s="4"/>
       <c r="L160" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
     </row>
     <row r="161" ht="14.25">
       <c r="A161" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="B161" s="9"/>
       <c r="C161" s="1"/>
       <c r="D161" s="2" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="E161" s="21" t="s">
         <v>10</v>
@@ -6846,12 +6861,12 @@
     </row>
     <row r="162" ht="14.25">
       <c r="A162" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="B162" s="9"/>
       <c r="C162" s="1"/>
       <c r="D162" s="2" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
       <c r="E162" s="21" t="s">
         <v>10</v>
@@ -6860,12 +6875,12 @@
     </row>
     <row r="163" ht="14.25">
       <c r="A163" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="B163" s="9"/>
       <c r="C163" s="1"/>
       <c r="D163" s="2" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
       <c r="E163" s="23" t="s">
         <v>66</v>
@@ -6874,12 +6889,12 @@
     </row>
     <row r="164" ht="14.25">
       <c r="A164" s="24" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="B164" s="9"/>
       <c r="C164" s="1"/>
       <c r="D164" s="2" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="E164" s="21" t="s">
         <v>10</v>
@@ -6888,12 +6903,12 @@
     </row>
     <row r="165" ht="14.25">
       <c r="A165" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
       <c r="B165" s="9"/>
       <c r="C165" s="1"/>
       <c r="D165" s="2" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="E165" s="21" t="s">
         <v>10</v>
@@ -6902,12 +6917,12 @@
     </row>
     <row r="166" ht="14.25">
       <c r="A166" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="B166" s="9"/>
       <c r="C166" s="1"/>
       <c r="D166" s="2" t="s">
-        <v>497</v>
+        <v>500</v>
       </c>
       <c r="E166" s="21" t="s">
         <v>10</v>
@@ -6916,12 +6931,12 @@
     </row>
     <row r="167" ht="14.25">
       <c r="A167" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
       <c r="B167" s="9"/>
       <c r="C167" s="1"/>
       <c r="D167" s="2" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
       <c r="E167" s="23" t="s">
         <v>66</v>
@@ -6930,12 +6945,12 @@
     </row>
     <row r="168" ht="14.25">
       <c r="A168" t="s">
-        <v>500</v>
+        <v>503</v>
       </c>
       <c r="B168" s="9"/>
       <c r="C168" s="1"/>
       <c r="D168" s="2" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
       <c r="E168" s="23" t="s">
         <v>66</v>
@@ -6944,12 +6959,12 @@
     </row>
     <row r="169" ht="14.25">
       <c r="A169" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
       <c r="B169" s="9"/>
       <c r="C169" s="1"/>
       <c r="D169" s="2" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="E169" s="23" t="s">
         <v>66</v>
@@ -6958,12 +6973,12 @@
     </row>
     <row r="170" ht="14.25">
       <c r="A170" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
       <c r="B170" s="9"/>
       <c r="C170" s="1"/>
       <c r="D170" s="2" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="E170" s="23" t="s">
         <v>66</v>
@@ -6972,12 +6987,12 @@
     </row>
     <row r="171" ht="14.25">
       <c r="A171" t="s">
-        <v>506</v>
+        <v>509</v>
       </c>
       <c r="B171" s="9"/>
       <c r="C171" s="1"/>
       <c r="D171" s="2" t="s">
-        <v>507</v>
+        <v>510</v>
       </c>
       <c r="E171" s="23" t="s">
         <v>66</v>
@@ -6986,12 +7001,12 @@
     </row>
     <row r="172" ht="14.25">
       <c r="A172" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="B172" s="9"/>
       <c r="C172" s="1"/>
       <c r="D172" s="2" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
       <c r="E172" s="21" t="s">
         <v>10</v>
@@ -7000,12 +7015,12 @@
     </row>
     <row r="173" ht="14.25">
       <c r="A173" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="B173" s="9"/>
       <c r="C173" s="1"/>
       <c r="D173" s="2" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
       <c r="E173" s="21" t="s">
         <v>10</v>
@@ -7014,12 +7029,12 @@
     </row>
     <row r="174" ht="14.25">
       <c r="A174" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="B174" s="9"/>
       <c r="C174" s="1"/>
       <c r="D174" s="2" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
       <c r="E174" s="21" t="s">
         <v>10</v>
@@ -7028,12 +7043,12 @@
     </row>
     <row r="175" ht="14.25">
       <c r="A175" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="B175" s="9"/>
       <c r="C175" s="1"/>
       <c r="D175" s="2" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="E175" s="23" t="s">
         <v>66</v>
@@ -7042,12 +7057,12 @@
     </row>
     <row r="176" ht="14.25">
       <c r="A176" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="B176" s="9"/>
       <c r="C176" s="1"/>
       <c r="D176" s="2" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="E176" s="23" t="s">
         <v>66</v>
@@ -7056,12 +7071,12 @@
     </row>
     <row r="177" ht="14.25">
       <c r="A177" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="B177" s="9"/>
       <c r="C177" s="1"/>
       <c r="D177" s="2" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="E177" s="23" t="s">
         <v>66</v>
@@ -7070,12 +7085,12 @@
     </row>
     <row r="178" ht="14.25">
       <c r="A178" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="B178" s="9"/>
       <c r="C178" s="1"/>
       <c r="D178" s="2" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="E178" s="21" t="s">
         <v>10</v>
@@ -7084,12 +7099,12 @@
     </row>
     <row r="179" ht="14.25">
       <c r="A179" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="B179" s="9"/>
       <c r="C179" s="1"/>
       <c r="D179" s="2" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="E179" s="23" t="s">
         <v>66</v>
@@ -7098,12 +7113,12 @@
     </row>
     <row r="180" ht="14.25">
       <c r="A180" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="B180" s="9"/>
       <c r="C180" s="1"/>
       <c r="D180" s="2" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="E180" s="21" t="s">
         <v>10</v>
@@ -7112,12 +7127,12 @@
     </row>
     <row r="181" ht="14.25">
       <c r="A181" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="B181" s="9"/>
       <c r="C181" s="1"/>
       <c r="D181" s="2" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="E181" s="23" t="s">
         <v>66</v>
@@ -7126,12 +7141,12 @@
     </row>
     <row r="182" ht="14.25">
       <c r="A182" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="B182" s="9"/>
       <c r="C182" s="1"/>
       <c r="D182" s="2" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="E182" s="21" t="s">
         <v>10</v>
@@ -7140,12 +7155,12 @@
     </row>
     <row r="183" ht="14.25">
       <c r="A183" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="B183" s="9"/>
       <c r="C183" s="1"/>
       <c r="D183" s="2" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="E183" s="21" t="s">
         <v>10</v>
@@ -7154,12 +7169,12 @@
     </row>
     <row r="184" ht="14.25">
       <c r="A184" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
       <c r="B184" s="9"/>
       <c r="C184" s="1"/>
       <c r="D184" s="2" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="E184" s="23" t="s">
         <v>66</v>
@@ -7168,12 +7183,12 @@
     </row>
     <row r="185" ht="14.25">
       <c r="A185" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="B185" s="9"/>
       <c r="C185" s="1"/>
       <c r="D185" s="2" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="E185" s="23" t="s">
         <v>66</v>
@@ -7182,12 +7197,12 @@
     </row>
     <row r="186" ht="14.25">
       <c r="A186" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="B186" s="9"/>
       <c r="C186" s="1"/>
       <c r="D186" s="2" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
       <c r="E186" s="23" t="s">
         <v>66</v>
@@ -7196,12 +7211,12 @@
     </row>
     <row r="187" ht="14.25">
       <c r="A187" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
       <c r="B187" s="9"/>
       <c r="C187" s="1"/>
       <c r="D187" s="2" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="E187" s="23" t="s">
         <v>66</v>
@@ -7210,12 +7225,12 @@
     </row>
     <row r="188" ht="14.25">
       <c r="A188" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="B188" s="9"/>
       <c r="C188" s="1"/>
       <c r="D188" s="2" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
       <c r="E188" s="21" t="s">
         <v>10</v>
@@ -7224,12 +7239,12 @@
     </row>
     <row r="189" ht="14.25">
       <c r="A189" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
       <c r="B189" s="9"/>
       <c r="C189" s="1"/>
       <c r="D189" s="2" t="s">
-        <v>543</v>
+        <v>546</v>
       </c>
       <c r="E189" s="23" t="s">
         <v>66</v>
@@ -7238,12 +7253,12 @@
     </row>
     <row r="190" ht="14.25">
       <c r="A190" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="B190" s="9"/>
       <c r="C190" s="1"/>
       <c r="D190" s="2" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
       <c r="E190" s="21" t="s">
         <v>10</v>
@@ -7252,12 +7267,12 @@
     </row>
     <row r="191" ht="14.25">
       <c r="A191" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="B191" s="9"/>
       <c r="C191" s="1"/>
       <c r="D191" s="2" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="E191" s="23" t="s">
         <v>66</v>
@@ -7266,12 +7281,12 @@
     </row>
     <row r="192" ht="14.25">
       <c r="A192" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="B192" s="9"/>
       <c r="C192" s="1"/>
       <c r="D192" s="2" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="E192" s="18" t="s">
         <v>66</v>
@@ -7294,7 +7309,7 @@
     </row>
     <row r="195" ht="14.25">
       <c r="A195" s="5" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="B195" s="5"/>
       <c r="C195" s="5"/>
@@ -7304,619 +7319,619 @@
     </row>
     <row r="196" ht="14.25">
       <c r="A196" s="4" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="B196" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C196" s="4" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
       <c r="D196" s="4" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
       <c r="E196" s="4"/>
       <c r="F196" s="4"/>
     </row>
     <row r="197" ht="14.25">
       <c r="A197" s="20" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
       <c r="B197" s="9"/>
       <c r="C197" s="1" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="F197" s="4"/>
     </row>
     <row r="198" ht="14.25">
       <c r="A198" s="20" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="B198" s="9"/>
       <c r="C198" s="1" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="F198" s="4"/>
       <c r="H198" s="6"/>
     </row>
     <row r="199" ht="14.25">
       <c r="A199" s="20" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="B199" s="9"/>
       <c r="C199" s="1" t="s">
-        <v>560</v>
+        <v>563</v>
       </c>
       <c r="D199" s="2" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="F199" s="4"/>
     </row>
     <row r="200" ht="14.25">
       <c r="A200" s="20" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
       <c r="B200" s="9"/>
       <c r="C200" s="1" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="F200" s="4"/>
     </row>
     <row r="201" ht="14.25">
       <c r="A201" s="20" t="s">
-        <v>563</v>
+        <v>566</v>
       </c>
       <c r="B201" s="9"/>
       <c r="C201" s="1" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="F201" s="4"/>
     </row>
     <row r="202" ht="14.25">
       <c r="A202" s="20" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
       <c r="B202" s="9"/>
       <c r="C202" s="1" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="F202" s="4"/>
     </row>
     <row r="203" ht="14.25">
       <c r="A203" s="20" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="B203" s="9"/>
       <c r="C203" s="1" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="D203" s="2" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="F203" s="4"/>
       <c r="H203" s="6"/>
     </row>
     <row r="204" ht="14.25">
       <c r="A204" s="20" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="B204" s="9"/>
       <c r="C204" s="1" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="F204" s="4"/>
       <c r="H204" s="6"/>
     </row>
     <row r="205" ht="14.25">
       <c r="A205" s="20" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="B205" s="9"/>
       <c r="C205" s="1" t="s">
-        <v>573</v>
+        <v>576</v>
       </c>
       <c r="D205" s="2" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="F205" s="4"/>
       <c r="H205" s="6"/>
     </row>
     <row r="206" ht="14.25">
       <c r="A206" s="20" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
       <c r="B206" s="9"/>
       <c r="C206" s="1" t="s">
-        <v>576</v>
+        <v>579</v>
       </c>
       <c r="D206" s="2" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="F206" s="4"/>
       <c r="H206" s="6"/>
     </row>
     <row r="207" ht="14.25">
       <c r="A207" s="20" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="B207" s="9"/>
       <c r="C207" s="1" t="s">
-        <v>578</v>
+        <v>581</v>
       </c>
       <c r="D207" s="2" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="F207" s="4"/>
       <c r="H207" s="6"/>
     </row>
     <row r="208" ht="14.25">
       <c r="A208" s="20" t="s">
-        <v>579</v>
+        <v>582</v>
       </c>
       <c r="B208" s="9"/>
       <c r="C208" s="1" t="s">
-        <v>580</v>
+        <v>583</v>
       </c>
       <c r="D208" s="2" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="F208" s="4"/>
       <c r="H208" s="6"/>
     </row>
     <row r="209" ht="14.25">
       <c r="A209" s="20" t="s">
-        <v>581</v>
+        <v>584</v>
       </c>
       <c r="B209" s="9"/>
       <c r="C209" s="1" t="s">
-        <v>582</v>
+        <v>585</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="F209" s="4"/>
       <c r="H209" s="6"/>
     </row>
     <row r="210" ht="14.25">
       <c r="A210" s="20" t="s">
-        <v>583</v>
+        <v>586</v>
       </c>
       <c r="B210" s="9"/>
       <c r="C210" s="1" t="s">
-        <v>584</v>
+        <v>587</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="F210" s="4"/>
     </row>
     <row r="211" ht="14.25">
       <c r="A211" s="20" t="s">
-        <v>585</v>
+        <v>588</v>
       </c>
       <c r="B211" s="9"/>
       <c r="C211" s="1" t="s">
-        <v>586</v>
+        <v>589</v>
       </c>
       <c r="D211" s="2" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="F211" s="4"/>
     </row>
     <row r="212" ht="14.25">
       <c r="A212" s="20" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="B212" s="9"/>
       <c r="C212" s="1" t="s">
-        <v>588</v>
+        <v>591</v>
       </c>
       <c r="D212" s="2" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="F212" s="4"/>
     </row>
     <row r="213" ht="14.25">
       <c r="A213" s="20" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
       <c r="B213" s="9"/>
       <c r="C213" s="1" t="s">
-        <v>590</v>
+        <v>593</v>
       </c>
       <c r="D213" s="2" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="F213" s="4"/>
     </row>
     <row r="214" ht="14.25">
       <c r="A214" s="20" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
       <c r="B214" s="9"/>
       <c r="C214" s="1" t="s">
-        <v>592</v>
+        <v>595</v>
       </c>
       <c r="D214" s="2" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="F214" s="4"/>
     </row>
     <row r="215" ht="14.25">
       <c r="A215" s="20" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
       <c r="B215" s="9"/>
       <c r="C215" s="1" t="s">
-        <v>594</v>
+        <v>597</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
       <c r="F215" s="4"/>
     </row>
     <row r="216" ht="14.25">
       <c r="A216" s="20" t="s">
-        <v>596</v>
+        <v>599</v>
       </c>
       <c r="B216" s="9"/>
       <c r="C216" s="1" t="s">
-        <v>597</v>
+        <v>600</v>
       </c>
       <c r="D216" s="2" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
       <c r="F216" s="4"/>
     </row>
     <row r="217" ht="14.25">
       <c r="A217" s="20" t="s">
-        <v>598</v>
+        <v>601</v>
       </c>
       <c r="B217" s="9"/>
       <c r="C217" s="1" t="s">
-        <v>599</v>
+        <v>602</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
       <c r="F217" s="4"/>
     </row>
     <row r="218" ht="14.25">
       <c r="A218" s="20" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="B218" s="9"/>
       <c r="C218" s="1" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
       <c r="F218" s="4"/>
     </row>
     <row r="219" ht="14.25">
       <c r="A219" s="20" t="s">
-        <v>602</v>
+        <v>605</v>
       </c>
       <c r="B219" s="9"/>
       <c r="C219" s="1" t="s">
-        <v>603</v>
+        <v>606</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
       <c r="F219" s="4"/>
     </row>
     <row r="220" ht="14.25">
       <c r="A220" s="20" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
       <c r="B220" s="9"/>
       <c r="C220" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="D220" s="2" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
       <c r="F220" s="4"/>
     </row>
     <row r="221" ht="14.25">
       <c r="A221" s="20" t="s">
-        <v>607</v>
+        <v>610</v>
       </c>
       <c r="B221" s="9"/>
       <c r="C221" s="1" t="s">
-        <v>608</v>
+        <v>611</v>
       </c>
       <c r="D221" s="2" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
       <c r="F221" s="4"/>
     </row>
     <row r="222" ht="14.25">
       <c r="A222" s="20" t="s">
-        <v>609</v>
+        <v>612</v>
       </c>
       <c r="B222" s="9"/>
       <c r="C222" s="1" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="D222" s="2" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
       <c r="F222" s="4"/>
     </row>
     <row r="223" ht="14.25">
       <c r="A223" s="20" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
       <c r="B223" s="9"/>
       <c r="C223" s="1" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
       <c r="D223" s="2" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
       <c r="F223" s="4"/>
     </row>
     <row r="224" ht="14.25">
       <c r="A224" s="20" t="s">
-        <v>613</v>
+        <v>616</v>
       </c>
       <c r="B224" s="9"/>
       <c r="C224" s="1" t="s">
-        <v>614</v>
+        <v>617</v>
       </c>
       <c r="D224" s="2" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
       <c r="F224" s="4"/>
     </row>
     <row r="225" ht="14.25">
       <c r="A225" s="20" t="s">
-        <v>615</v>
+        <v>618</v>
       </c>
       <c r="B225" s="9"/>
       <c r="C225" s="1" t="s">
-        <v>616</v>
+        <v>619</v>
       </c>
       <c r="D225" s="2" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
       <c r="F225" s="4"/>
     </row>
     <row r="226" ht="14.25">
       <c r="A226" s="20" t="s">
-        <v>617</v>
+        <v>620</v>
       </c>
       <c r="B226" s="9"/>
       <c r="C226" s="1" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
       <c r="D226" s="2" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
       <c r="F226" s="4"/>
     </row>
     <row r="227" ht="14.25">
       <c r="A227" s="20" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
       <c r="B227" s="9"/>
       <c r="C227" s="1" t="s">
-        <v>620</v>
+        <v>623</v>
       </c>
       <c r="D227" s="2" t="s">
-        <v>621</v>
+        <v>624</v>
       </c>
       <c r="F227" s="4"/>
     </row>
     <row r="228" ht="14.25">
       <c r="A228" s="20" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
       <c r="B228" s="9"/>
       <c r="C228" s="1" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
       <c r="D228" s="2" t="s">
-        <v>621</v>
+        <v>624</v>
       </c>
       <c r="F228" s="4"/>
     </row>
     <row r="229" ht="14.25">
       <c r="A229" s="20" t="s">
-        <v>624</v>
+        <v>627</v>
       </c>
       <c r="B229" s="9"/>
       <c r="C229" s="1" t="s">
-        <v>625</v>
+        <v>628</v>
       </c>
       <c r="D229" s="2" t="s">
-        <v>621</v>
+        <v>624</v>
       </c>
       <c r="F229" s="4"/>
     </row>
     <row r="230" ht="14.25">
       <c r="A230" s="20" t="s">
-        <v>626</v>
+        <v>629</v>
       </c>
       <c r="B230" s="9"/>
       <c r="C230" s="1" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="D230" s="2" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
       <c r="F230" s="4"/>
     </row>
     <row r="231" ht="14.25">
       <c r="A231" s="20" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="B231" s="9"/>
       <c r="C231" s="1" t="s">
-        <v>630</v>
+        <v>633</v>
       </c>
       <c r="D231" s="2" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
       <c r="F231" s="4"/>
     </row>
     <row r="232" ht="14.25">
       <c r="A232" t="s">
-        <v>631</v>
+        <v>634</v>
       </c>
       <c r="B232" s="9"/>
       <c r="C232" s="1" t="s">
-        <v>632</v>
+        <v>635</v>
       </c>
       <c r="D232" s="2" t="s">
-        <v>633</v>
+        <v>636</v>
       </c>
       <c r="F232" s="4"/>
       <c r="H232" s="6"/>
     </row>
     <row r="233" ht="14.25">
       <c r="A233" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
       <c r="B233" s="9"/>
       <c r="C233" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="D233" s="2" t="s">
-        <v>636</v>
+        <v>639</v>
       </c>
       <c r="F233" s="4"/>
       <c r="H233" s="6"/>
     </row>
     <row r="234" ht="14.25">
       <c r="A234" t="s">
-        <v>637</v>
+        <v>640</v>
       </c>
       <c r="B234" s="9"/>
       <c r="C234" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="D234" s="2" t="s">
-        <v>639</v>
+        <v>642</v>
       </c>
       <c r="F234" s="4"/>
       <c r="H234" s="6"/>
     </row>
     <row r="235" ht="14.25">
       <c r="A235" t="s">
-        <v>640</v>
+        <v>643</v>
       </c>
       <c r="B235" s="9"/>
       <c r="C235" s="1" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
       <c r="D235" s="2" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="F235" s="4"/>
       <c r="H235" s="6"/>
     </row>
     <row r="236" ht="14.25">
       <c r="A236" t="s">
-        <v>642</v>
+        <v>645</v>
       </c>
       <c r="B236" s="9"/>
       <c r="C236" s="1" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
       <c r="D236" s="2" t="s">
-        <v>644</v>
+        <v>647</v>
       </c>
       <c r="F236" s="4"/>
       <c r="H236" s="6"/>
     </row>
     <row r="237" ht="14.25">
       <c r="A237" t="s">
-        <v>645</v>
+        <v>648</v>
       </c>
       <c r="B237" s="9"/>
       <c r="C237" s="1" t="s">
-        <v>646</v>
+        <v>649</v>
       </c>
       <c r="D237" s="2" t="s">
-        <v>647</v>
+        <v>650</v>
       </c>
       <c r="F237" s="4"/>
       <c r="H237" s="6"/>
     </row>
     <row r="238" ht="14.25">
       <c r="A238" t="s">
-        <v>648</v>
+        <v>651</v>
       </c>
       <c r="B238" s="9"/>
       <c r="C238" s="1" t="s">
-        <v>649</v>
+        <v>652</v>
       </c>
       <c r="D238" s="2" t="s">
-        <v>650</v>
+        <v>653</v>
       </c>
       <c r="F238" s="4"/>
       <c r="H238" s="6"/>
     </row>
     <row r="239" ht="14.25">
       <c r="A239" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
       <c r="B239" s="9"/>
       <c r="C239" s="1" t="s">
-        <v>652</v>
+        <v>655</v>
       </c>
       <c r="D239" s="2" t="s">
-        <v>650</v>
+        <v>653</v>
       </c>
       <c r="F239" s="4"/>
       <c r="H239" s="6"/>
     </row>
     <row r="240" ht="14.25">
       <c r="A240" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="B240" s="9"/>
       <c r="C240" s="1" t="s">
-        <v>654</v>
+        <v>657</v>
       </c>
       <c r="D240" s="2" t="s">
-        <v>650</v>
+        <v>653</v>
       </c>
       <c r="F240" s="4"/>
       <c r="H240" s="6"/>
     </row>
     <row r="241" ht="14.25">
       <c r="A241" t="s">
-        <v>655</v>
+        <v>658</v>
       </c>
       <c r="B241" s="9"/>
       <c r="C241" s="1" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
       <c r="D241" s="2" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
       <c r="E241" s="3"/>
       <c r="F241" s="4"/>
@@ -7924,14 +7939,14 @@
     </row>
     <row r="242" ht="14.25">
       <c r="A242" t="s">
-        <v>658</v>
+        <v>661</v>
       </c>
       <c r="B242" s="9"/>
       <c r="C242" s="1" t="s">
-        <v>659</v>
+        <v>662</v>
       </c>
       <c r="D242" s="2" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="E242" s="3"/>
       <c r="F242" s="4"/>
@@ -7939,14 +7954,14 @@
     </row>
     <row r="243" ht="14.25">
       <c r="A243" t="s">
-        <v>661</v>
+        <v>664</v>
       </c>
       <c r="B243" s="9"/>
       <c r="C243" s="1" t="s">
-        <v>662</v>
+        <v>665</v>
       </c>
       <c r="D243" s="2" t="s">
-        <v>650</v>
+        <v>653</v>
       </c>
       <c r="E243" s="3"/>
       <c r="F243" s="4"/>
@@ -7954,14 +7969,14 @@
     </row>
     <row r="244" ht="14.25">
       <c r="A244" t="s">
-        <v>663</v>
+        <v>666</v>
       </c>
       <c r="B244" s="9"/>
       <c r="C244" s="1" t="s">
-        <v>664</v>
+        <v>667</v>
       </c>
       <c r="D244" s="2" t="s">
-        <v>665</v>
+        <v>668</v>
       </c>
       <c r="E244" s="3"/>
       <c r="F244" s="4"/>
@@ -7969,14 +7984,14 @@
     </row>
     <row r="245" ht="14.25">
       <c r="A245" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
       <c r="B245" s="9"/>
       <c r="C245" s="1" t="s">
-        <v>667</v>
+        <v>670</v>
       </c>
       <c r="D245" s="2" t="s">
-        <v>668</v>
+        <v>671</v>
       </c>
       <c r="E245" s="3"/>
       <c r="F245" s="4"/>
@@ -7984,14 +7999,14 @@
     </row>
     <row r="246" ht="14.25">
       <c r="A246" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
       <c r="B246" s="9"/>
       <c r="C246" s="1" t="s">
-        <v>670</v>
+        <v>673</v>
       </c>
       <c r="D246" s="2" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
       <c r="E246" s="3"/>
       <c r="F246" s="4"/>
@@ -8013,7 +8028,7 @@
     </row>
     <row r="249" ht="14.25">
       <c r="A249" s="5" t="s">
-        <v>672</v>
+        <v>675</v>
       </c>
       <c r="B249" s="5"/>
       <c r="C249" s="5"/>
@@ -8041,12 +8056,12 @@
     </row>
     <row r="251" ht="14.25">
       <c r="A251" s="20" t="s">
-        <v>673</v>
+        <v>676</v>
       </c>
       <c r="B251" s="9"/>
       <c r="C251" s="1"/>
       <c r="D251" s="25" t="s">
-        <v>674</v>
+        <v>677</v>
       </c>
       <c r="E251" s="16" t="s">
         <v>10</v>
@@ -8055,12 +8070,12 @@
     </row>
     <row r="252" ht="14.25">
       <c r="A252" s="20" t="s">
-        <v>675</v>
+        <v>678</v>
       </c>
       <c r="B252" s="9"/>
       <c r="C252" s="1"/>
       <c r="D252" s="25" t="s">
-        <v>676</v>
+        <v>679</v>
       </c>
       <c r="E252" s="21" t="s">
         <v>10</v>
@@ -8069,12 +8084,12 @@
     </row>
     <row r="253" ht="14.25">
       <c r="A253" s="20" t="s">
-        <v>677</v>
+        <v>680</v>
       </c>
       <c r="B253" s="9"/>
       <c r="C253" s="1"/>
       <c r="D253" s="25" t="s">
-        <v>678</v>
+        <v>681</v>
       </c>
       <c r="E253" s="21" t="s">
         <v>10</v>
@@ -8083,12 +8098,12 @@
     </row>
     <row r="254" ht="14.25">
       <c r="A254" s="20" t="s">
-        <v>679</v>
+        <v>682</v>
       </c>
       <c r="B254" s="9"/>
       <c r="C254" s="1"/>
       <c r="D254" s="25" t="s">
-        <v>680</v>
+        <v>683</v>
       </c>
       <c r="E254" s="21" t="s">
         <v>10</v>
@@ -8097,12 +8112,12 @@
     </row>
     <row r="255" ht="14.25">
       <c r="A255" s="20" t="s">
-        <v>681</v>
+        <v>684</v>
       </c>
       <c r="B255" s="9"/>
       <c r="C255" s="1"/>
       <c r="D255" s="25" t="s">
-        <v>682</v>
+        <v>685</v>
       </c>
       <c r="E255" s="21" t="s">
         <v>10</v>
@@ -8111,12 +8126,12 @@
     </row>
     <row r="256" ht="14.25">
       <c r="A256" s="20" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="B256" s="9"/>
       <c r="C256" s="1"/>
       <c r="D256" s="25" t="s">
-        <v>682</v>
+        <v>685</v>
       </c>
       <c r="E256" s="21" t="s">
         <v>10</v>
@@ -8125,12 +8140,12 @@
     </row>
     <row r="257" ht="14.25">
       <c r="A257" s="20" t="s">
-        <v>684</v>
+        <v>687</v>
       </c>
       <c r="B257" s="9"/>
       <c r="C257" s="1"/>
       <c r="D257" s="25" t="s">
-        <v>676</v>
+        <v>679</v>
       </c>
       <c r="E257" s="21" t="s">
         <v>10</v>
@@ -8139,12 +8154,12 @@
     </row>
     <row r="258" ht="14.25">
       <c r="A258" s="20" t="s">
-        <v>685</v>
+        <v>688</v>
       </c>
       <c r="B258" s="9"/>
       <c r="C258" s="1"/>
       <c r="D258" s="25" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="E258" s="21" t="s">
         <v>10</v>
@@ -8153,12 +8168,12 @@
     </row>
     <row r="259" ht="14.25">
       <c r="A259" s="20" t="s">
-        <v>687</v>
+        <v>690</v>
       </c>
       <c r="B259" s="9"/>
       <c r="C259" s="1"/>
       <c r="D259" s="25" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="E259" s="21" t="s">
         <v>10</v>
@@ -8167,12 +8182,12 @@
     </row>
     <row r="260" ht="14.25">
       <c r="A260" s="20" t="s">
-        <v>688</v>
+        <v>691</v>
       </c>
       <c r="B260" s="9"/>
       <c r="C260" s="1"/>
       <c r="D260" s="25" t="s">
-        <v>689</v>
+        <v>692</v>
       </c>
       <c r="E260" s="23" t="s">
         <v>66</v>
@@ -8181,12 +8196,12 @@
     </row>
     <row r="261" ht="14.25">
       <c r="A261" s="20" t="s">
-        <v>690</v>
+        <v>693</v>
       </c>
       <c r="B261" s="9"/>
       <c r="C261" s="1"/>
       <c r="D261" s="25" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="E261" s="21" t="s">
         <v>10</v>
@@ -8195,12 +8210,12 @@
     </row>
     <row r="262" ht="14.25">
       <c r="A262" s="20" t="s">
-        <v>691</v>
+        <v>694</v>
       </c>
       <c r="B262" s="9"/>
       <c r="C262" s="1"/>
       <c r="D262" s="25" t="s">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="E262" s="23" t="s">
         <v>66</v>
@@ -8209,12 +8224,12 @@
     </row>
     <row r="263" ht="14.25">
       <c r="A263" s="20" t="s">
-        <v>693</v>
+        <v>696</v>
       </c>
       <c r="B263" s="9"/>
       <c r="C263" s="1"/>
       <c r="D263" s="25" t="s">
-        <v>694</v>
+        <v>697</v>
       </c>
       <c r="E263" s="21" t="s">
         <v>10</v>
@@ -8228,7 +8243,7 @@
       <c r="B264" s="9"/>
       <c r="C264" s="1"/>
       <c r="D264" s="25" t="s">
-        <v>695</v>
+        <v>698</v>
       </c>
       <c r="E264" s="23" t="s">
         <v>66</v>
@@ -8242,7 +8257,7 @@
       <c r="B265" s="9"/>
       <c r="C265" s="1"/>
       <c r="D265" s="25" t="s">
-        <v>696</v>
+        <v>699</v>
       </c>
       <c r="E265" s="21" t="s">
         <v>10</v>
@@ -8251,12 +8266,12 @@
     </row>
     <row r="266" ht="14.25">
       <c r="A266" s="20" t="s">
-        <v>697</v>
+        <v>700</v>
       </c>
       <c r="B266" s="9"/>
       <c r="C266" s="1"/>
       <c r="D266" s="25" t="s">
-        <v>698</v>
+        <v>701</v>
       </c>
       <c r="E266" s="23" t="s">
         <v>66</v>
@@ -8265,12 +8280,12 @@
     </row>
     <row r="267" ht="14.25">
       <c r="A267" s="20" t="s">
-        <v>699</v>
+        <v>702</v>
       </c>
       <c r="B267" s="9"/>
       <c r="C267" s="1"/>
       <c r="D267" s="25" t="s">
-        <v>700</v>
+        <v>703</v>
       </c>
       <c r="E267" s="21" t="s">
         <v>10</v>
@@ -8279,12 +8294,12 @@
     </row>
     <row r="268" ht="14.25">
       <c r="A268" s="20" t="s">
-        <v>701</v>
+        <v>704</v>
       </c>
       <c r="B268" s="9"/>
       <c r="C268" s="1"/>
       <c r="D268" s="25" t="s">
-        <v>702</v>
+        <v>705</v>
       </c>
       <c r="E268" s="21" t="s">
         <v>10</v>
@@ -8293,12 +8308,12 @@
     </row>
     <row r="269" ht="14.25">
       <c r="A269" s="20" t="s">
-        <v>703</v>
+        <v>706</v>
       </c>
       <c r="B269" s="9"/>
       <c r="C269" s="1"/>
       <c r="D269" s="25" t="s">
-        <v>704</v>
+        <v>707</v>
       </c>
       <c r="E269" s="23" t="s">
         <v>66</v>
@@ -8307,12 +8322,12 @@
     </row>
     <row r="270" ht="14.25">
       <c r="A270" s="20" t="s">
-        <v>705</v>
+        <v>708</v>
       </c>
       <c r="B270" s="9"/>
       <c r="C270" s="1"/>
       <c r="D270" s="25" t="s">
-        <v>682</v>
+        <v>685</v>
       </c>
       <c r="E270" s="21" t="s">
         <v>10</v>
@@ -8321,12 +8336,12 @@
     </row>
     <row r="271" ht="14.25">
       <c r="A271" s="20" t="s">
-        <v>706</v>
+        <v>709</v>
       </c>
       <c r="B271" s="9"/>
       <c r="C271" s="1"/>
       <c r="D271" s="25" t="s">
-        <v>707</v>
+        <v>710</v>
       </c>
       <c r="E271" s="21" t="s">
         <v>10</v>
@@ -8335,12 +8350,12 @@
     </row>
     <row r="272" ht="14.25">
       <c r="A272" s="20" t="s">
-        <v>708</v>
+        <v>711</v>
       </c>
       <c r="B272" s="9"/>
       <c r="C272" s="1"/>
       <c r="D272" s="25" t="s">
-        <v>682</v>
+        <v>685</v>
       </c>
       <c r="E272" s="21" t="s">
         <v>10</v>
@@ -8349,12 +8364,12 @@
     </row>
     <row r="273" ht="14.25">
       <c r="A273" s="20" t="s">
-        <v>709</v>
+        <v>712</v>
       </c>
       <c r="B273" s="9"/>
       <c r="C273" s="1"/>
       <c r="D273" s="25" t="s">
-        <v>710</v>
+        <v>713</v>
       </c>
       <c r="E273" s="23" t="s">
         <v>66</v>
@@ -8363,12 +8378,12 @@
     </row>
     <row r="274" ht="14.25">
       <c r="A274" s="20" t="s">
-        <v>711</v>
+        <v>714</v>
       </c>
       <c r="B274" s="9"/>
       <c r="C274" s="1"/>
       <c r="D274" s="25" t="s">
-        <v>712</v>
+        <v>715</v>
       </c>
       <c r="E274" s="21" t="s">
         <v>10</v>
@@ -8377,12 +8392,12 @@
     </row>
     <row r="275" ht="14.25">
       <c r="A275" s="20" t="s">
-        <v>713</v>
+        <v>716</v>
       </c>
       <c r="B275" s="9"/>
       <c r="C275" s="1"/>
       <c r="D275" s="25" t="s">
-        <v>700</v>
+        <v>703</v>
       </c>
       <c r="E275" s="23" t="s">
         <v>66</v>
@@ -8391,12 +8406,12 @@
     </row>
     <row r="276" ht="14.25">
       <c r="A276" s="20" t="s">
-        <v>714</v>
+        <v>717</v>
       </c>
       <c r="B276" s="9"/>
       <c r="C276" s="1"/>
       <c r="D276" s="25" t="s">
-        <v>715</v>
+        <v>718</v>
       </c>
       <c r="E276" s="21" t="s">
         <v>10</v>
@@ -8405,12 +8420,12 @@
     </row>
     <row r="277" ht="14.25">
       <c r="A277" s="20" t="s">
-        <v>716</v>
+        <v>719</v>
       </c>
       <c r="B277" s="9"/>
       <c r="C277" s="1"/>
       <c r="D277" s="25" t="s">
-        <v>674</v>
+        <v>677</v>
       </c>
       <c r="E277" s="21" t="s">
         <v>10</v>
@@ -8419,12 +8434,12 @@
     </row>
     <row r="278" ht="14.25">
       <c r="A278" s="20" t="s">
-        <v>717</v>
+        <v>720</v>
       </c>
       <c r="B278" s="9"/>
       <c r="C278" s="1"/>
       <c r="D278" s="25" t="s">
-        <v>718</v>
+        <v>721</v>
       </c>
       <c r="E278" s="23" t="s">
         <v>66</v>
@@ -8433,12 +8448,12 @@
     </row>
     <row r="279" ht="14.25">
       <c r="A279" s="20" t="s">
-        <v>719</v>
+        <v>722</v>
       </c>
       <c r="B279" s="9"/>
       <c r="C279" s="1"/>
       <c r="D279" s="25" t="s">
-        <v>720</v>
+        <v>723</v>
       </c>
       <c r="E279" s="23" t="s">
         <v>66</v>
@@ -8447,12 +8462,12 @@
     </row>
     <row r="280" ht="14.25">
       <c r="A280" s="20" t="s">
-        <v>721</v>
+        <v>724</v>
       </c>
       <c r="B280" s="9"/>
       <c r="C280" s="1"/>
       <c r="D280" s="25" t="s">
-        <v>722</v>
+        <v>725</v>
       </c>
       <c r="E280" s="21" t="s">
         <v>10</v>
@@ -8461,12 +8476,12 @@
     </row>
     <row r="281" ht="14.25">
       <c r="A281" s="20" t="s">
-        <v>723</v>
+        <v>726</v>
       </c>
       <c r="B281" s="9"/>
       <c r="C281" s="1"/>
       <c r="D281" s="25" t="s">
-        <v>724</v>
+        <v>727</v>
       </c>
       <c r="E281" s="23" t="s">
         <v>66</v>
@@ -8475,12 +8490,12 @@
     </row>
     <row r="282" ht="14.25">
       <c r="A282" s="20" t="s">
-        <v>725</v>
+        <v>728</v>
       </c>
       <c r="B282" s="9"/>
       <c r="C282" s="1"/>
       <c r="D282" s="25" t="s">
-        <v>726</v>
+        <v>729</v>
       </c>
       <c r="E282" s="21" t="s">
         <v>10</v>
@@ -8489,12 +8504,12 @@
     </row>
     <row r="283" ht="14.25">
       <c r="A283" s="20" t="s">
-        <v>727</v>
+        <v>730</v>
       </c>
       <c r="B283" s="9"/>
       <c r="C283" s="1"/>
       <c r="D283" s="25" t="s">
-        <v>682</v>
+        <v>685</v>
       </c>
       <c r="E283" s="21" t="s">
         <v>10</v>
@@ -8503,12 +8518,12 @@
     </row>
     <row r="284" ht="14.25">
       <c r="A284" s="20" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="B284" s="9"/>
       <c r="C284" s="1"/>
       <c r="D284" s="25" t="s">
-        <v>729</v>
+        <v>732</v>
       </c>
       <c r="E284" s="21" t="s">
         <v>10</v>
@@ -8517,12 +8532,12 @@
     </row>
     <row r="285" ht="14.25">
       <c r="A285" s="20" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="B285" s="9"/>
       <c r="C285" s="1"/>
       <c r="D285" s="25" t="s">
-        <v>730</v>
+        <v>733</v>
       </c>
       <c r="E285" s="21" t="s">
         <v>10</v>
@@ -8531,12 +8546,12 @@
     </row>
     <row r="286" ht="14.25">
       <c r="A286" s="20" t="s">
-        <v>731</v>
+        <v>734</v>
       </c>
       <c r="B286" s="9"/>
       <c r="C286" s="1"/>
       <c r="D286" s="25" t="s">
-        <v>732</v>
+        <v>735</v>
       </c>
       <c r="E286" s="23" t="s">
         <v>66</v>
@@ -8545,12 +8560,12 @@
     </row>
     <row r="287" ht="14.25">
       <c r="A287" s="20" t="s">
-        <v>733</v>
+        <v>736</v>
       </c>
       <c r="B287" s="9"/>
       <c r="C287" s="1"/>
       <c r="D287" s="25" t="s">
-        <v>734</v>
+        <v>737</v>
       </c>
       <c r="E287" s="21" t="s">
         <v>10</v>
@@ -8559,12 +8574,12 @@
     </row>
     <row r="288" ht="14.25">
       <c r="A288" s="20" t="s">
-        <v>735</v>
+        <v>738</v>
       </c>
       <c r="B288" s="9"/>
       <c r="C288" s="1"/>
       <c r="D288" s="25" t="s">
-        <v>736</v>
+        <v>739</v>
       </c>
       <c r="E288" s="21" t="s">
         <v>10</v>
@@ -8573,12 +8588,12 @@
     </row>
     <row r="289" ht="14.25">
       <c r="A289" s="20" t="s">
-        <v>737</v>
+        <v>740</v>
       </c>
       <c r="B289" s="9"/>
       <c r="C289" s="1"/>
       <c r="D289" s="25" t="s">
-        <v>682</v>
+        <v>685</v>
       </c>
       <c r="E289" s="21" t="s">
         <v>10</v>
@@ -8587,12 +8602,12 @@
     </row>
     <row r="290" ht="14.25">
       <c r="A290" s="20" t="s">
-        <v>738</v>
+        <v>741</v>
       </c>
       <c r="B290" s="9"/>
       <c r="C290" s="1"/>
       <c r="D290" s="25" t="s">
-        <v>702</v>
+        <v>705</v>
       </c>
       <c r="E290" s="23" t="s">
         <v>66</v>
@@ -8601,12 +8616,12 @@
     </row>
     <row r="291" ht="14.25">
       <c r="A291" s="20" t="s">
-        <v>739</v>
+        <v>742</v>
       </c>
       <c r="B291" s="9"/>
       <c r="C291" s="1"/>
       <c r="D291" s="25" t="s">
-        <v>740</v>
+        <v>743</v>
       </c>
       <c r="E291" s="16" t="s">
         <v>10</v>
@@ -8992,6 +9007,7 @@
     <hyperlink r:id="rId123" ref="C154"/>
     <hyperlink r:id="rId124" ref="C155"/>
     <hyperlink r:id="rId125" ref="C156"/>
+    <hyperlink r:id="rId126" ref="C157"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
vault backup: 2026-01-12 14:33:33
</commit_message>
<xml_diff>
--- a/Excalidraw/switch.xlsx
+++ b/Excalidraw/switch.xlsx
@@ -9,14 +9,11 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <calcPr/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{D0CA8CA8-9F24-4464-BF8E-62219DCF47F9}"/>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="744">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="745">
   <si>
     <t>DSA</t>
   </si>
@@ -1473,6 +1470,9 @@
   </si>
   <si>
     <t xml:space="preserve">distributed message queue using partitioned, replicated append-only logs with leader-follower replication, pull-based consumers, ISR-backed durability, and transactional guarantees to achieve high throughput, fault tolerance, and exactly-once processing at scale.</t>
+  </si>
+  <si>
+    <t>https://github.com/yashaggarwal85d/Neural-Vault/blob/main/Excalidraw/Design%20a%20Distributed%20Message%20Queue%20(Kafka).md</t>
   </si>
   <si>
     <t xml:space="preserve">Streaming / Log Data</t>
@@ -6799,15 +6799,17 @@
       <c r="F157" s="4"/>
     </row>
     <row r="158" ht="14.25">
-      <c r="A158" t="s">
+      <c r="A158" s="10" t="s">
         <v>481</v>
       </c>
       <c r="B158" s="9" t="s">
         <v>482</v>
       </c>
-      <c r="C158" s="1"/>
+      <c r="C158" s="11" t="s">
+        <v>483</v>
+      </c>
       <c r="D158" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="E158" s="23" t="s">
         <v>66</v>
@@ -6816,12 +6818,12 @@
     </row>
     <row r="159" ht="14.25">
       <c r="A159" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B159" s="9"/>
       <c r="C159" s="1"/>
       <c r="D159" s="2" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="E159" s="23" t="s">
         <v>66</v>
@@ -6830,29 +6832,29 @@
     </row>
     <row r="160" ht="14.25">
       <c r="A160" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B160" s="9"/>
       <c r="C160" s="1"/>
       <c r="D160" s="2" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="E160" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F160" s="4"/>
       <c r="L160" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row r="161" ht="14.25">
       <c r="A161" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B161" s="9"/>
       <c r="C161" s="1"/>
       <c r="D161" s="2" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="E161" s="21" t="s">
         <v>10</v>
@@ -6861,12 +6863,12 @@
     </row>
     <row r="162" ht="14.25">
       <c r="A162" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B162" s="9"/>
       <c r="C162" s="1"/>
       <c r="D162" s="2" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="E162" s="21" t="s">
         <v>10</v>
@@ -6875,12 +6877,12 @@
     </row>
     <row r="163" ht="14.25">
       <c r="A163" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B163" s="9"/>
       <c r="C163" s="1"/>
       <c r="D163" s="2" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="E163" s="23" t="s">
         <v>66</v>
@@ -6889,12 +6891,12 @@
     </row>
     <row r="164" ht="14.25">
       <c r="A164" s="24" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B164" s="9"/>
       <c r="C164" s="1"/>
       <c r="D164" s="2" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="E164" s="21" t="s">
         <v>10</v>
@@ -6903,12 +6905,12 @@
     </row>
     <row r="165" ht="14.25">
       <c r="A165" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B165" s="9"/>
       <c r="C165" s="1"/>
       <c r="D165" s="2" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="E165" s="21" t="s">
         <v>10</v>
@@ -6917,12 +6919,12 @@
     </row>
     <row r="166" ht="14.25">
       <c r="A166" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B166" s="9"/>
       <c r="C166" s="1"/>
       <c r="D166" s="2" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="E166" s="21" t="s">
         <v>10</v>
@@ -6931,12 +6933,12 @@
     </row>
     <row r="167" ht="14.25">
       <c r="A167" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="B167" s="9"/>
       <c r="C167" s="1"/>
       <c r="D167" s="2" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="E167" s="23" t="s">
         <v>66</v>
@@ -6945,12 +6947,12 @@
     </row>
     <row r="168" ht="14.25">
       <c r="A168" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B168" s="9"/>
       <c r="C168" s="1"/>
       <c r="D168" s="2" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="E168" s="23" t="s">
         <v>66</v>
@@ -6959,12 +6961,12 @@
     </row>
     <row r="169" ht="14.25">
       <c r="A169" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="B169" s="9"/>
       <c r="C169" s="1"/>
       <c r="D169" s="2" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="E169" s="23" t="s">
         <v>66</v>
@@ -6973,12 +6975,12 @@
     </row>
     <row r="170" ht="14.25">
       <c r="A170" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="B170" s="9"/>
       <c r="C170" s="1"/>
       <c r="D170" s="2" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="E170" s="23" t="s">
         <v>66</v>
@@ -6987,12 +6989,12 @@
     </row>
     <row r="171" ht="14.25">
       <c r="A171" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B171" s="9"/>
       <c r="C171" s="1"/>
       <c r="D171" s="2" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="E171" s="23" t="s">
         <v>66</v>
@@ -7001,12 +7003,12 @@
     </row>
     <row r="172" ht="14.25">
       <c r="A172" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B172" s="9"/>
       <c r="C172" s="1"/>
       <c r="D172" s="2" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="E172" s="21" t="s">
         <v>10</v>
@@ -7015,12 +7017,12 @@
     </row>
     <row r="173" ht="14.25">
       <c r="A173" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B173" s="9"/>
       <c r="C173" s="1"/>
       <c r="D173" s="2" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="E173" s="21" t="s">
         <v>10</v>
@@ -7029,12 +7031,12 @@
     </row>
     <row r="174" ht="14.25">
       <c r="A174" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B174" s="9"/>
       <c r="C174" s="1"/>
       <c r="D174" s="2" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="E174" s="21" t="s">
         <v>10</v>
@@ -7043,12 +7045,12 @@
     </row>
     <row r="175" ht="14.25">
       <c r="A175" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B175" s="9"/>
       <c r="C175" s="1"/>
       <c r="D175" s="2" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="E175" s="23" t="s">
         <v>66</v>
@@ -7057,12 +7059,12 @@
     </row>
     <row r="176" ht="14.25">
       <c r="A176" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="B176" s="9"/>
       <c r="C176" s="1"/>
       <c r="D176" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="E176" s="23" t="s">
         <v>66</v>
@@ -7071,12 +7073,12 @@
     </row>
     <row r="177" ht="14.25">
       <c r="A177" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B177" s="9"/>
       <c r="C177" s="1"/>
       <c r="D177" s="2" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="E177" s="23" t="s">
         <v>66</v>
@@ -7085,12 +7087,12 @@
     </row>
     <row r="178" ht="14.25">
       <c r="A178" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B178" s="9"/>
       <c r="C178" s="1"/>
       <c r="D178" s="2" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="E178" s="21" t="s">
         <v>10</v>
@@ -7099,12 +7101,12 @@
     </row>
     <row r="179" ht="14.25">
       <c r="A179" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="B179" s="9"/>
       <c r="C179" s="1"/>
       <c r="D179" s="2" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="E179" s="23" t="s">
         <v>66</v>
@@ -7113,12 +7115,12 @@
     </row>
     <row r="180" ht="14.25">
       <c r="A180" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B180" s="9"/>
       <c r="C180" s="1"/>
       <c r="D180" s="2" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="E180" s="21" t="s">
         <v>10</v>
@@ -7127,12 +7129,12 @@
     </row>
     <row r="181" ht="14.25">
       <c r="A181" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B181" s="9"/>
       <c r="C181" s="1"/>
       <c r="D181" s="2" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="E181" s="23" t="s">
         <v>66</v>
@@ -7141,12 +7143,12 @@
     </row>
     <row r="182" ht="14.25">
       <c r="A182" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="B182" s="9"/>
       <c r="C182" s="1"/>
       <c r="D182" s="2" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="E182" s="21" t="s">
         <v>10</v>
@@ -7155,12 +7157,12 @@
     </row>
     <row r="183" ht="14.25">
       <c r="A183" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="B183" s="9"/>
       <c r="C183" s="1"/>
       <c r="D183" s="2" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="E183" s="21" t="s">
         <v>10</v>
@@ -7169,12 +7171,12 @@
     </row>
     <row r="184" ht="14.25">
       <c r="A184" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="B184" s="9"/>
       <c r="C184" s="1"/>
       <c r="D184" s="2" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="E184" s="23" t="s">
         <v>66</v>
@@ -7183,12 +7185,12 @@
     </row>
     <row r="185" ht="14.25">
       <c r="A185" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="B185" s="9"/>
       <c r="C185" s="1"/>
       <c r="D185" s="2" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="E185" s="23" t="s">
         <v>66</v>
@@ -7197,12 +7199,12 @@
     </row>
     <row r="186" ht="14.25">
       <c r="A186" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="B186" s="9"/>
       <c r="C186" s="1"/>
       <c r="D186" s="2" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="E186" s="23" t="s">
         <v>66</v>
@@ -7211,12 +7213,12 @@
     </row>
     <row r="187" ht="14.25">
       <c r="A187" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="B187" s="9"/>
       <c r="C187" s="1"/>
       <c r="D187" s="2" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="E187" s="23" t="s">
         <v>66</v>
@@ -7225,12 +7227,12 @@
     </row>
     <row r="188" ht="14.25">
       <c r="A188" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="B188" s="9"/>
       <c r="C188" s="1"/>
       <c r="D188" s="2" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="E188" s="21" t="s">
         <v>10</v>
@@ -7239,12 +7241,12 @@
     </row>
     <row r="189" ht="14.25">
       <c r="A189" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B189" s="9"/>
       <c r="C189" s="1"/>
       <c r="D189" s="2" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="E189" s="23" t="s">
         <v>66</v>
@@ -7253,12 +7255,12 @@
     </row>
     <row r="190" ht="14.25">
       <c r="A190" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="B190" s="9"/>
       <c r="C190" s="1"/>
       <c r="D190" s="2" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="E190" s="21" t="s">
         <v>10</v>
@@ -7267,12 +7269,12 @@
     </row>
     <row r="191" ht="14.25">
       <c r="A191" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="B191" s="9"/>
       <c r="C191" s="1"/>
       <c r="D191" s="2" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E191" s="23" t="s">
         <v>66</v>
@@ -7281,12 +7283,12 @@
     </row>
     <row r="192" ht="14.25">
       <c r="A192" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="B192" s="9"/>
       <c r="C192" s="1"/>
       <c r="D192" s="2" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="E192" s="18" t="s">
         <v>66</v>
@@ -7309,7 +7311,7 @@
     </row>
     <row r="195" ht="14.25">
       <c r="A195" s="5" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="B195" s="5"/>
       <c r="C195" s="5"/>
@@ -7319,619 +7321,619 @@
     </row>
     <row r="196" ht="14.25">
       <c r="A196" s="4" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="B196" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C196" s="4" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="D196" s="4" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="E196" s="4"/>
       <c r="F196" s="4"/>
     </row>
     <row r="197" ht="14.25">
       <c r="A197" s="20" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="B197" s="9"/>
       <c r="C197" s="1" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="F197" s="4"/>
     </row>
     <row r="198" ht="14.25">
       <c r="A198" s="20" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="B198" s="9"/>
       <c r="C198" s="1" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="F198" s="4"/>
       <c r="H198" s="6"/>
     </row>
     <row r="199" ht="14.25">
       <c r="A199" s="20" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="B199" s="9"/>
       <c r="C199" s="1" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="D199" s="2" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="F199" s="4"/>
     </row>
     <row r="200" ht="14.25">
       <c r="A200" s="20" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="B200" s="9"/>
       <c r="C200" s="1" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="F200" s="4"/>
     </row>
     <row r="201" ht="14.25">
       <c r="A201" s="20" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="B201" s="9"/>
       <c r="C201" s="1" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="F201" s="4"/>
     </row>
     <row r="202" ht="14.25">
       <c r="A202" s="20" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="B202" s="9"/>
       <c r="C202" s="1" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="F202" s="4"/>
     </row>
     <row r="203" ht="14.25">
       <c r="A203" s="20" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B203" s="9"/>
       <c r="C203" s="1" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="D203" s="2" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="F203" s="4"/>
       <c r="H203" s="6"/>
     </row>
     <row r="204" ht="14.25">
       <c r="A204" s="20" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="B204" s="9"/>
       <c r="C204" s="1" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="F204" s="4"/>
       <c r="H204" s="6"/>
     </row>
     <row r="205" ht="14.25">
       <c r="A205" s="20" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="B205" s="9"/>
       <c r="C205" s="1" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="D205" s="2" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="F205" s="4"/>
       <c r="H205" s="6"/>
     </row>
     <row r="206" ht="14.25">
       <c r="A206" s="20" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="B206" s="9"/>
       <c r="C206" s="1" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="D206" s="2" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="F206" s="4"/>
       <c r="H206" s="6"/>
     </row>
     <row r="207" ht="14.25">
       <c r="A207" s="20" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="B207" s="9"/>
       <c r="C207" s="1" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D207" s="2" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="F207" s="4"/>
       <c r="H207" s="6"/>
     </row>
     <row r="208" ht="14.25">
       <c r="A208" s="20" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="B208" s="9"/>
       <c r="C208" s="1" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="D208" s="2" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="F208" s="4"/>
       <c r="H208" s="6"/>
     </row>
     <row r="209" ht="14.25">
       <c r="A209" s="20" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="B209" s="9"/>
       <c r="C209" s="1" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="F209" s="4"/>
       <c r="H209" s="6"/>
     </row>
     <row r="210" ht="14.25">
       <c r="A210" s="20" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="B210" s="9"/>
       <c r="C210" s="1" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="F210" s="4"/>
     </row>
     <row r="211" ht="14.25">
       <c r="A211" s="20" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="B211" s="9"/>
       <c r="C211" s="1" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="D211" s="2" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="F211" s="4"/>
     </row>
     <row r="212" ht="14.25">
       <c r="A212" s="20" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="B212" s="9"/>
       <c r="C212" s="1" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="D212" s="2" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="F212" s="4"/>
     </row>
     <row r="213" ht="14.25">
       <c r="A213" s="20" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="B213" s="9"/>
       <c r="C213" s="1" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="D213" s="2" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="F213" s="4"/>
     </row>
     <row r="214" ht="14.25">
       <c r="A214" s="20" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="B214" s="9"/>
       <c r="C214" s="1" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="D214" s="2" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="F214" s="4"/>
     </row>
     <row r="215" ht="14.25">
       <c r="A215" s="20" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="B215" s="9"/>
       <c r="C215" s="1" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="F215" s="4"/>
     </row>
     <row r="216" ht="14.25">
       <c r="A216" s="20" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="B216" s="9"/>
       <c r="C216" s="1" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="D216" s="2" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="F216" s="4"/>
     </row>
     <row r="217" ht="14.25">
       <c r="A217" s="20" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="B217" s="9"/>
       <c r="C217" s="1" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="F217" s="4"/>
     </row>
     <row r="218" ht="14.25">
       <c r="A218" s="20" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B218" s="9"/>
       <c r="C218" s="1" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="F218" s="4"/>
     </row>
     <row r="219" ht="14.25">
       <c r="A219" s="20" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="B219" s="9"/>
       <c r="C219" s="1" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="F219" s="4"/>
     </row>
     <row r="220" ht="14.25">
       <c r="A220" s="20" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="B220" s="9"/>
       <c r="C220" s="1" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="D220" s="2" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="F220" s="4"/>
     </row>
     <row r="221" ht="14.25">
       <c r="A221" s="20" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="B221" s="9"/>
       <c r="C221" s="1" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="D221" s="2" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="F221" s="4"/>
     </row>
     <row r="222" ht="14.25">
       <c r="A222" s="20" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="B222" s="9"/>
       <c r="C222" s="1" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="D222" s="2" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="F222" s="4"/>
     </row>
     <row r="223" ht="14.25">
       <c r="A223" s="20" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="B223" s="9"/>
       <c r="C223" s="1" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="D223" s="2" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="F223" s="4"/>
     </row>
     <row r="224" ht="14.25">
       <c r="A224" s="20" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="B224" s="9"/>
       <c r="C224" s="1" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="D224" s="2" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="F224" s="4"/>
     </row>
     <row r="225" ht="14.25">
       <c r="A225" s="20" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="B225" s="9"/>
       <c r="C225" s="1" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="D225" s="2" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="F225" s="4"/>
     </row>
     <row r="226" ht="14.25">
       <c r="A226" s="20" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="B226" s="9"/>
       <c r="C226" s="1" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="D226" s="2" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="F226" s="4"/>
     </row>
     <row r="227" ht="14.25">
       <c r="A227" s="20" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="B227" s="9"/>
       <c r="C227" s="1" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="D227" s="2" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="F227" s="4"/>
     </row>
     <row r="228" ht="14.25">
       <c r="A228" s="20" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="B228" s="9"/>
       <c r="C228" s="1" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="D228" s="2" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="F228" s="4"/>
     </row>
     <row r="229" ht="14.25">
       <c r="A229" s="20" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="B229" s="9"/>
       <c r="C229" s="1" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="D229" s="2" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="F229" s="4"/>
     </row>
     <row r="230" ht="14.25">
       <c r="A230" s="20" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="B230" s="9"/>
       <c r="C230" s="1" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="D230" s="2" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="F230" s="4"/>
     </row>
     <row r="231" ht="14.25">
       <c r="A231" s="20" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="B231" s="9"/>
       <c r="C231" s="1" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="D231" s="2" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="F231" s="4"/>
     </row>
     <row r="232" ht="14.25">
       <c r="A232" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="B232" s="9"/>
       <c r="C232" s="1" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="D232" s="2" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="F232" s="4"/>
       <c r="H232" s="6"/>
     </row>
     <row r="233" ht="14.25">
       <c r="A233" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="B233" s="9"/>
       <c r="C233" s="1" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="D233" s="2" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="F233" s="4"/>
       <c r="H233" s="6"/>
     </row>
     <row r="234" ht="14.25">
       <c r="A234" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="B234" s="9"/>
       <c r="C234" s="1" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="D234" s="2" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="F234" s="4"/>
       <c r="H234" s="6"/>
     </row>
     <row r="235" ht="14.25">
       <c r="A235" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="B235" s="9"/>
       <c r="C235" s="1" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="D235" s="2" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="F235" s="4"/>
       <c r="H235" s="6"/>
     </row>
     <row r="236" ht="14.25">
       <c r="A236" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="B236" s="9"/>
       <c r="C236" s="1" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="D236" s="2" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="F236" s="4"/>
       <c r="H236" s="6"/>
     </row>
     <row r="237" ht="14.25">
       <c r="A237" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="B237" s="9"/>
       <c r="C237" s="1" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="D237" s="2" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="F237" s="4"/>
       <c r="H237" s="6"/>
     </row>
     <row r="238" ht="14.25">
       <c r="A238" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="B238" s="9"/>
       <c r="C238" s="1" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="D238" s="2" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="F238" s="4"/>
       <c r="H238" s="6"/>
     </row>
     <row r="239" ht="14.25">
       <c r="A239" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="B239" s="9"/>
       <c r="C239" s="1" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="D239" s="2" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="F239" s="4"/>
       <c r="H239" s="6"/>
     </row>
     <row r="240" ht="14.25">
       <c r="A240" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="B240" s="9"/>
       <c r="C240" s="1" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="D240" s="2" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="F240" s="4"/>
       <c r="H240" s="6"/>
     </row>
     <row r="241" ht="14.25">
       <c r="A241" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="B241" s="9"/>
       <c r="C241" s="1" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="D241" s="2" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="E241" s="3"/>
       <c r="F241" s="4"/>
@@ -7939,14 +7941,14 @@
     </row>
     <row r="242" ht="14.25">
       <c r="A242" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="B242" s="9"/>
       <c r="C242" s="1" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="D242" s="2" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="E242" s="3"/>
       <c r="F242" s="4"/>
@@ -7954,14 +7956,14 @@
     </row>
     <row r="243" ht="14.25">
       <c r="A243" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="B243" s="9"/>
       <c r="C243" s="1" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="D243" s="2" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="E243" s="3"/>
       <c r="F243" s="4"/>
@@ -7969,14 +7971,14 @@
     </row>
     <row r="244" ht="14.25">
       <c r="A244" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="B244" s="9"/>
       <c r="C244" s="1" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="D244" s="2" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="E244" s="3"/>
       <c r="F244" s="4"/>
@@ -7984,14 +7986,14 @@
     </row>
     <row r="245" ht="14.25">
       <c r="A245" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="B245" s="9"/>
       <c r="C245" s="1" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="D245" s="2" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="E245" s="3"/>
       <c r="F245" s="4"/>
@@ -7999,14 +8001,14 @@
     </row>
     <row r="246" ht="14.25">
       <c r="A246" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="B246" s="9"/>
       <c r="C246" s="1" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="D246" s="2" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="E246" s="3"/>
       <c r="F246" s="4"/>
@@ -8028,7 +8030,7 @@
     </row>
     <row r="249" ht="14.25">
       <c r="A249" s="5" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="B249" s="5"/>
       <c r="C249" s="5"/>
@@ -8056,12 +8058,12 @@
     </row>
     <row r="251" ht="14.25">
       <c r="A251" s="20" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="B251" s="9"/>
       <c r="C251" s="1"/>
       <c r="D251" s="25" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="E251" s="16" t="s">
         <v>10</v>
@@ -8070,12 +8072,12 @@
     </row>
     <row r="252" ht="14.25">
       <c r="A252" s="20" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="B252" s="9"/>
       <c r="C252" s="1"/>
       <c r="D252" s="25" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="E252" s="21" t="s">
         <v>10</v>
@@ -8084,12 +8086,12 @@
     </row>
     <row r="253" ht="14.25">
       <c r="A253" s="20" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="B253" s="9"/>
       <c r="C253" s="1"/>
       <c r="D253" s="25" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="E253" s="21" t="s">
         <v>10</v>
@@ -8098,12 +8100,12 @@
     </row>
     <row r="254" ht="14.25">
       <c r="A254" s="20" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="B254" s="9"/>
       <c r="C254" s="1"/>
       <c r="D254" s="25" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="E254" s="21" t="s">
         <v>10</v>
@@ -8112,12 +8114,12 @@
     </row>
     <row r="255" ht="14.25">
       <c r="A255" s="20" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="B255" s="9"/>
       <c r="C255" s="1"/>
       <c r="D255" s="25" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="E255" s="21" t="s">
         <v>10</v>
@@ -8126,12 +8128,12 @@
     </row>
     <row r="256" ht="14.25">
       <c r="A256" s="20" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="B256" s="9"/>
       <c r="C256" s="1"/>
       <c r="D256" s="25" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="E256" s="21" t="s">
         <v>10</v>
@@ -8140,12 +8142,12 @@
     </row>
     <row r="257" ht="14.25">
       <c r="A257" s="20" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="B257" s="9"/>
       <c r="C257" s="1"/>
       <c r="D257" s="25" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="E257" s="21" t="s">
         <v>10</v>
@@ -8154,12 +8156,12 @@
     </row>
     <row r="258" ht="14.25">
       <c r="A258" s="20" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="B258" s="9"/>
       <c r="C258" s="1"/>
       <c r="D258" s="25" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="E258" s="21" t="s">
         <v>10</v>
@@ -8168,12 +8170,12 @@
     </row>
     <row r="259" ht="14.25">
       <c r="A259" s="20" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="B259" s="9"/>
       <c r="C259" s="1"/>
       <c r="D259" s="25" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="E259" s="21" t="s">
         <v>10</v>
@@ -8182,12 +8184,12 @@
     </row>
     <row r="260" ht="14.25">
       <c r="A260" s="20" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="B260" s="9"/>
       <c r="C260" s="1"/>
       <c r="D260" s="25" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="E260" s="23" t="s">
         <v>66</v>
@@ -8196,12 +8198,12 @@
     </row>
     <row r="261" ht="14.25">
       <c r="A261" s="20" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="B261" s="9"/>
       <c r="C261" s="1"/>
       <c r="D261" s="25" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="E261" s="21" t="s">
         <v>10</v>
@@ -8210,12 +8212,12 @@
     </row>
     <row r="262" ht="14.25">
       <c r="A262" s="20" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="B262" s="9"/>
       <c r="C262" s="1"/>
       <c r="D262" s="25" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="E262" s="23" t="s">
         <v>66</v>
@@ -8224,12 +8226,12 @@
     </row>
     <row r="263" ht="14.25">
       <c r="A263" s="20" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="B263" s="9"/>
       <c r="C263" s="1"/>
       <c r="D263" s="25" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="E263" s="21" t="s">
         <v>10</v>
@@ -8243,7 +8245,7 @@
       <c r="B264" s="9"/>
       <c r="C264" s="1"/>
       <c r="D264" s="25" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="E264" s="23" t="s">
         <v>66</v>
@@ -8257,7 +8259,7 @@
       <c r="B265" s="9"/>
       <c r="C265" s="1"/>
       <c r="D265" s="25" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="E265" s="21" t="s">
         <v>10</v>
@@ -8266,12 +8268,12 @@
     </row>
     <row r="266" ht="14.25">
       <c r="A266" s="20" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="B266" s="9"/>
       <c r="C266" s="1"/>
       <c r="D266" s="25" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="E266" s="23" t="s">
         <v>66</v>
@@ -8280,12 +8282,12 @@
     </row>
     <row r="267" ht="14.25">
       <c r="A267" s="20" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="B267" s="9"/>
       <c r="C267" s="1"/>
       <c r="D267" s="25" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="E267" s="21" t="s">
         <v>10</v>
@@ -8294,12 +8296,12 @@
     </row>
     <row r="268" ht="14.25">
       <c r="A268" s="20" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B268" s="9"/>
       <c r="C268" s="1"/>
       <c r="D268" s="25" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="E268" s="21" t="s">
         <v>10</v>
@@ -8308,12 +8310,12 @@
     </row>
     <row r="269" ht="14.25">
       <c r="A269" s="20" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="B269" s="9"/>
       <c r="C269" s="1"/>
       <c r="D269" s="25" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="E269" s="23" t="s">
         <v>66</v>
@@ -8322,12 +8324,12 @@
     </row>
     <row r="270" ht="14.25">
       <c r="A270" s="20" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="B270" s="9"/>
       <c r="C270" s="1"/>
       <c r="D270" s="25" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="E270" s="21" t="s">
         <v>10</v>
@@ -8336,12 +8338,12 @@
     </row>
     <row r="271" ht="14.25">
       <c r="A271" s="20" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="B271" s="9"/>
       <c r="C271" s="1"/>
       <c r="D271" s="25" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="E271" s="21" t="s">
         <v>10</v>
@@ -8350,12 +8352,12 @@
     </row>
     <row r="272" ht="14.25">
       <c r="A272" s="20" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="B272" s="9"/>
       <c r="C272" s="1"/>
       <c r="D272" s="25" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="E272" s="21" t="s">
         <v>10</v>
@@ -8364,12 +8366,12 @@
     </row>
     <row r="273" ht="14.25">
       <c r="A273" s="20" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="B273" s="9"/>
       <c r="C273" s="1"/>
       <c r="D273" s="25" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="E273" s="23" t="s">
         <v>66</v>
@@ -8378,12 +8380,12 @@
     </row>
     <row r="274" ht="14.25">
       <c r="A274" s="20" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B274" s="9"/>
       <c r="C274" s="1"/>
       <c r="D274" s="25" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="E274" s="21" t="s">
         <v>10</v>
@@ -8392,12 +8394,12 @@
     </row>
     <row r="275" ht="14.25">
       <c r="A275" s="20" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="B275" s="9"/>
       <c r="C275" s="1"/>
       <c r="D275" s="25" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="E275" s="23" t="s">
         <v>66</v>
@@ -8406,12 +8408,12 @@
     </row>
     <row r="276" ht="14.25">
       <c r="A276" s="20" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="B276" s="9"/>
       <c r="C276" s="1"/>
       <c r="D276" s="25" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="E276" s="21" t="s">
         <v>10</v>
@@ -8420,12 +8422,12 @@
     </row>
     <row r="277" ht="14.25">
       <c r="A277" s="20" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="B277" s="9"/>
       <c r="C277" s="1"/>
       <c r="D277" s="25" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="E277" s="21" t="s">
         <v>10</v>
@@ -8434,12 +8436,12 @@
     </row>
     <row r="278" ht="14.25">
       <c r="A278" s="20" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="B278" s="9"/>
       <c r="C278" s="1"/>
       <c r="D278" s="25" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="E278" s="23" t="s">
         <v>66</v>
@@ -8448,12 +8450,12 @@
     </row>
     <row r="279" ht="14.25">
       <c r="A279" s="20" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="B279" s="9"/>
       <c r="C279" s="1"/>
       <c r="D279" s="25" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="E279" s="23" t="s">
         <v>66</v>
@@ -8462,12 +8464,12 @@
     </row>
     <row r="280" ht="14.25">
       <c r="A280" s="20" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="B280" s="9"/>
       <c r="C280" s="1"/>
       <c r="D280" s="25" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="E280" s="21" t="s">
         <v>10</v>
@@ -8476,12 +8478,12 @@
     </row>
     <row r="281" ht="14.25">
       <c r="A281" s="20" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="B281" s="9"/>
       <c r="C281" s="1"/>
       <c r="D281" s="25" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="E281" s="23" t="s">
         <v>66</v>
@@ -8490,12 +8492,12 @@
     </row>
     <row r="282" ht="14.25">
       <c r="A282" s="20" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="B282" s="9"/>
       <c r="C282" s="1"/>
       <c r="D282" s="25" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="E282" s="21" t="s">
         <v>10</v>
@@ -8504,12 +8506,12 @@
     </row>
     <row r="283" ht="14.25">
       <c r="A283" s="20" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="B283" s="9"/>
       <c r="C283" s="1"/>
       <c r="D283" s="25" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="E283" s="21" t="s">
         <v>10</v>
@@ -8518,12 +8520,12 @@
     </row>
     <row r="284" ht="14.25">
       <c r="A284" s="20" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="B284" s="9"/>
       <c r="C284" s="1"/>
       <c r="D284" s="25" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="E284" s="21" t="s">
         <v>10</v>
@@ -8532,12 +8534,12 @@
     </row>
     <row r="285" ht="14.25">
       <c r="A285" s="20" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B285" s="9"/>
       <c r="C285" s="1"/>
       <c r="D285" s="25" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="E285" s="21" t="s">
         <v>10</v>
@@ -8546,12 +8548,12 @@
     </row>
     <row r="286" ht="14.25">
       <c r="A286" s="20" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="B286" s="9"/>
       <c r="C286" s="1"/>
       <c r="D286" s="25" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="E286" s="23" t="s">
         <v>66</v>
@@ -8560,12 +8562,12 @@
     </row>
     <row r="287" ht="14.25">
       <c r="A287" s="20" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="B287" s="9"/>
       <c r="C287" s="1"/>
       <c r="D287" s="25" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="E287" s="21" t="s">
         <v>10</v>
@@ -8574,12 +8576,12 @@
     </row>
     <row r="288" ht="14.25">
       <c r="A288" s="20" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="B288" s="9"/>
       <c r="C288" s="1"/>
       <c r="D288" s="25" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="E288" s="21" t="s">
         <v>10</v>
@@ -8588,12 +8590,12 @@
     </row>
     <row r="289" ht="14.25">
       <c r="A289" s="20" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="B289" s="9"/>
       <c r="C289" s="1"/>
       <c r="D289" s="25" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="E289" s="21" t="s">
         <v>10</v>
@@ -8602,12 +8604,12 @@
     </row>
     <row r="290" ht="14.25">
       <c r="A290" s="20" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="B290" s="9"/>
       <c r="C290" s="1"/>
       <c r="D290" s="25" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="E290" s="23" t="s">
         <v>66</v>
@@ -8616,12 +8618,12 @@
     </row>
     <row r="291" ht="14.25">
       <c r="A291" s="20" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="B291" s="9"/>
       <c r="C291" s="1"/>
       <c r="D291" s="25" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="E291" s="16" t="s">
         <v>10</v>
@@ -9008,6 +9010,7 @@
     <hyperlink r:id="rId124" ref="C155"/>
     <hyperlink r:id="rId125" ref="C156"/>
     <hyperlink r:id="rId126" ref="C157"/>
+    <hyperlink r:id="rId127" ref="C158"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
vault backup: 2026-01-14 18:39:26
</commit_message>
<xml_diff>
--- a/Excalidraw/switch.xlsx
+++ b/Excalidraw/switch.xlsx
@@ -9,11 +9,14 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <calcPr/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{D0CA8CA8-9F24-4464-BF8E-62219DCF47F9}"/>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="745">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="751">
   <si>
     <t>DSA</t>
   </si>
@@ -1300,6 +1303,15 @@
   </si>
   <si>
     <t xml:space="preserve">Backtracking + Bitmask DP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Separate squares 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Binary search on answer, stopping based on the range given</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/separate-squares-i</t>
   </si>
   <si>
     <t xml:space="preserve">HLD concepts</t>
@@ -1481,10 +1493,19 @@
     <t xml:space="preserve">Design a Distributed File System (S3/HDFS)</t>
   </si>
   <si>
+    <t xml:space="preserve">Just like Key-value store (DynamoDB)</t>
+  </si>
+  <si>
+    <t>https://github.com/yashaggarwal85d/Neural-Vault/blob/main/Excalidraw/Design%20a%20Distributed%20File%20System%20(S3).md</t>
+  </si>
+  <si>
     <t xml:space="preserve">Storage / Blob</t>
   </si>
   <si>
     <t xml:space="preserve">Design Google Drive / Dropbox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">globally distributed, strongly consistent metadata system with eventually consistent blob storage, optimized for large-scale file sync, durability, and low-latency access.</t>
   </si>
   <si>
     <t xml:space="preserve">File Sync / Versioning</t>
@@ -2459,7 +2480,7 @@
     <xf fontId="6" fillId="12" borderId="2" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="3" fillId="13" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="3" fillId="8" borderId="0" numFmtId="0" xfId="7" applyFont="1" applyFill="1"/>
     <xf fontId="3" fillId="7" borderId="0" numFmtId="0" xfId="6" applyFont="1" applyFill="1"/>
@@ -2492,6 +2513,9 @@
     </xf>
     <xf fontId="3" fillId="4" borderId="3" numFmtId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf fontId="7" fillId="8" borderId="0" numFmtId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="1" fillId="2" borderId="1" numFmtId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2995,7 +3019,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A141" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A138" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -6300,356 +6324,444 @@
       <c r="CO132"/>
       <c r="CP132"/>
     </row>
-    <row r="133" s="4" customFormat="1" ht="14.25">
-      <c r="A133" s="4"/>
-      <c r="B133" s="4"/>
-      <c r="C133" s="4"/>
-      <c r="D133" s="4"/>
-      <c r="E133" s="4"/>
+    <row r="133" s="0" customFormat="1" ht="14.25">
+      <c r="A133" s="17" t="s">
+        <v>429</v>
+      </c>
+      <c r="B133" s="9" t="s">
+        <v>430</v>
+      </c>
+      <c r="C133" s="19" t="s">
+        <v>431</v>
+      </c>
+      <c r="D133" s="15" t="s">
+        <v>416</v>
+      </c>
+      <c r="E133" s="16" t="s">
+        <v>10</v>
+      </c>
       <c r="F133" s="4"/>
-      <c r="G133"/>
-      <c r="H133"/>
-      <c r="I133"/>
-      <c r="J133" s="6"/>
-      <c r="K133"/>
-      <c r="L133"/>
-      <c r="M133"/>
-      <c r="N133"/>
-      <c r="O133"/>
-      <c r="P133"/>
-      <c r="Q133"/>
-      <c r="R133"/>
-      <c r="S133"/>
-      <c r="T133"/>
-      <c r="U133"/>
-      <c r="V133"/>
-      <c r="W133"/>
-      <c r="X133"/>
-      <c r="Y133"/>
-      <c r="Z133"/>
-      <c r="AA133"/>
-      <c r="AB133"/>
-      <c r="AC133"/>
-      <c r="AD133"/>
-      <c r="AE133"/>
-      <c r="AF133"/>
-      <c r="AG133"/>
-      <c r="AH133"/>
-      <c r="AI133"/>
-      <c r="AJ133"/>
-      <c r="AK133"/>
-      <c r="AL133"/>
-      <c r="AM133"/>
-      <c r="AN133"/>
-      <c r="AO133"/>
-      <c r="AP133"/>
-      <c r="AQ133"/>
-      <c r="AR133" s="4"/>
-      <c r="AS133" s="4"/>
-      <c r="AT133" s="4"/>
-      <c r="AU133" s="4"/>
-      <c r="AV133" s="4"/>
-      <c r="AW133" s="4"/>
-      <c r="AX133" s="4"/>
-      <c r="AY133" s="4"/>
-      <c r="AZ133" s="4"/>
-      <c r="BA133" s="4"/>
-      <c r="BB133" s="4"/>
-      <c r="BC133" s="4"/>
-      <c r="BD133" s="4"/>
-      <c r="BE133" s="4"/>
-      <c r="BF133" s="4"/>
-      <c r="BG133" s="4"/>
-      <c r="BH133" s="4"/>
-      <c r="BI133" s="4"/>
-      <c r="BJ133" s="4"/>
-      <c r="BK133" s="4"/>
-      <c r="BL133" s="4"/>
-      <c r="BM133" s="4"/>
-      <c r="BN133" s="4"/>
-      <c r="BO133" s="4"/>
-      <c r="BP133" s="4"/>
-      <c r="BQ133" s="4"/>
-      <c r="BR133" s="4"/>
-      <c r="BS133" s="4"/>
-      <c r="BT133" s="4"/>
-      <c r="BU133" s="4"/>
-      <c r="BV133" s="4"/>
-      <c r="BW133" s="4"/>
-      <c r="BX133" s="4"/>
-      <c r="BY133" s="4"/>
-      <c r="BZ133" s="4"/>
-      <c r="CA133" s="4"/>
-      <c r="CB133" s="4"/>
-      <c r="CC133" s="4"/>
-      <c r="CD133" s="4"/>
-      <c r="CE133" s="4"/>
-      <c r="CF133" s="4"/>
-      <c r="CG133" s="4"/>
-      <c r="CH133" s="4"/>
-      <c r="CI133" s="4"/>
-      <c r="CJ133" s="4"/>
-      <c r="CK133" s="4"/>
-      <c r="CL133" s="4"/>
-      <c r="CM133" s="4"/>
-      <c r="CN133" s="4"/>
-      <c r="CO133" s="4"/>
-      <c r="CP133" s="4"/>
-    </row>
-    <row r="134" ht="14.25">
-      <c r="C134"/>
-      <c r="D134"/>
-      <c r="E134"/>
-      <c r="F134"/>
+      <c r="G133" s="6"/>
+      <c r="H133" s="6"/>
+      <c r="I133" s="6"/>
+      <c r="J133"/>
+      <c r="K133" s="6"/>
+      <c r="L133" s="6"/>
+      <c r="M133" s="6"/>
+      <c r="N133" s="6"/>
+      <c r="O133" s="6"/>
+      <c r="P133" s="6"/>
+      <c r="Q133" s="6"/>
+      <c r="R133" s="6"/>
+      <c r="S133" s="6"/>
+      <c r="T133" s="6"/>
+      <c r="U133" s="6"/>
+      <c r="V133" s="6"/>
+      <c r="W133" s="6"/>
+      <c r="X133" s="6"/>
+      <c r="Y133" s="6"/>
+      <c r="Z133" s="6"/>
+      <c r="AA133" s="6"/>
+      <c r="AB133" s="6"/>
+      <c r="AC133" s="6"/>
+      <c r="AD133" s="6"/>
+      <c r="AE133" s="6"/>
+      <c r="AF133" s="6"/>
+      <c r="AG133" s="6"/>
+      <c r="AH133" s="6"/>
+      <c r="AI133" s="6"/>
+      <c r="AJ133" s="6"/>
+      <c r="AK133" s="6"/>
+      <c r="AL133" s="6"/>
+      <c r="AM133" s="6"/>
+      <c r="AN133" s="6"/>
+      <c r="AO133" s="6"/>
+      <c r="AP133" s="6"/>
+      <c r="AQ133" s="6"/>
+      <c r="AR133" s="6"/>
+      <c r="AS133" s="6"/>
+      <c r="AT133" s="6"/>
+      <c r="AU133" s="6"/>
+      <c r="AV133" s="6"/>
+      <c r="AW133" s="6"/>
+      <c r="AX133" s="6"/>
+      <c r="AY133" s="6"/>
+      <c r="AZ133" s="6"/>
+      <c r="BA133" s="6"/>
+      <c r="BB133" s="6"/>
+      <c r="BC133" s="6"/>
+      <c r="BD133" s="6"/>
+      <c r="BE133" s="6"/>
+      <c r="BF133" s="6"/>
+      <c r="BG133" s="6"/>
+      <c r="BH133" s="6"/>
+      <c r="BI133" s="6"/>
+      <c r="BJ133" s="6"/>
+      <c r="BK133" s="6"/>
+      <c r="BL133" s="6"/>
+      <c r="BM133" s="6"/>
+      <c r="BN133" s="6"/>
+      <c r="BO133" s="6"/>
+      <c r="BP133" s="6"/>
+      <c r="BQ133" s="6"/>
+      <c r="BR133" s="6"/>
+      <c r="BS133" s="6"/>
+      <c r="BT133" s="6"/>
+      <c r="BU133" s="6"/>
+      <c r="BV133" s="6"/>
+      <c r="BW133" s="6"/>
+      <c r="BX133" s="6"/>
+      <c r="BY133" s="6"/>
+      <c r="BZ133" s="6"/>
+      <c r="CA133" s="6"/>
+      <c r="CB133" s="6"/>
+      <c r="CC133" s="6"/>
+      <c r="CD133" s="6"/>
+      <c r="CE133" s="6"/>
+      <c r="CF133" s="6"/>
+      <c r="CG133" s="6"/>
+      <c r="CH133" s="6"/>
+      <c r="CI133" s="6"/>
+      <c r="CJ133" s="6"/>
+      <c r="CK133" s="6"/>
+      <c r="CL133" s="6"/>
+      <c r="CM133" s="6"/>
+      <c r="CN133" s="6"/>
+      <c r="CO133" s="6"/>
+      <c r="CP133" s="6"/>
+    </row>
+    <row r="134" s="4" customFormat="1" ht="14.25">
+      <c r="A134" s="4"/>
+      <c r="B134" s="4"/>
+      <c r="C134" s="4"/>
+      <c r="D134" s="4"/>
+      <c r="E134" s="4"/>
+      <c r="F134" s="4"/>
+      <c r="G134"/>
+      <c r="H134"/>
+      <c r="I134"/>
+      <c r="J134" s="6"/>
+      <c r="K134"/>
+      <c r="L134"/>
+      <c r="M134"/>
+      <c r="N134"/>
+      <c r="O134"/>
+      <c r="P134"/>
+      <c r="Q134"/>
+      <c r="R134"/>
+      <c r="S134"/>
+      <c r="T134"/>
+      <c r="U134"/>
+      <c r="V134"/>
+      <c r="W134"/>
+      <c r="X134"/>
+      <c r="Y134"/>
+      <c r="Z134"/>
+      <c r="AA134"/>
+      <c r="AB134"/>
+      <c r="AC134"/>
+      <c r="AD134"/>
+      <c r="AE134"/>
+      <c r="AF134"/>
+      <c r="AG134"/>
+      <c r="AH134"/>
+      <c r="AI134"/>
+      <c r="AJ134"/>
+      <c r="AK134"/>
+      <c r="AL134"/>
+      <c r="AM134"/>
+      <c r="AN134"/>
+      <c r="AO134"/>
+      <c r="AP134"/>
+      <c r="AQ134"/>
+      <c r="AR134" s="4"/>
+      <c r="AS134" s="4"/>
+      <c r="AT134" s="4"/>
+      <c r="AU134" s="4"/>
+      <c r="AV134" s="4"/>
+      <c r="AW134" s="4"/>
+      <c r="AX134" s="4"/>
+      <c r="AY134" s="4"/>
+      <c r="AZ134" s="4"/>
+      <c r="BA134" s="4"/>
+      <c r="BB134" s="4"/>
+      <c r="BC134" s="4"/>
+      <c r="BD134" s="4"/>
+      <c r="BE134" s="4"/>
+      <c r="BF134" s="4"/>
+      <c r="BG134" s="4"/>
+      <c r="BH134" s="4"/>
+      <c r="BI134" s="4"/>
+      <c r="BJ134" s="4"/>
+      <c r="BK134" s="4"/>
+      <c r="BL134" s="4"/>
+      <c r="BM134" s="4"/>
+      <c r="BN134" s="4"/>
+      <c r="BO134" s="4"/>
+      <c r="BP134" s="4"/>
+      <c r="BQ134" s="4"/>
+      <c r="BR134" s="4"/>
+      <c r="BS134" s="4"/>
+      <c r="BT134" s="4"/>
+      <c r="BU134" s="4"/>
+      <c r="BV134" s="4"/>
+      <c r="BW134" s="4"/>
+      <c r="BX134" s="4"/>
+      <c r="BY134" s="4"/>
+      <c r="BZ134" s="4"/>
+      <c r="CA134" s="4"/>
+      <c r="CB134" s="4"/>
+      <c r="CC134" s="4"/>
+      <c r="CD134" s="4"/>
+      <c r="CE134" s="4"/>
+      <c r="CF134" s="4"/>
+      <c r="CG134" s="4"/>
+      <c r="CH134" s="4"/>
+      <c r="CI134" s="4"/>
+      <c r="CJ134" s="4"/>
+      <c r="CK134" s="4"/>
+      <c r="CL134" s="4"/>
+      <c r="CM134" s="4"/>
+      <c r="CN134" s="4"/>
+      <c r="CO134" s="4"/>
+      <c r="CP134" s="4"/>
     </row>
     <row r="135" ht="14.25">
-      <c r="A135" s="5" t="s">
-        <v>429</v>
-      </c>
-      <c r="B135" s="5"/>
       <c r="C135"/>
       <c r="D135"/>
       <c r="E135"/>
       <c r="F135"/>
     </row>
     <row r="136" ht="14.25">
-      <c r="A136" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B136" s="19" t="s">
-        <v>2</v>
-      </c>
+      <c r="A136" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="B136" s="5"/>
       <c r="C136"/>
       <c r="D136"/>
       <c r="E136"/>
       <c r="F136"/>
-      <c r="G136" s="20"/>
-      <c r="H136" s="20"/>
-      <c r="I136" s="20"/>
-      <c r="K136" s="20"/>
-      <c r="L136" s="20"/>
-      <c r="M136" s="20"/>
-      <c r="N136" s="20"/>
-      <c r="O136" s="20"/>
-      <c r="P136" s="20"/>
-      <c r="Q136" s="20"/>
-      <c r="R136" s="20"/>
-      <c r="S136" s="20"/>
-      <c r="T136" s="20"/>
-      <c r="U136" s="20"/>
-      <c r="V136" s="20"/>
-      <c r="W136" s="20"/>
-      <c r="X136" s="20"/>
-      <c r="Y136" s="20"/>
-      <c r="Z136" s="20"/>
-      <c r="AA136" s="20"/>
-      <c r="AB136" s="20"/>
-      <c r="AC136" s="20"/>
-      <c r="AD136" s="20"/>
-      <c r="AE136" s="20"/>
-      <c r="AF136" s="20"/>
-      <c r="AG136" s="20"/>
-      <c r="AH136" s="20"/>
-      <c r="AI136" s="20"/>
-      <c r="AJ136" s="20"/>
-      <c r="AK136" s="20"/>
-      <c r="AL136" s="20"/>
-      <c r="AM136" s="20"/>
-      <c r="AN136" s="20"/>
-      <c r="AO136" s="20"/>
-      <c r="AP136" s="20"/>
-      <c r="AQ136" s="20"/>
-    </row>
-    <row r="137" ht="42.75">
-      <c r="A137" s="7" t="s">
-        <v>430</v>
-      </c>
-      <c r="B137" s="12" t="s">
-        <v>431</v>
-      </c>
-      <c r="C137" s="6"/>
-      <c r="D137" s="6"/>
-      <c r="E137" s="6"/>
-      <c r="F137" s="6"/>
+    </row>
+    <row r="137" ht="14.25">
+      <c r="A137" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B137" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C137"/>
+      <c r="D137"/>
+      <c r="E137"/>
+      <c r="F137"/>
+      <c r="G137" s="21"/>
+      <c r="H137" s="21"/>
+      <c r="I137" s="21"/>
+      <c r="K137" s="21"/>
+      <c r="L137" s="21"/>
+      <c r="M137" s="21"/>
+      <c r="N137" s="21"/>
+      <c r="O137" s="21"/>
+      <c r="P137" s="21"/>
+      <c r="Q137" s="21"/>
+      <c r="R137" s="21"/>
+      <c r="S137" s="21"/>
+      <c r="T137" s="21"/>
+      <c r="U137" s="21"/>
+      <c r="V137" s="21"/>
+      <c r="W137" s="21"/>
+      <c r="X137" s="21"/>
+      <c r="Y137" s="21"/>
+      <c r="Z137" s="21"/>
+      <c r="AA137" s="21"/>
+      <c r="AB137" s="21"/>
+      <c r="AC137" s="21"/>
+      <c r="AD137" s="21"/>
+      <c r="AE137" s="21"/>
+      <c r="AF137" s="21"/>
+      <c r="AG137" s="21"/>
+      <c r="AH137" s="21"/>
+      <c r="AI137" s="21"/>
+      <c r="AJ137" s="21"/>
+      <c r="AK137" s="21"/>
+      <c r="AL137" s="21"/>
+      <c r="AM137" s="21"/>
+      <c r="AN137" s="21"/>
+      <c r="AO137" s="21"/>
+      <c r="AP137" s="21"/>
+      <c r="AQ137" s="21"/>
     </row>
     <row r="138" ht="42.75">
-      <c r="A138" s="10" t="s">
-        <v>432</v>
+      <c r="A138" s="7" t="s">
+        <v>433</v>
       </c>
       <c r="B138" s="12" t="s">
-        <v>433</v>
-      </c>
-      <c r="C138"/>
-      <c r="D138"/>
-      <c r="E138"/>
-      <c r="F138"/>
-    </row>
-    <row r="139" ht="14.25">
-      <c r="A139" s="7" t="s">
         <v>434</v>
       </c>
-      <c r="B139" s="9" t="s">
+      <c r="C138" s="6"/>
+      <c r="D138" s="6"/>
+      <c r="E138" s="6"/>
+      <c r="F138" s="6"/>
+    </row>
+    <row r="139" ht="42.75">
+      <c r="A139" s="10" t="s">
         <v>435</v>
       </c>
-      <c r="C139" s="6"/>
-      <c r="D139" s="6"/>
-      <c r="E139" s="6"/>
-      <c r="F139" s="6"/>
+      <c r="B139" s="12" t="s">
+        <v>436</v>
+      </c>
+      <c r="C139"/>
+      <c r="D139"/>
+      <c r="E139"/>
+      <c r="F139"/>
     </row>
     <row r="140" ht="14.25">
-      <c r="A140" s="10" t="s">
-        <v>436</v>
+      <c r="A140" s="7" t="s">
+        <v>437</v>
       </c>
       <c r="B140" s="9" t="s">
-        <v>437</v>
-      </c>
-      <c r="C140"/>
-      <c r="D140"/>
-      <c r="E140"/>
-      <c r="F140"/>
-    </row>
-    <row r="141" ht="71.25">
+        <v>438</v>
+      </c>
+      <c r="C140" s="6"/>
+      <c r="D140" s="6"/>
+      <c r="E140" s="6"/>
+      <c r="F140" s="6"/>
+    </row>
+    <row r="141" ht="14.25">
       <c r="A141" s="10" t="s">
-        <v>438</v>
-      </c>
-      <c r="B141" s="12" t="s">
         <v>439</v>
+      </c>
+      <c r="B141" s="9" t="s">
+        <v>440</v>
       </c>
       <c r="C141"/>
       <c r="D141"/>
       <c r="E141"/>
       <c r="F141"/>
     </row>
-    <row r="142" ht="28.5">
-      <c r="A142" s="7" t="s">
-        <v>440</v>
+    <row r="142" ht="71.25">
+      <c r="A142" s="10" t="s">
+        <v>441</v>
       </c>
       <c r="B142" s="12" t="s">
-        <v>441</v>
-      </c>
-      <c r="C142" s="6"/>
-      <c r="D142" s="6"/>
-      <c r="E142" s="6"/>
-      <c r="F142" s="6"/>
-    </row>
-    <row r="143" ht="14.25">
-      <c r="B143" s="9"/>
-      <c r="C143"/>
-      <c r="D143"/>
-      <c r="E143"/>
-      <c r="F143"/>
-    </row>
-    <row r="144" ht="13.5" customHeight="1">
-      <c r="A144" s="4"/>
-      <c r="B144" s="4"/>
-      <c r="C144" s="6"/>
-      <c r="D144" s="6"/>
-      <c r="E144" s="6"/>
-      <c r="F144" s="6"/>
-    </row>
-    <row r="145" ht="14.25">
+        <v>442</v>
+      </c>
+      <c r="C142"/>
+      <c r="D142"/>
+      <c r="E142"/>
+      <c r="F142"/>
+    </row>
+    <row r="143" ht="28.5">
+      <c r="A143" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="B143" s="12" t="s">
+        <v>444</v>
+      </c>
+      <c r="C143" s="6"/>
+      <c r="D143" s="6"/>
+      <c r="E143" s="6"/>
+      <c r="F143" s="6"/>
+    </row>
+    <row r="144" ht="14.25">
+      <c r="B144" s="9"/>
+      <c r="C144"/>
+      <c r="D144"/>
+      <c r="E144"/>
+      <c r="F144"/>
+    </row>
+    <row r="145" ht="13.5" customHeight="1">
+      <c r="A145" s="4"/>
+      <c r="B145" s="4"/>
       <c r="C145" s="6"/>
       <c r="D145" s="6"/>
       <c r="E145" s="6"/>
       <c r="F145" s="6"/>
     </row>
     <row r="146" ht="14.25">
-      <c r="A146" s="5" t="s">
-        <v>442</v>
-      </c>
-      <c r="B146" s="5"/>
-      <c r="C146" s="5"/>
-      <c r="D146" s="5"/>
-      <c r="E146" s="5"/>
-      <c r="F146" s="5"/>
-    </row>
-    <row r="147" s="0" customFormat="1" ht="14.25">
-      <c r="A147" s="19" t="s">
+      <c r="C146" s="6"/>
+      <c r="D146" s="6"/>
+      <c r="E146" s="6"/>
+      <c r="F146" s="6"/>
+    </row>
+    <row r="147" ht="14.25">
+      <c r="A147" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="B147" s="5"/>
+      <c r="C147" s="5"/>
+      <c r="D147" s="5"/>
+      <c r="E147" s="5"/>
+      <c r="F147" s="5"/>
+    </row>
+    <row r="148" s="0" customFormat="1" ht="14.25">
+      <c r="A148" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B147" s="19" t="s">
+      <c r="B148" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C147" s="19" t="s">
-        <v>443</v>
-      </c>
-      <c r="D147" s="19" t="s">
+      <c r="C148" s="20" t="s">
+        <v>446</v>
+      </c>
+      <c r="D148" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E147" s="4" t="s">
+      <c r="E148" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F147" s="4"/>
-      <c r="G147"/>
-      <c r="H147"/>
-      <c r="I147"/>
-      <c r="J147" s="6"/>
-      <c r="K147"/>
-      <c r="L147"/>
-      <c r="M147"/>
-      <c r="N147"/>
-      <c r="O147"/>
-      <c r="P147"/>
-      <c r="Q147"/>
-      <c r="R147"/>
-      <c r="S147"/>
-      <c r="T147"/>
-      <c r="U147"/>
-      <c r="V147"/>
-      <c r="W147"/>
-      <c r="X147"/>
-      <c r="Y147"/>
-      <c r="Z147"/>
-      <c r="AA147"/>
-      <c r="AB147"/>
-      <c r="AC147"/>
-      <c r="AD147"/>
-      <c r="AE147"/>
-      <c r="AF147"/>
-      <c r="AG147"/>
-      <c r="AH147"/>
-      <c r="AI147"/>
-      <c r="AJ147"/>
-      <c r="AK147"/>
-      <c r="AL147"/>
-      <c r="AM147"/>
-      <c r="AN147"/>
-      <c r="AO147"/>
-      <c r="AP147"/>
-      <c r="AQ147"/>
-    </row>
-    <row r="148" ht="14.25">
-      <c r="A148" s="7" t="s">
-        <v>444</v>
-      </c>
-      <c r="B148" s="9" t="s">
-        <v>445</v>
-      </c>
-      <c r="C148" s="11" t="s">
-        <v>446</v>
-      </c>
-      <c r="D148" s="2" t="s">
-        <v>447</v>
-      </c>
-      <c r="E148" s="16" t="s">
-        <v>10</v>
-      </c>
       <c r="F148" s="4"/>
+      <c r="G148"/>
+      <c r="H148"/>
+      <c r="I148"/>
+      <c r="J148" s="6"/>
+      <c r="K148"/>
+      <c r="L148"/>
+      <c r="M148"/>
+      <c r="N148"/>
+      <c r="O148"/>
+      <c r="P148"/>
+      <c r="Q148"/>
+      <c r="R148"/>
+      <c r="S148"/>
+      <c r="T148"/>
+      <c r="U148"/>
+      <c r="V148"/>
+      <c r="W148"/>
+      <c r="X148"/>
+      <c r="Y148"/>
+      <c r="Z148"/>
+      <c r="AA148"/>
+      <c r="AB148"/>
+      <c r="AC148"/>
+      <c r="AD148"/>
+      <c r="AE148"/>
+      <c r="AF148"/>
+      <c r="AG148"/>
+      <c r="AH148"/>
+      <c r="AI148"/>
+      <c r="AJ148"/>
+      <c r="AK148"/>
+      <c r="AL148"/>
+      <c r="AM148"/>
+      <c r="AN148"/>
+      <c r="AO148"/>
+      <c r="AP148"/>
+      <c r="AQ148"/>
     </row>
     <row r="149" ht="14.25">
       <c r="A149" s="7" t="s">
+        <v>447</v>
+      </c>
+      <c r="B149" s="9" t="s">
         <v>448</v>
       </c>
-      <c r="B149" s="9" t="s">
+      <c r="C149" s="11" t="s">
         <v>449</v>
       </c>
-      <c r="C149" s="11" t="s">
+      <c r="D149" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="D149" s="2" t="s">
-        <v>447</v>
-      </c>
-      <c r="E149" s="21" t="s">
+      <c r="E149" s="16" t="s">
         <v>10</v>
       </c>
       <c r="F149" s="4"/>
@@ -6665,123 +6777,123 @@
         <v>453</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>454</v>
-      </c>
-      <c r="E150" s="21" t="s">
+        <v>450</v>
+      </c>
+      <c r="E150" s="22" t="s">
         <v>10</v>
       </c>
       <c r="F150" s="4"/>
     </row>
     <row r="151" ht="14.25">
       <c r="A151" s="7" t="s">
+        <v>454</v>
+      </c>
+      <c r="B151" s="9" t="s">
         <v>455</v>
       </c>
-      <c r="B151" s="9" t="s">
+      <c r="C151" s="11" t="s">
         <v>456</v>
       </c>
-      <c r="C151" s="11" t="s">
+      <c r="D151" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="D151" s="2" t="s">
+      <c r="E151" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F151" s="4"/>
+    </row>
+    <row r="152" ht="14.25">
+      <c r="A152" s="7" t="s">
         <v>458</v>
       </c>
-      <c r="E151" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F151" s="4"/>
-    </row>
-    <row r="152" ht="14.25">
-      <c r="A152" s="10" t="s">
+      <c r="B152" s="9" t="s">
         <v>459</v>
       </c>
-      <c r="B152" s="9" t="s">
+      <c r="C152" s="11" t="s">
         <v>460</v>
       </c>
-      <c r="C152" s="11" t="s">
+      <c r="D152" s="2" t="s">
         <v>461</v>
       </c>
-      <c r="D152" s="2" t="s">
+      <c r="E152" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F152" s="4"/>
+    </row>
+    <row r="153" ht="14.25">
+      <c r="A153" s="10" t="s">
         <v>462</v>
       </c>
-      <c r="E152" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F152" s="4"/>
-    </row>
-    <row r="153" ht="15">
-      <c r="A153" s="10" t="s">
+      <c r="B153" s="9" t="s">
         <v>463</v>
       </c>
-      <c r="B153" s="22" t="s">
+      <c r="C153" s="11" t="s">
         <v>464</v>
       </c>
-      <c r="C153" s="11" t="s">
+      <c r="D153" s="2" t="s">
         <v>465</v>
       </c>
-      <c r="D153" s="2" t="s">
+      <c r="E153" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F153" s="4"/>
+    </row>
+    <row r="154" ht="15">
+      <c r="A154" s="10" t="s">
         <v>466</v>
       </c>
-      <c r="E153" s="23" t="s">
+      <c r="B154" s="23" t="s">
+        <v>467</v>
+      </c>
+      <c r="C154" s="11" t="s">
+        <v>468</v>
+      </c>
+      <c r="D154" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="E154" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="F153" s="4"/>
-    </row>
-    <row r="154" ht="42.75">
-      <c r="A154" s="7" t="s">
-        <v>467</v>
-      </c>
-      <c r="B154" s="12" t="s">
-        <v>468</v>
-      </c>
-      <c r="C154" s="11" t="s">
-        <v>469</v>
-      </c>
-      <c r="D154" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="E154" s="23" t="s">
-        <v>66</v>
-      </c>
       <c r="F154" s="4"/>
     </row>
-    <row r="155" ht="14.25">
+    <row r="155" ht="42.75">
       <c r="A155" s="7" t="s">
         <v>470</v>
       </c>
-      <c r="B155" s="9" t="s">
+      <c r="B155" s="12" t="s">
         <v>471</v>
       </c>
       <c r="C155" s="11" t="s">
         <v>472</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>473</v>
-      </c>
-      <c r="E155" s="21" t="s">
-        <v>10</v>
+        <v>469</v>
+      </c>
+      <c r="E155" s="24" t="s">
+        <v>66</v>
       </c>
       <c r="F155" s="4"/>
     </row>
     <row r="156" ht="14.25">
       <c r="A156" s="7" t="s">
+        <v>473</v>
+      </c>
+      <c r="B156" s="9" t="s">
         <v>474</v>
       </c>
-      <c r="B156" s="9" t="s">
+      <c r="C156" s="11" t="s">
         <v>475</v>
       </c>
-      <c r="C156" s="11" t="s">
+      <c r="D156" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="D156" s="2" t="s">
-        <v>473</v>
-      </c>
-      <c r="E156" s="23" t="s">
-        <v>66</v>
+      <c r="E156" s="22" t="s">
+        <v>10</v>
       </c>
       <c r="F156" s="4"/>
     </row>
     <row r="157" ht="14.25">
-      <c r="A157" s="10" t="s">
+      <c r="A157" s="7" t="s">
         <v>477</v>
       </c>
       <c r="B157" s="9" t="s">
@@ -6791,1164 +6903,1173 @@
         <v>479</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="E157" s="23" t="s">
+        <v>476</v>
+      </c>
+      <c r="E157" s="24" t="s">
         <v>66</v>
       </c>
       <c r="F157" s="4"/>
     </row>
     <row r="158" ht="14.25">
       <c r="A158" s="10" t="s">
+        <v>480</v>
+      </c>
+      <c r="B158" s="9" t="s">
         <v>481</v>
       </c>
-      <c r="B158" s="9" t="s">
+      <c r="C158" s="11" t="s">
         <v>482</v>
       </c>
-      <c r="C158" s="11" t="s">
+      <c r="D158" s="2" t="s">
         <v>483</v>
       </c>
-      <c r="D158" s="2" t="s">
+      <c r="E158" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="F158" s="4"/>
+    </row>
+    <row r="159" ht="14.25">
+      <c r="A159" s="10" t="s">
         <v>484</v>
       </c>
-      <c r="E158" s="23" t="s">
+      <c r="B159" s="9" t="s">
+        <v>485</v>
+      </c>
+      <c r="C159" s="11" t="s">
+        <v>486</v>
+      </c>
+      <c r="D159" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="E159" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="F158" s="4"/>
-    </row>
-    <row r="159" ht="14.25">
-      <c r="A159" t="s">
-        <v>485</v>
-      </c>
-      <c r="B159" s="9"/>
-      <c r="C159" s="1"/>
-      <c r="D159" s="2" t="s">
-        <v>486</v>
-      </c>
-      <c r="E159" s="23" t="s">
+      <c r="F159" s="4"/>
+    </row>
+    <row r="160" ht="14.25">
+      <c r="A160" s="7" t="s">
+        <v>488</v>
+      </c>
+      <c r="B160" s="9" t="s">
+        <v>489</v>
+      </c>
+      <c r="C160" s="11" t="s">
+        <v>490</v>
+      </c>
+      <c r="D160" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="E160" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="F159" s="4"/>
-    </row>
-    <row r="160" ht="14.25">
-      <c r="A160" t="s">
-        <v>487</v>
-      </c>
-      <c r="B160" s="9"/>
-      <c r="C160" s="1"/>
-      <c r="D160" s="2" t="s">
-        <v>488</v>
-      </c>
-      <c r="E160" s="23" t="s">
-        <v>66</v>
-      </c>
       <c r="F160" s="4"/>
-      <c r="L160" t="s">
-        <v>489</v>
-      </c>
     </row>
     <row r="161" ht="14.25">
-      <c r="A161" t="s">
-        <v>490</v>
-      </c>
-      <c r="B161" s="9"/>
+      <c r="A161" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="B161" s="9" t="s">
+        <v>493</v>
+      </c>
       <c r="C161" s="1"/>
       <c r="D161" s="2" t="s">
-        <v>491</v>
-      </c>
-      <c r="E161" s="21" t="s">
-        <v>10</v>
+        <v>494</v>
+      </c>
+      <c r="E161" s="24" t="s">
+        <v>66</v>
       </c>
       <c r="F161" s="4"/>
+      <c r="L161" t="s">
+        <v>495</v>
+      </c>
     </row>
     <row r="162" ht="14.25">
       <c r="A162" t="s">
-        <v>492</v>
+        <v>496</v>
       </c>
       <c r="B162" s="9"/>
       <c r="C162" s="1"/>
       <c r="D162" s="2" t="s">
-        <v>493</v>
-      </c>
-      <c r="E162" s="21" t="s">
+        <v>497</v>
+      </c>
+      <c r="E162" s="22" t="s">
         <v>10</v>
       </c>
       <c r="F162" s="4"/>
     </row>
     <row r="163" ht="14.25">
       <c r="A163" t="s">
-        <v>494</v>
+        <v>498</v>
       </c>
       <c r="B163" s="9"/>
       <c r="C163" s="1"/>
       <c r="D163" s="2" t="s">
-        <v>495</v>
-      </c>
-      <c r="E163" s="23" t="s">
-        <v>66</v>
+        <v>499</v>
+      </c>
+      <c r="E163" s="22" t="s">
+        <v>10</v>
       </c>
       <c r="F163" s="4"/>
     </row>
     <row r="164" ht="14.25">
-      <c r="A164" s="24" t="s">
-        <v>496</v>
+      <c r="A164" t="s">
+        <v>500</v>
       </c>
       <c r="B164" s="9"/>
       <c r="C164" s="1"/>
       <c r="D164" s="2" t="s">
-        <v>497</v>
-      </c>
-      <c r="E164" s="21" t="s">
-        <v>10</v>
+        <v>501</v>
+      </c>
+      <c r="E164" s="24" t="s">
+        <v>66</v>
       </c>
       <c r="F164" s="4"/>
     </row>
     <row r="165" ht="14.25">
-      <c r="A165" t="s">
-        <v>498</v>
+      <c r="A165" s="25" t="s">
+        <v>502</v>
       </c>
       <c r="B165" s="9"/>
       <c r="C165" s="1"/>
       <c r="D165" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="E165" s="21" t="s">
+        <v>503</v>
+      </c>
+      <c r="E165" s="22" t="s">
         <v>10</v>
       </c>
       <c r="F165" s="4"/>
     </row>
     <row r="166" ht="14.25">
       <c r="A166" t="s">
-        <v>500</v>
+        <v>504</v>
       </c>
       <c r="B166" s="9"/>
       <c r="C166" s="1"/>
       <c r="D166" s="2" t="s">
-        <v>501</v>
-      </c>
-      <c r="E166" s="21" t="s">
+        <v>505</v>
+      </c>
+      <c r="E166" s="22" t="s">
         <v>10</v>
       </c>
       <c r="F166" s="4"/>
     </row>
     <row r="167" ht="14.25">
       <c r="A167" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
       <c r="B167" s="9"/>
       <c r="C167" s="1"/>
       <c r="D167" s="2" t="s">
-        <v>503</v>
-      </c>
-      <c r="E167" s="23" t="s">
-        <v>66</v>
+        <v>507</v>
+      </c>
+      <c r="E167" s="22" t="s">
+        <v>10</v>
       </c>
       <c r="F167" s="4"/>
     </row>
     <row r="168" ht="14.25">
       <c r="A168" t="s">
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="B168" s="9"/>
       <c r="C168" s="1"/>
       <c r="D168" s="2" t="s">
-        <v>505</v>
-      </c>
-      <c r="E168" s="23" t="s">
+        <v>509</v>
+      </c>
+      <c r="E168" s="24" t="s">
         <v>66</v>
       </c>
       <c r="F168" s="4"/>
     </row>
     <row r="169" ht="14.25">
       <c r="A169" t="s">
-        <v>506</v>
+        <v>510</v>
       </c>
       <c r="B169" s="9"/>
       <c r="C169" s="1"/>
       <c r="D169" s="2" t="s">
-        <v>507</v>
-      </c>
-      <c r="E169" s="23" t="s">
+        <v>511</v>
+      </c>
+      <c r="E169" s="24" t="s">
         <v>66</v>
       </c>
       <c r="F169" s="4"/>
     </row>
     <row r="170" ht="14.25">
       <c r="A170" t="s">
-        <v>508</v>
+        <v>512</v>
       </c>
       <c r="B170" s="9"/>
       <c r="C170" s="1"/>
       <c r="D170" s="2" t="s">
-        <v>509</v>
-      </c>
-      <c r="E170" s="23" t="s">
+        <v>513</v>
+      </c>
+      <c r="E170" s="24" t="s">
         <v>66</v>
       </c>
       <c r="F170" s="4"/>
     </row>
     <row r="171" ht="14.25">
       <c r="A171" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="B171" s="9"/>
       <c r="C171" s="1"/>
       <c r="D171" s="2" t="s">
-        <v>511</v>
-      </c>
-      <c r="E171" s="23" t="s">
+        <v>515</v>
+      </c>
+      <c r="E171" s="24" t="s">
         <v>66</v>
       </c>
       <c r="F171" s="4"/>
     </row>
     <row r="172" ht="14.25">
       <c r="A172" t="s">
-        <v>512</v>
+        <v>516</v>
       </c>
       <c r="B172" s="9"/>
       <c r="C172" s="1"/>
       <c r="D172" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E172" s="21" t="s">
-        <v>10</v>
+        <v>517</v>
+      </c>
+      <c r="E172" s="24" t="s">
+        <v>66</v>
       </c>
       <c r="F172" s="4"/>
     </row>
     <row r="173" ht="14.25">
       <c r="A173" t="s">
-        <v>514</v>
+        <v>518</v>
       </c>
       <c r="B173" s="9"/>
       <c r="C173" s="1"/>
       <c r="D173" s="2" t="s">
-        <v>515</v>
-      </c>
-      <c r="E173" s="21" t="s">
+        <v>519</v>
+      </c>
+      <c r="E173" s="22" t="s">
         <v>10</v>
       </c>
       <c r="F173" s="4"/>
     </row>
     <row r="174" ht="14.25">
       <c r="A174" t="s">
-        <v>516</v>
+        <v>520</v>
       </c>
       <c r="B174" s="9"/>
       <c r="C174" s="1"/>
       <c r="D174" s="2" t="s">
-        <v>517</v>
-      </c>
-      <c r="E174" s="21" t="s">
+        <v>521</v>
+      </c>
+      <c r="E174" s="22" t="s">
         <v>10</v>
       </c>
       <c r="F174" s="4"/>
     </row>
     <row r="175" ht="14.25">
       <c r="A175" t="s">
-        <v>518</v>
+        <v>522</v>
       </c>
       <c r="B175" s="9"/>
       <c r="C175" s="1"/>
       <c r="D175" s="2" t="s">
-        <v>519</v>
-      </c>
-      <c r="E175" s="23" t="s">
-        <v>66</v>
+        <v>523</v>
+      </c>
+      <c r="E175" s="22" t="s">
+        <v>10</v>
       </c>
       <c r="F175" s="4"/>
     </row>
     <row r="176" ht="14.25">
       <c r="A176" t="s">
-        <v>520</v>
+        <v>524</v>
       </c>
       <c r="B176" s="9"/>
       <c r="C176" s="1"/>
       <c r="D176" s="2" t="s">
-        <v>521</v>
-      </c>
-      <c r="E176" s="23" t="s">
+        <v>525</v>
+      </c>
+      <c r="E176" s="24" t="s">
         <v>66</v>
       </c>
       <c r="F176" s="4"/>
     </row>
     <row r="177" ht="14.25">
       <c r="A177" t="s">
-        <v>522</v>
+        <v>526</v>
       </c>
       <c r="B177" s="9"/>
       <c r="C177" s="1"/>
       <c r="D177" s="2" t="s">
-        <v>523</v>
-      </c>
-      <c r="E177" s="23" t="s">
+        <v>527</v>
+      </c>
+      <c r="E177" s="24" t="s">
         <v>66</v>
       </c>
       <c r="F177" s="4"/>
     </row>
     <row r="178" ht="14.25">
       <c r="A178" t="s">
-        <v>524</v>
+        <v>528</v>
       </c>
       <c r="B178" s="9"/>
       <c r="C178" s="1"/>
       <c r="D178" s="2" t="s">
-        <v>525</v>
-      </c>
-      <c r="E178" s="21" t="s">
-        <v>10</v>
+        <v>529</v>
+      </c>
+      <c r="E178" s="24" t="s">
+        <v>66</v>
       </c>
       <c r="F178" s="4"/>
     </row>
     <row r="179" ht="14.25">
       <c r="A179" t="s">
-        <v>526</v>
+        <v>530</v>
       </c>
       <c r="B179" s="9"/>
       <c r="C179" s="1"/>
       <c r="D179" s="2" t="s">
-        <v>527</v>
-      </c>
-      <c r="E179" s="23" t="s">
-        <v>66</v>
+        <v>531</v>
+      </c>
+      <c r="E179" s="22" t="s">
+        <v>10</v>
       </c>
       <c r="F179" s="4"/>
     </row>
     <row r="180" ht="14.25">
       <c r="A180" t="s">
-        <v>528</v>
+        <v>532</v>
       </c>
       <c r="B180" s="9"/>
       <c r="C180" s="1"/>
       <c r="D180" s="2" t="s">
-        <v>529</v>
-      </c>
-      <c r="E180" s="21" t="s">
-        <v>10</v>
+        <v>533</v>
+      </c>
+      <c r="E180" s="24" t="s">
+        <v>66</v>
       </c>
       <c r="F180" s="4"/>
     </row>
     <row r="181" ht="14.25">
       <c r="A181" t="s">
-        <v>530</v>
+        <v>534</v>
       </c>
       <c r="B181" s="9"/>
       <c r="C181" s="1"/>
       <c r="D181" s="2" t="s">
-        <v>531</v>
-      </c>
-      <c r="E181" s="23" t="s">
-        <v>66</v>
+        <v>535</v>
+      </c>
+      <c r="E181" s="22" t="s">
+        <v>10</v>
       </c>
       <c r="F181" s="4"/>
     </row>
     <row r="182" ht="14.25">
       <c r="A182" t="s">
-        <v>532</v>
+        <v>536</v>
       </c>
       <c r="B182" s="9"/>
       <c r="C182" s="1"/>
       <c r="D182" s="2" t="s">
-        <v>533</v>
-      </c>
-      <c r="E182" s="21" t="s">
-        <v>10</v>
+        <v>537</v>
+      </c>
+      <c r="E182" s="24" t="s">
+        <v>66</v>
       </c>
       <c r="F182" s="4"/>
     </row>
     <row r="183" ht="14.25">
       <c r="A183" t="s">
-        <v>534</v>
+        <v>538</v>
       </c>
       <c r="B183" s="9"/>
       <c r="C183" s="1"/>
       <c r="D183" s="2" t="s">
-        <v>535</v>
-      </c>
-      <c r="E183" s="21" t="s">
+        <v>539</v>
+      </c>
+      <c r="E183" s="22" t="s">
         <v>10</v>
       </c>
       <c r="F183" s="4"/>
     </row>
     <row r="184" ht="14.25">
       <c r="A184" t="s">
-        <v>536</v>
+        <v>540</v>
       </c>
       <c r="B184" s="9"/>
       <c r="C184" s="1"/>
       <c r="D184" s="2" t="s">
-        <v>537</v>
-      </c>
-      <c r="E184" s="23" t="s">
-        <v>66</v>
+        <v>541</v>
+      </c>
+      <c r="E184" s="22" t="s">
+        <v>10</v>
       </c>
       <c r="F184" s="4"/>
     </row>
     <row r="185" ht="14.25">
       <c r="A185" t="s">
-        <v>538</v>
+        <v>542</v>
       </c>
       <c r="B185" s="9"/>
       <c r="C185" s="1"/>
       <c r="D185" s="2" t="s">
-        <v>539</v>
-      </c>
-      <c r="E185" s="23" t="s">
+        <v>543</v>
+      </c>
+      <c r="E185" s="24" t="s">
         <v>66</v>
       </c>
       <c r="F185" s="4"/>
     </row>
     <row r="186" ht="14.25">
       <c r="A186" t="s">
-        <v>540</v>
+        <v>544</v>
       </c>
       <c r="B186" s="9"/>
       <c r="C186" s="1"/>
       <c r="D186" s="2" t="s">
-        <v>541</v>
-      </c>
-      <c r="E186" s="23" t="s">
+        <v>545</v>
+      </c>
+      <c r="E186" s="24" t="s">
         <v>66</v>
       </c>
       <c r="F186" s="4"/>
     </row>
     <row r="187" ht="14.25">
       <c r="A187" t="s">
-        <v>542</v>
+        <v>546</v>
       </c>
       <c r="B187" s="9"/>
       <c r="C187" s="1"/>
       <c r="D187" s="2" t="s">
-        <v>543</v>
-      </c>
-      <c r="E187" s="23" t="s">
+        <v>547</v>
+      </c>
+      <c r="E187" s="24" t="s">
         <v>66</v>
       </c>
       <c r="F187" s="4"/>
     </row>
     <row r="188" ht="14.25">
       <c r="A188" t="s">
-        <v>544</v>
+        <v>548</v>
       </c>
       <c r="B188" s="9"/>
       <c r="C188" s="1"/>
       <c r="D188" s="2" t="s">
-        <v>545</v>
-      </c>
-      <c r="E188" s="21" t="s">
-        <v>10</v>
+        <v>549</v>
+      </c>
+      <c r="E188" s="24" t="s">
+        <v>66</v>
       </c>
       <c r="F188" s="4"/>
     </row>
     <row r="189" ht="14.25">
       <c r="A189" t="s">
-        <v>546</v>
+        <v>550</v>
       </c>
       <c r="B189" s="9"/>
       <c r="C189" s="1"/>
       <c r="D189" s="2" t="s">
-        <v>547</v>
-      </c>
-      <c r="E189" s="23" t="s">
-        <v>66</v>
+        <v>551</v>
+      </c>
+      <c r="E189" s="22" t="s">
+        <v>10</v>
       </c>
       <c r="F189" s="4"/>
     </row>
     <row r="190" ht="14.25">
       <c r="A190" t="s">
-        <v>548</v>
+        <v>552</v>
       </c>
       <c r="B190" s="9"/>
       <c r="C190" s="1"/>
       <c r="D190" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="E190" s="21" t="s">
-        <v>10</v>
+        <v>553</v>
+      </c>
+      <c r="E190" s="24" t="s">
+        <v>66</v>
       </c>
       <c r="F190" s="4"/>
     </row>
     <row r="191" ht="14.25">
       <c r="A191" t="s">
-        <v>550</v>
+        <v>554</v>
       </c>
       <c r="B191" s="9"/>
       <c r="C191" s="1"/>
       <c r="D191" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="E191" s="23" t="s">
-        <v>66</v>
+        <v>555</v>
+      </c>
+      <c r="E191" s="22" t="s">
+        <v>10</v>
       </c>
       <c r="F191" s="4"/>
     </row>
     <row r="192" ht="14.25">
       <c r="A192" t="s">
-        <v>552</v>
+        <v>556</v>
       </c>
       <c r="B192" s="9"/>
       <c r="C192" s="1"/>
       <c r="D192" s="2" t="s">
-        <v>553</v>
-      </c>
-      <c r="E192" s="18" t="s">
+        <v>557</v>
+      </c>
+      <c r="E192" s="24" t="s">
         <v>66</v>
       </c>
       <c r="F192" s="4"/>
     </row>
     <row r="193" ht="14.25">
-      <c r="A193" s="4"/>
-      <c r="B193" s="4"/>
-      <c r="C193" s="4"/>
-      <c r="D193" s="4"/>
-      <c r="E193" s="4"/>
+      <c r="A193" t="s">
+        <v>558</v>
+      </c>
+      <c r="B193" s="9"/>
+      <c r="C193" s="1"/>
+      <c r="D193" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="E193" s="18" t="s">
+        <v>66</v>
+      </c>
       <c r="F193" s="4"/>
     </row>
     <row r="194" ht="14.25">
-      <c r="C194"/>
-      <c r="D194"/>
-      <c r="E194"/>
-      <c r="F194"/>
+      <c r="A194" s="4"/>
+      <c r="B194" s="4"/>
+      <c r="C194" s="4"/>
+      <c r="D194" s="4"/>
+      <c r="E194" s="4"/>
+      <c r="F194" s="4"/>
     </row>
     <row r="195" ht="14.25">
-      <c r="A195" s="5" t="s">
-        <v>554</v>
-      </c>
-      <c r="B195" s="5"/>
-      <c r="C195" s="5"/>
-      <c r="D195" s="5"/>
-      <c r="E195" s="5"/>
-      <c r="F195" s="5"/>
+      <c r="C195"/>
+      <c r="D195"/>
+      <c r="E195"/>
+      <c r="F195"/>
     </row>
     <row r="196" ht="14.25">
-      <c r="A196" s="4" t="s">
-        <v>555</v>
-      </c>
-      <c r="B196" s="4" t="s">
+      <c r="A196" s="5" t="s">
+        <v>560</v>
+      </c>
+      <c r="B196" s="5"/>
+      <c r="C196" s="5"/>
+      <c r="D196" s="5"/>
+      <c r="E196" s="5"/>
+      <c r="F196" s="5"/>
+    </row>
+    <row r="197" ht="14.25">
+      <c r="A197" s="4" t="s">
+        <v>561</v>
+      </c>
+      <c r="B197" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C196" s="4" t="s">
-        <v>556</v>
-      </c>
-      <c r="D196" s="4" t="s">
-        <v>557</v>
-      </c>
-      <c r="E196" s="4"/>
-      <c r="F196" s="4"/>
-    </row>
-    <row r="197" ht="14.25">
-      <c r="A197" s="20" t="s">
-        <v>558</v>
-      </c>
-      <c r="B197" s="9"/>
-      <c r="C197" s="1" t="s">
-        <v>559</v>
-      </c>
-      <c r="D197" s="2" t="s">
-        <v>560</v>
-      </c>
+      <c r="C197" s="4" t="s">
+        <v>562</v>
+      </c>
+      <c r="D197" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="E197" s="4"/>
       <c r="F197" s="4"/>
     </row>
     <row r="198" ht="14.25">
-      <c r="A198" s="20" t="s">
-        <v>561</v>
+      <c r="A198" s="21" t="s">
+        <v>564</v>
       </c>
       <c r="B198" s="9"/>
       <c r="C198" s="1" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>560</v>
+        <v>566</v>
       </c>
       <c r="F198" s="4"/>
-      <c r="H198" s="6"/>
     </row>
     <row r="199" ht="14.25">
-      <c r="A199" s="20" t="s">
-        <v>563</v>
+      <c r="A199" s="21" t="s">
+        <v>567</v>
       </c>
       <c r="B199" s="9"/>
       <c r="C199" s="1" t="s">
-        <v>564</v>
+        <v>568</v>
       </c>
       <c r="D199" s="2" t="s">
-        <v>560</v>
+        <v>566</v>
       </c>
       <c r="F199" s="4"/>
+      <c r="H199" s="6"/>
     </row>
     <row r="200" ht="14.25">
-      <c r="A200" s="20" t="s">
-        <v>565</v>
+      <c r="A200" s="21" t="s">
+        <v>569</v>
       </c>
       <c r="B200" s="9"/>
       <c r="C200" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="D200" s="2" t="s">
         <v>566</v>
       </c>
-      <c r="D200" s="2" t="s">
-        <v>560</v>
-      </c>
       <c r="F200" s="4"/>
     </row>
     <row r="201" ht="14.25">
-      <c r="A201" s="20" t="s">
-        <v>567</v>
+      <c r="A201" s="21" t="s">
+        <v>571</v>
       </c>
       <c r="B201" s="9"/>
       <c r="C201" s="1" t="s">
-        <v>568</v>
+        <v>572</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>560</v>
+        <v>566</v>
       </c>
       <c r="F201" s="4"/>
     </row>
     <row r="202" ht="14.25">
-      <c r="A202" s="20" t="s">
-        <v>569</v>
+      <c r="A202" s="21" t="s">
+        <v>573</v>
       </c>
       <c r="B202" s="9"/>
       <c r="C202" s="1" t="s">
-        <v>570</v>
+        <v>574</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
       <c r="F202" s="4"/>
     </row>
     <row r="203" ht="14.25">
-      <c r="A203" s="20" t="s">
-        <v>572</v>
+      <c r="A203" s="21" t="s">
+        <v>575</v>
       </c>
       <c r="B203" s="9"/>
       <c r="C203" s="1" t="s">
-        <v>573</v>
+        <v>576</v>
       </c>
       <c r="D203" s="2" t="s">
-        <v>571</v>
+        <v>577</v>
       </c>
       <c r="F203" s="4"/>
-      <c r="H203" s="6"/>
     </row>
     <row r="204" ht="14.25">
-      <c r="A204" s="20" t="s">
-        <v>574</v>
+      <c r="A204" s="21" t="s">
+        <v>578</v>
       </c>
       <c r="B204" s="9"/>
       <c r="C204" s="1" t="s">
-        <v>575</v>
+        <v>579</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>571</v>
+        <v>577</v>
       </c>
       <c r="F204" s="4"/>
       <c r="H204" s="6"/>
     </row>
     <row r="205" ht="14.25">
-      <c r="A205" s="20" t="s">
-        <v>576</v>
+      <c r="A205" s="21" t="s">
+        <v>580</v>
       </c>
       <c r="B205" s="9"/>
       <c r="C205" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="D205" s="2" t="s">
         <v>577</v>
-      </c>
-      <c r="D205" s="2" t="s">
-        <v>578</v>
       </c>
       <c r="F205" s="4"/>
       <c r="H205" s="6"/>
     </row>
     <row r="206" ht="14.25">
-      <c r="A206" s="20" t="s">
-        <v>579</v>
+      <c r="A206" s="21" t="s">
+        <v>582</v>
       </c>
       <c r="B206" s="9"/>
       <c r="C206" s="1" t="s">
-        <v>580</v>
+        <v>583</v>
       </c>
       <c r="D206" s="2" t="s">
-        <v>578</v>
+        <v>584</v>
       </c>
       <c r="F206" s="4"/>
       <c r="H206" s="6"/>
     </row>
     <row r="207" ht="14.25">
-      <c r="A207" s="20" t="s">
-        <v>581</v>
+      <c r="A207" s="21" t="s">
+        <v>585</v>
       </c>
       <c r="B207" s="9"/>
       <c r="C207" s="1" t="s">
-        <v>582</v>
+        <v>586</v>
       </c>
       <c r="D207" s="2" t="s">
-        <v>578</v>
+        <v>584</v>
       </c>
       <c r="F207" s="4"/>
       <c r="H207" s="6"/>
     </row>
     <row r="208" ht="14.25">
-      <c r="A208" s="20" t="s">
-        <v>583</v>
+      <c r="A208" s="21" t="s">
+        <v>587</v>
       </c>
       <c r="B208" s="9"/>
       <c r="C208" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="D208" s="2" t="s">
         <v>584</v>
-      </c>
-      <c r="D208" s="2" t="s">
-        <v>578</v>
       </c>
       <c r="F208" s="4"/>
       <c r="H208" s="6"/>
     </row>
     <row r="209" ht="14.25">
-      <c r="A209" s="20" t="s">
-        <v>585</v>
+      <c r="A209" s="21" t="s">
+        <v>589</v>
       </c>
       <c r="B209" s="9"/>
       <c r="C209" s="1" t="s">
-        <v>586</v>
+        <v>590</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>578</v>
+        <v>584</v>
       </c>
       <c r="F209" s="4"/>
       <c r="H209" s="6"/>
     </row>
     <row r="210" ht="14.25">
-      <c r="A210" s="20" t="s">
-        <v>587</v>
+      <c r="A210" s="21" t="s">
+        <v>591</v>
       </c>
       <c r="B210" s="9"/>
       <c r="C210" s="1" t="s">
-        <v>588</v>
+        <v>592</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>578</v>
+        <v>584</v>
       </c>
       <c r="F210" s="4"/>
+      <c r="H210" s="6"/>
     </row>
     <row r="211" ht="14.25">
-      <c r="A211" s="20" t="s">
-        <v>589</v>
+      <c r="A211" s="21" t="s">
+        <v>593</v>
       </c>
       <c r="B211" s="9"/>
       <c r="C211" s="1" t="s">
-        <v>590</v>
+        <v>594</v>
       </c>
       <c r="D211" s="2" t="s">
-        <v>578</v>
+        <v>584</v>
       </c>
       <c r="F211" s="4"/>
     </row>
     <row r="212" ht="14.25">
-      <c r="A212" s="20" t="s">
-        <v>591</v>
+      <c r="A212" s="21" t="s">
+        <v>595</v>
       </c>
       <c r="B212" s="9"/>
       <c r="C212" s="1" t="s">
-        <v>592</v>
+        <v>596</v>
       </c>
       <c r="D212" s="2" t="s">
-        <v>578</v>
+        <v>584</v>
       </c>
       <c r="F212" s="4"/>
     </row>
     <row r="213" ht="14.25">
-      <c r="A213" s="20" t="s">
-        <v>593</v>
+      <c r="A213" s="21" t="s">
+        <v>597</v>
       </c>
       <c r="B213" s="9"/>
       <c r="C213" s="1" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="D213" s="2" t="s">
-        <v>578</v>
+        <v>584</v>
       </c>
       <c r="F213" s="4"/>
     </row>
     <row r="214" ht="14.25">
-      <c r="A214" s="20" t="s">
-        <v>595</v>
+      <c r="A214" s="21" t="s">
+        <v>599</v>
       </c>
       <c r="B214" s="9"/>
       <c r="C214" s="1" t="s">
-        <v>596</v>
+        <v>600</v>
       </c>
       <c r="D214" s="2" t="s">
-        <v>578</v>
+        <v>584</v>
       </c>
       <c r="F214" s="4"/>
     </row>
     <row r="215" ht="14.25">
-      <c r="A215" s="20" t="s">
-        <v>597</v>
+      <c r="A215" s="21" t="s">
+        <v>601</v>
       </c>
       <c r="B215" s="9"/>
       <c r="C215" s="1" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>599</v>
+        <v>584</v>
       </c>
       <c r="F215" s="4"/>
     </row>
     <row r="216" ht="14.25">
-      <c r="A216" s="20" t="s">
-        <v>600</v>
+      <c r="A216" s="21" t="s">
+        <v>603</v>
       </c>
       <c r="B216" s="9"/>
       <c r="C216" s="1" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
       <c r="D216" s="2" t="s">
-        <v>599</v>
+        <v>605</v>
       </c>
       <c r="F216" s="4"/>
     </row>
     <row r="217" ht="14.25">
-      <c r="A217" s="20" t="s">
-        <v>602</v>
+      <c r="A217" s="21" t="s">
+        <v>606</v>
       </c>
       <c r="B217" s="9"/>
       <c r="C217" s="1" t="s">
-        <v>603</v>
+        <v>607</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>599</v>
+        <v>605</v>
       </c>
       <c r="F217" s="4"/>
     </row>
     <row r="218" ht="14.25">
-      <c r="A218" s="20" t="s">
-        <v>604</v>
+      <c r="A218" s="21" t="s">
+        <v>608</v>
       </c>
       <c r="B218" s="9"/>
       <c r="C218" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="D218" s="2" t="s">
         <v>605</v>
       </c>
-      <c r="D218" s="2" t="s">
-        <v>599</v>
-      </c>
       <c r="F218" s="4"/>
     </row>
     <row r="219" ht="14.25">
-      <c r="A219" s="20" t="s">
-        <v>606</v>
+      <c r="A219" s="21" t="s">
+        <v>610</v>
       </c>
       <c r="B219" s="9"/>
       <c r="C219" s="1" t="s">
-        <v>607</v>
+        <v>611</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>599</v>
+        <v>605</v>
       </c>
       <c r="F219" s="4"/>
     </row>
     <row r="220" ht="14.25">
-      <c r="A220" s="20" t="s">
-        <v>608</v>
+      <c r="A220" s="21" t="s">
+        <v>612</v>
       </c>
       <c r="B220" s="9"/>
       <c r="C220" s="1" t="s">
-        <v>609</v>
+        <v>613</v>
       </c>
       <c r="D220" s="2" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="F220" s="4"/>
     </row>
     <row r="221" ht="14.25">
-      <c r="A221" s="20" t="s">
-        <v>611</v>
+      <c r="A221" s="21" t="s">
+        <v>614</v>
       </c>
       <c r="B221" s="9"/>
       <c r="C221" s="1" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
       <c r="D221" s="2" t="s">
-        <v>610</v>
+        <v>616</v>
       </c>
       <c r="F221" s="4"/>
     </row>
     <row r="222" ht="14.25">
-      <c r="A222" s="20" t="s">
-        <v>613</v>
+      <c r="A222" s="21" t="s">
+        <v>617</v>
       </c>
       <c r="B222" s="9"/>
       <c r="C222" s="1" t="s">
-        <v>614</v>
+        <v>618</v>
       </c>
       <c r="D222" s="2" t="s">
-        <v>610</v>
+        <v>616</v>
       </c>
       <c r="F222" s="4"/>
     </row>
     <row r="223" ht="14.25">
-      <c r="A223" s="20" t="s">
-        <v>615</v>
+      <c r="A223" s="21" t="s">
+        <v>619</v>
       </c>
       <c r="B223" s="9"/>
       <c r="C223" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="D223" s="2" t="s">
         <v>616</v>
       </c>
-      <c r="D223" s="2" t="s">
-        <v>610</v>
-      </c>
       <c r="F223" s="4"/>
     </row>
     <row r="224" ht="14.25">
-      <c r="A224" s="20" t="s">
-        <v>617</v>
+      <c r="A224" s="21" t="s">
+        <v>621</v>
       </c>
       <c r="B224" s="9"/>
       <c r="C224" s="1" t="s">
-        <v>618</v>
+        <v>622</v>
       </c>
       <c r="D224" s="2" t="s">
-        <v>610</v>
+        <v>616</v>
       </c>
       <c r="F224" s="4"/>
     </row>
     <row r="225" ht="14.25">
-      <c r="A225" s="20" t="s">
-        <v>619</v>
+      <c r="A225" s="21" t="s">
+        <v>623</v>
       </c>
       <c r="B225" s="9"/>
       <c r="C225" s="1" t="s">
-        <v>620</v>
+        <v>624</v>
       </c>
       <c r="D225" s="2" t="s">
-        <v>610</v>
+        <v>616</v>
       </c>
       <c r="F225" s="4"/>
     </row>
     <row r="226" ht="14.25">
-      <c r="A226" s="20" t="s">
-        <v>621</v>
+      <c r="A226" s="21" t="s">
+        <v>625</v>
       </c>
       <c r="B226" s="9"/>
       <c r="C226" s="1" t="s">
-        <v>622</v>
+        <v>626</v>
       </c>
       <c r="D226" s="2" t="s">
-        <v>610</v>
+        <v>616</v>
       </c>
       <c r="F226" s="4"/>
     </row>
     <row r="227" ht="14.25">
-      <c r="A227" s="20" t="s">
-        <v>623</v>
+      <c r="A227" s="21" t="s">
+        <v>627</v>
       </c>
       <c r="B227" s="9"/>
       <c r="C227" s="1" t="s">
-        <v>624</v>
+        <v>628</v>
       </c>
       <c r="D227" s="2" t="s">
-        <v>625</v>
+        <v>616</v>
       </c>
       <c r="F227" s="4"/>
     </row>
     <row r="228" ht="14.25">
-      <c r="A228" s="20" t="s">
-        <v>626</v>
+      <c r="A228" s="21" t="s">
+        <v>629</v>
       </c>
       <c r="B228" s="9"/>
       <c r="C228" s="1" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="D228" s="2" t="s">
-        <v>625</v>
+        <v>631</v>
       </c>
       <c r="F228" s="4"/>
     </row>
     <row r="229" ht="14.25">
-      <c r="A229" s="20" t="s">
-        <v>628</v>
+      <c r="A229" s="21" t="s">
+        <v>632</v>
       </c>
       <c r="B229" s="9"/>
       <c r="C229" s="1" t="s">
-        <v>629</v>
+        <v>633</v>
       </c>
       <c r="D229" s="2" t="s">
-        <v>625</v>
+        <v>631</v>
       </c>
       <c r="F229" s="4"/>
     </row>
     <row r="230" ht="14.25">
-      <c r="A230" s="20" t="s">
-        <v>630</v>
+      <c r="A230" s="21" t="s">
+        <v>634</v>
       </c>
       <c r="B230" s="9"/>
       <c r="C230" s="1" t="s">
+        <v>635</v>
+      </c>
+      <c r="D230" s="2" t="s">
         <v>631</v>
       </c>
-      <c r="D230" s="2" t="s">
-        <v>632</v>
-      </c>
       <c r="F230" s="4"/>
     </row>
     <row r="231" ht="14.25">
-      <c r="A231" s="20" t="s">
-        <v>633</v>
+      <c r="A231" s="21" t="s">
+        <v>636</v>
       </c>
       <c r="B231" s="9"/>
       <c r="C231" s="1" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
       <c r="D231" s="2" t="s">
-        <v>632</v>
+        <v>638</v>
       </c>
       <c r="F231" s="4"/>
     </row>
     <row r="232" ht="14.25">
-      <c r="A232" t="s">
-        <v>635</v>
+      <c r="A232" s="21" t="s">
+        <v>639</v>
       </c>
       <c r="B232" s="9"/>
       <c r="C232" s="1" t="s">
-        <v>636</v>
+        <v>640</v>
       </c>
       <c r="D232" s="2" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="F232" s="4"/>
-      <c r="H232" s="6"/>
     </row>
     <row r="233" ht="14.25">
       <c r="A233" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B233" s="9"/>
       <c r="C233" s="1" t="s">
-        <v>639</v>
+        <v>642</v>
       </c>
       <c r="D233" s="2" t="s">
-        <v>640</v>
+        <v>643</v>
       </c>
       <c r="F233" s="4"/>
       <c r="H233" s="6"/>
     </row>
     <row r="234" ht="14.25">
       <c r="A234" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
       <c r="B234" s="9"/>
       <c r="C234" s="1" t="s">
-        <v>642</v>
+        <v>645</v>
       </c>
       <c r="D234" s="2" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
       <c r="F234" s="4"/>
       <c r="H234" s="6"/>
     </row>
     <row r="235" ht="14.25">
       <c r="A235" t="s">
-        <v>644</v>
+        <v>647</v>
       </c>
       <c r="B235" s="9"/>
       <c r="C235" s="1" t="s">
-        <v>645</v>
+        <v>648</v>
       </c>
       <c r="D235" s="2" t="s">
-        <v>578</v>
+        <v>649</v>
       </c>
       <c r="F235" s="4"/>
       <c r="H235" s="6"/>
     </row>
     <row r="236" ht="14.25">
       <c r="A236" t="s">
-        <v>646</v>
+        <v>650</v>
       </c>
       <c r="B236" s="9"/>
       <c r="C236" s="1" t="s">
-        <v>647</v>
+        <v>651</v>
       </c>
       <c r="D236" s="2" t="s">
-        <v>648</v>
+        <v>584</v>
       </c>
       <c r="F236" s="4"/>
       <c r="H236" s="6"/>
     </row>
     <row r="237" ht="14.25">
       <c r="A237" t="s">
-        <v>649</v>
+        <v>652</v>
       </c>
       <c r="B237" s="9"/>
       <c r="C237" s="1" t="s">
-        <v>650</v>
+        <v>653</v>
       </c>
       <c r="D237" s="2" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
       <c r="F237" s="4"/>
       <c r="H237" s="6"/>
     </row>
     <row r="238" ht="14.25">
       <c r="A238" t="s">
-        <v>652</v>
+        <v>655</v>
       </c>
       <c r="B238" s="9"/>
       <c r="C238" s="1" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="D238" s="2" t="s">
-        <v>654</v>
+        <v>657</v>
       </c>
       <c r="F238" s="4"/>
       <c r="H238" s="6"/>
     </row>
     <row r="239" ht="14.25">
       <c r="A239" t="s">
-        <v>655</v>
+        <v>658</v>
       </c>
       <c r="B239" s="9"/>
       <c r="C239" s="1" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
       <c r="D239" s="2" t="s">
-        <v>654</v>
+        <v>660</v>
       </c>
       <c r="F239" s="4"/>
       <c r="H239" s="6"/>
     </row>
     <row r="240" ht="14.25">
       <c r="A240" t="s">
-        <v>657</v>
+        <v>661</v>
       </c>
       <c r="B240" s="9"/>
       <c r="C240" s="1" t="s">
-        <v>658</v>
+        <v>662</v>
       </c>
       <c r="D240" s="2" t="s">
-        <v>654</v>
+        <v>660</v>
       </c>
       <c r="F240" s="4"/>
       <c r="H240" s="6"/>
     </row>
     <row r="241" ht="14.25">
       <c r="A241" t="s">
-        <v>659</v>
+        <v>663</v>
       </c>
       <c r="B241" s="9"/>
       <c r="C241" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="D241" s="2" t="s">
         <v>660</v>
       </c>
-      <c r="D241" s="2" t="s">
-        <v>661</v>
-      </c>
-      <c r="E241" s="3"/>
       <c r="F241" s="4"/>
       <c r="H241" s="6"/>
     </row>
     <row r="242" ht="14.25">
       <c r="A242" t="s">
-        <v>662</v>
+        <v>665</v>
       </c>
       <c r="B242" s="9"/>
       <c r="C242" s="1" t="s">
-        <v>663</v>
+        <v>666</v>
       </c>
       <c r="D242" s="2" t="s">
-        <v>664</v>
+        <v>667</v>
       </c>
       <c r="E242" s="3"/>
       <c r="F242" s="4"/>
@@ -7956,14 +8077,14 @@
     </row>
     <row r="243" ht="14.25">
       <c r="A243" t="s">
-        <v>665</v>
+        <v>668</v>
       </c>
       <c r="B243" s="9"/>
       <c r="C243" s="1" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
       <c r="D243" s="2" t="s">
-        <v>654</v>
+        <v>670</v>
       </c>
       <c r="E243" s="3"/>
       <c r="F243" s="4"/>
@@ -7971,14 +8092,14 @@
     </row>
     <row r="244" ht="14.25">
       <c r="A244" t="s">
-        <v>667</v>
+        <v>671</v>
       </c>
       <c r="B244" s="9"/>
       <c r="C244" s="1" t="s">
-        <v>668</v>
+        <v>672</v>
       </c>
       <c r="D244" s="2" t="s">
-        <v>669</v>
+        <v>660</v>
       </c>
       <c r="E244" s="3"/>
       <c r="F244" s="4"/>
@@ -7986,14 +8107,14 @@
     </row>
     <row r="245" ht="14.25">
       <c r="A245" t="s">
-        <v>670</v>
+        <v>673</v>
       </c>
       <c r="B245" s="9"/>
       <c r="C245" s="1" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
       <c r="D245" s="2" t="s">
-        <v>672</v>
+        <v>675</v>
       </c>
       <c r="E245" s="3"/>
       <c r="F245" s="4"/>
@@ -8001,648 +8122,657 @@
     </row>
     <row r="246" ht="14.25">
       <c r="A246" t="s">
-        <v>673</v>
+        <v>676</v>
       </c>
       <c r="B246" s="9"/>
       <c r="C246" s="1" t="s">
-        <v>674</v>
+        <v>677</v>
       </c>
       <c r="D246" s="2" t="s">
-        <v>675</v>
+        <v>678</v>
       </c>
       <c r="E246" s="3"/>
       <c r="F246" s="4"/>
       <c r="H246" s="6"/>
     </row>
     <row r="247" ht="14.25">
-      <c r="A247" s="4"/>
-      <c r="B247" s="4"/>
-      <c r="C247" s="4"/>
-      <c r="D247" s="4"/>
-      <c r="E247" s="4"/>
+      <c r="A247" t="s">
+        <v>679</v>
+      </c>
+      <c r="B247" s="9"/>
+      <c r="C247" s="1" t="s">
+        <v>680</v>
+      </c>
+      <c r="D247" s="2" t="s">
+        <v>681</v>
+      </c>
+      <c r="E247" s="3"/>
       <c r="F247" s="4"/>
+      <c r="H247" s="6"/>
     </row>
     <row r="248" ht="14.25">
-      <c r="C248" s="1"/>
-      <c r="D248" s="2"/>
-      <c r="E248" s="3"/>
+      <c r="A248" s="4"/>
+      <c r="B248" s="4"/>
+      <c r="C248" s="4"/>
+      <c r="D248" s="4"/>
+      <c r="E248" s="4"/>
       <c r="F248" s="4"/>
     </row>
     <row r="249" ht="14.25">
-      <c r="A249" s="5" t="s">
-        <v>676</v>
-      </c>
-      <c r="B249" s="5"/>
-      <c r="C249" s="5"/>
-      <c r="D249" s="5"/>
-      <c r="E249" s="5"/>
-      <c r="F249" s="5"/>
+      <c r="C249" s="1"/>
+      <c r="D249" s="2"/>
+      <c r="E249" s="3"/>
+      <c r="F249" s="4"/>
     </row>
     <row r="250" ht="14.25">
-      <c r="A250" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B250" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="C250" s="19" t="s">
-        <v>443</v>
-      </c>
-      <c r="D250" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E250" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F250" s="4"/>
+      <c r="A250" s="5" t="s">
+        <v>682</v>
+      </c>
+      <c r="B250" s="5"/>
+      <c r="C250" s="5"/>
+      <c r="D250" s="5"/>
+      <c r="E250" s="5"/>
+      <c r="F250" s="5"/>
     </row>
     <row r="251" ht="14.25">
       <c r="A251" s="20" t="s">
-        <v>677</v>
-      </c>
-      <c r="B251" s="9"/>
-      <c r="C251" s="1"/>
-      <c r="D251" s="25" t="s">
-        <v>678</v>
-      </c>
-      <c r="E251" s="16" t="s">
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="B251" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C251" s="20" t="s">
+        <v>446</v>
+      </c>
+      <c r="D251" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E251" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="F251" s="4"/>
     </row>
     <row r="252" ht="14.25">
-      <c r="A252" s="20" t="s">
-        <v>679</v>
+      <c r="A252" s="21" t="s">
+        <v>683</v>
       </c>
       <c r="B252" s="9"/>
       <c r="C252" s="1"/>
-      <c r="D252" s="25" t="s">
-        <v>680</v>
-      </c>
-      <c r="E252" s="21" t="s">
+      <c r="D252" s="26" t="s">
+        <v>684</v>
+      </c>
+      <c r="E252" s="16" t="s">
         <v>10</v>
       </c>
       <c r="F252" s="4"/>
     </row>
     <row r="253" ht="14.25">
-      <c r="A253" s="20" t="s">
-        <v>681</v>
+      <c r="A253" s="21" t="s">
+        <v>685</v>
       </c>
       <c r="B253" s="9"/>
       <c r="C253" s="1"/>
-      <c r="D253" s="25" t="s">
-        <v>682</v>
-      </c>
-      <c r="E253" s="21" t="s">
+      <c r="D253" s="26" t="s">
+        <v>686</v>
+      </c>
+      <c r="E253" s="22" t="s">
         <v>10</v>
       </c>
       <c r="F253" s="4"/>
     </row>
     <row r="254" ht="14.25">
-      <c r="A254" s="20" t="s">
-        <v>683</v>
+      <c r="A254" s="21" t="s">
+        <v>687</v>
       </c>
       <c r="B254" s="9"/>
       <c r="C254" s="1"/>
-      <c r="D254" s="25" t="s">
-        <v>684</v>
-      </c>
-      <c r="E254" s="21" t="s">
+      <c r="D254" s="26" t="s">
+        <v>688</v>
+      </c>
+      <c r="E254" s="22" t="s">
         <v>10</v>
       </c>
       <c r="F254" s="4"/>
     </row>
     <row r="255" ht="14.25">
-      <c r="A255" s="20" t="s">
-        <v>685</v>
+      <c r="A255" s="21" t="s">
+        <v>689</v>
       </c>
       <c r="B255" s="9"/>
       <c r="C255" s="1"/>
-      <c r="D255" s="25" t="s">
-        <v>686</v>
-      </c>
-      <c r="E255" s="21" t="s">
+      <c r="D255" s="26" t="s">
+        <v>690</v>
+      </c>
+      <c r="E255" s="22" t="s">
         <v>10</v>
       </c>
       <c r="F255" s="4"/>
     </row>
     <row r="256" ht="14.25">
-      <c r="A256" s="20" t="s">
-        <v>687</v>
+      <c r="A256" s="21" t="s">
+        <v>691</v>
       </c>
       <c r="B256" s="9"/>
       <c r="C256" s="1"/>
-      <c r="D256" s="25" t="s">
-        <v>686</v>
-      </c>
-      <c r="E256" s="21" t="s">
+      <c r="D256" s="26" t="s">
+        <v>692</v>
+      </c>
+      <c r="E256" s="22" t="s">
         <v>10</v>
       </c>
       <c r="F256" s="4"/>
     </row>
     <row r="257" ht="14.25">
-      <c r="A257" s="20" t="s">
-        <v>688</v>
+      <c r="A257" s="21" t="s">
+        <v>693</v>
       </c>
       <c r="B257" s="9"/>
       <c r="C257" s="1"/>
-      <c r="D257" s="25" t="s">
-        <v>680</v>
-      </c>
-      <c r="E257" s="21" t="s">
+      <c r="D257" s="26" t="s">
+        <v>692</v>
+      </c>
+      <c r="E257" s="22" t="s">
         <v>10</v>
       </c>
       <c r="F257" s="4"/>
     </row>
     <row r="258" ht="14.25">
-      <c r="A258" s="20" t="s">
-        <v>689</v>
+      <c r="A258" s="21" t="s">
+        <v>694</v>
       </c>
       <c r="B258" s="9"/>
       <c r="C258" s="1"/>
-      <c r="D258" s="25" t="s">
-        <v>690</v>
-      </c>
-      <c r="E258" s="21" t="s">
+      <c r="D258" s="26" t="s">
+        <v>686</v>
+      </c>
+      <c r="E258" s="22" t="s">
         <v>10</v>
       </c>
       <c r="F258" s="4"/>
     </row>
     <row r="259" ht="14.25">
-      <c r="A259" s="20" t="s">
-        <v>691</v>
+      <c r="A259" s="21" t="s">
+        <v>695</v>
       </c>
       <c r="B259" s="9"/>
       <c r="C259" s="1"/>
-      <c r="D259" s="25" t="s">
-        <v>690</v>
-      </c>
-      <c r="E259" s="21" t="s">
+      <c r="D259" s="26" t="s">
+        <v>696</v>
+      </c>
+      <c r="E259" s="22" t="s">
         <v>10</v>
       </c>
       <c r="F259" s="4"/>
     </row>
     <row r="260" ht="14.25">
-      <c r="A260" s="20" t="s">
-        <v>692</v>
+      <c r="A260" s="21" t="s">
+        <v>697</v>
       </c>
       <c r="B260" s="9"/>
       <c r="C260" s="1"/>
-      <c r="D260" s="25" t="s">
-        <v>693</v>
-      </c>
-      <c r="E260" s="23" t="s">
-        <v>66</v>
+      <c r="D260" s="26" t="s">
+        <v>696</v>
+      </c>
+      <c r="E260" s="22" t="s">
+        <v>10</v>
       </c>
       <c r="F260" s="4"/>
     </row>
     <row r="261" ht="14.25">
-      <c r="A261" s="20" t="s">
-        <v>694</v>
+      <c r="A261" s="21" t="s">
+        <v>698</v>
       </c>
       <c r="B261" s="9"/>
       <c r="C261" s="1"/>
-      <c r="D261" s="25" t="s">
-        <v>690</v>
-      </c>
-      <c r="E261" s="21" t="s">
-        <v>10</v>
+      <c r="D261" s="26" t="s">
+        <v>699</v>
+      </c>
+      <c r="E261" s="24" t="s">
+        <v>66</v>
       </c>
       <c r="F261" s="4"/>
     </row>
     <row r="262" ht="14.25">
-      <c r="A262" s="20" t="s">
-        <v>695</v>
+      <c r="A262" s="21" t="s">
+        <v>700</v>
       </c>
       <c r="B262" s="9"/>
       <c r="C262" s="1"/>
-      <c r="D262" s="25" t="s">
+      <c r="D262" s="26" t="s">
         <v>696</v>
       </c>
-      <c r="E262" s="23" t="s">
-        <v>66</v>
+      <c r="E262" s="22" t="s">
+        <v>10</v>
       </c>
       <c r="F262" s="4"/>
     </row>
     <row r="263" ht="14.25">
-      <c r="A263" s="20" t="s">
-        <v>697</v>
+      <c r="A263" s="21" t="s">
+        <v>701</v>
       </c>
       <c r="B263" s="9"/>
       <c r="C263" s="1"/>
-      <c r="D263" s="25" t="s">
-        <v>698</v>
-      </c>
-      <c r="E263" s="21" t="s">
-        <v>10</v>
+      <c r="D263" s="26" t="s">
+        <v>702</v>
+      </c>
+      <c r="E263" s="24" t="s">
+        <v>66</v>
       </c>
       <c r="F263" s="4"/>
     </row>
     <row r="264" ht="14.25">
-      <c r="A264" s="20" t="s">
-        <v>451</v>
+      <c r="A264" s="21" t="s">
+        <v>703</v>
       </c>
       <c r="B264" s="9"/>
       <c r="C264" s="1"/>
-      <c r="D264" s="25" t="s">
-        <v>699</v>
-      </c>
-      <c r="E264" s="23" t="s">
-        <v>66</v>
+      <c r="D264" s="26" t="s">
+        <v>704</v>
+      </c>
+      <c r="E264" s="22" t="s">
+        <v>10</v>
       </c>
       <c r="F264" s="4"/>
     </row>
     <row r="265" ht="14.25">
-      <c r="A265" s="20" t="s">
-        <v>444</v>
+      <c r="A265" s="21" t="s">
+        <v>454</v>
       </c>
       <c r="B265" s="9"/>
       <c r="C265" s="1"/>
-      <c r="D265" s="25" t="s">
-        <v>700</v>
-      </c>
-      <c r="E265" s="21" t="s">
-        <v>10</v>
+      <c r="D265" s="26" t="s">
+        <v>705</v>
+      </c>
+      <c r="E265" s="24" t="s">
+        <v>66</v>
       </c>
       <c r="F265" s="4"/>
     </row>
     <row r="266" ht="14.25">
-      <c r="A266" s="20" t="s">
-        <v>701</v>
+      <c r="A266" s="21" t="s">
+        <v>447</v>
       </c>
       <c r="B266" s="9"/>
       <c r="C266" s="1"/>
-      <c r="D266" s="25" t="s">
-        <v>702</v>
-      </c>
-      <c r="E266" s="23" t="s">
-        <v>66</v>
+      <c r="D266" s="26" t="s">
+        <v>706</v>
+      </c>
+      <c r="E266" s="22" t="s">
+        <v>10</v>
       </c>
       <c r="F266" s="4"/>
     </row>
     <row r="267" ht="14.25">
-      <c r="A267" s="20" t="s">
-        <v>703</v>
+      <c r="A267" s="21" t="s">
+        <v>707</v>
       </c>
       <c r="B267" s="9"/>
       <c r="C267" s="1"/>
-      <c r="D267" s="25" t="s">
-        <v>704</v>
-      </c>
-      <c r="E267" s="21" t="s">
-        <v>10</v>
+      <c r="D267" s="26" t="s">
+        <v>708</v>
+      </c>
+      <c r="E267" s="24" t="s">
+        <v>66</v>
       </c>
       <c r="F267" s="4"/>
     </row>
     <row r="268" ht="14.25">
-      <c r="A268" s="20" t="s">
-        <v>705</v>
+      <c r="A268" s="21" t="s">
+        <v>709</v>
       </c>
       <c r="B268" s="9"/>
       <c r="C268" s="1"/>
-      <c r="D268" s="25" t="s">
-        <v>706</v>
-      </c>
-      <c r="E268" s="21" t="s">
+      <c r="D268" s="26" t="s">
+        <v>710</v>
+      </c>
+      <c r="E268" s="22" t="s">
         <v>10</v>
       </c>
       <c r="F268" s="4"/>
     </row>
     <row r="269" ht="14.25">
-      <c r="A269" s="20" t="s">
-        <v>707</v>
+      <c r="A269" s="21" t="s">
+        <v>711</v>
       </c>
       <c r="B269" s="9"/>
       <c r="C269" s="1"/>
-      <c r="D269" s="25" t="s">
-        <v>708</v>
-      </c>
-      <c r="E269" s="23" t="s">
-        <v>66</v>
+      <c r="D269" s="26" t="s">
+        <v>712</v>
+      </c>
+      <c r="E269" s="22" t="s">
+        <v>10</v>
       </c>
       <c r="F269" s="4"/>
     </row>
     <row r="270" ht="14.25">
-      <c r="A270" s="20" t="s">
-        <v>709</v>
+      <c r="A270" s="21" t="s">
+        <v>713</v>
       </c>
       <c r="B270" s="9"/>
       <c r="C270" s="1"/>
-      <c r="D270" s="25" t="s">
-        <v>686</v>
-      </c>
-      <c r="E270" s="21" t="s">
-        <v>10</v>
+      <c r="D270" s="26" t="s">
+        <v>714</v>
+      </c>
+      <c r="E270" s="24" t="s">
+        <v>66</v>
       </c>
       <c r="F270" s="4"/>
     </row>
     <row r="271" ht="14.25">
-      <c r="A271" s="20" t="s">
-        <v>710</v>
+      <c r="A271" s="21" t="s">
+        <v>715</v>
       </c>
       <c r="B271" s="9"/>
       <c r="C271" s="1"/>
-      <c r="D271" s="25" t="s">
-        <v>711</v>
-      </c>
-      <c r="E271" s="21" t="s">
+      <c r="D271" s="26" t="s">
+        <v>692</v>
+      </c>
+      <c r="E271" s="22" t="s">
         <v>10</v>
       </c>
       <c r="F271" s="4"/>
     </row>
     <row r="272" ht="14.25">
-      <c r="A272" s="20" t="s">
-        <v>712</v>
+      <c r="A272" s="21" t="s">
+        <v>716</v>
       </c>
       <c r="B272" s="9"/>
       <c r="C272" s="1"/>
-      <c r="D272" s="25" t="s">
-        <v>686</v>
-      </c>
-      <c r="E272" s="21" t="s">
+      <c r="D272" s="26" t="s">
+        <v>717</v>
+      </c>
+      <c r="E272" s="22" t="s">
         <v>10</v>
       </c>
       <c r="F272" s="4"/>
     </row>
     <row r="273" ht="14.25">
-      <c r="A273" s="20" t="s">
-        <v>713</v>
+      <c r="A273" s="21" t="s">
+        <v>718</v>
       </c>
       <c r="B273" s="9"/>
       <c r="C273" s="1"/>
-      <c r="D273" s="25" t="s">
-        <v>714</v>
-      </c>
-      <c r="E273" s="23" t="s">
-        <v>66</v>
+      <c r="D273" s="26" t="s">
+        <v>692</v>
+      </c>
+      <c r="E273" s="22" t="s">
+        <v>10</v>
       </c>
       <c r="F273" s="4"/>
     </row>
     <row r="274" ht="14.25">
-      <c r="A274" s="20" t="s">
-        <v>715</v>
+      <c r="A274" s="21" t="s">
+        <v>719</v>
       </c>
       <c r="B274" s="9"/>
       <c r="C274" s="1"/>
-      <c r="D274" s="25" t="s">
-        <v>716</v>
-      </c>
-      <c r="E274" s="21" t="s">
-        <v>10</v>
+      <c r="D274" s="26" t="s">
+        <v>720</v>
+      </c>
+      <c r="E274" s="24" t="s">
+        <v>66</v>
       </c>
       <c r="F274" s="4"/>
     </row>
     <row r="275" ht="14.25">
-      <c r="A275" s="20" t="s">
-        <v>717</v>
+      <c r="A275" s="21" t="s">
+        <v>721</v>
       </c>
       <c r="B275" s="9"/>
       <c r="C275" s="1"/>
-      <c r="D275" s="25" t="s">
-        <v>704</v>
-      </c>
-      <c r="E275" s="23" t="s">
-        <v>66</v>
+      <c r="D275" s="26" t="s">
+        <v>722</v>
+      </c>
+      <c r="E275" s="22" t="s">
+        <v>10</v>
       </c>
       <c r="F275" s="4"/>
     </row>
     <row r="276" ht="14.25">
-      <c r="A276" s="20" t="s">
-        <v>718</v>
+      <c r="A276" s="21" t="s">
+        <v>723</v>
       </c>
       <c r="B276" s="9"/>
       <c r="C276" s="1"/>
-      <c r="D276" s="25" t="s">
-        <v>719</v>
-      </c>
-      <c r="E276" s="21" t="s">
-        <v>10</v>
+      <c r="D276" s="26" t="s">
+        <v>710</v>
+      </c>
+      <c r="E276" s="24" t="s">
+        <v>66</v>
       </c>
       <c r="F276" s="4"/>
     </row>
     <row r="277" ht="14.25">
-      <c r="A277" s="20" t="s">
-        <v>720</v>
+      <c r="A277" s="21" t="s">
+        <v>724</v>
       </c>
       <c r="B277" s="9"/>
       <c r="C277" s="1"/>
-      <c r="D277" s="25" t="s">
-        <v>678</v>
-      </c>
-      <c r="E277" s="21" t="s">
+      <c r="D277" s="26" t="s">
+        <v>725</v>
+      </c>
+      <c r="E277" s="22" t="s">
         <v>10</v>
       </c>
       <c r="F277" s="4"/>
     </row>
     <row r="278" ht="14.25">
-      <c r="A278" s="20" t="s">
-        <v>721</v>
+      <c r="A278" s="21" t="s">
+        <v>726</v>
       </c>
       <c r="B278" s="9"/>
       <c r="C278" s="1"/>
-      <c r="D278" s="25" t="s">
-        <v>722</v>
-      </c>
-      <c r="E278" s="23" t="s">
-        <v>66</v>
+      <c r="D278" s="26" t="s">
+        <v>684</v>
+      </c>
+      <c r="E278" s="22" t="s">
+        <v>10</v>
       </c>
       <c r="F278" s="4"/>
     </row>
     <row r="279" ht="14.25">
-      <c r="A279" s="20" t="s">
-        <v>723</v>
+      <c r="A279" s="21" t="s">
+        <v>727</v>
       </c>
       <c r="B279" s="9"/>
       <c r="C279" s="1"/>
-      <c r="D279" s="25" t="s">
-        <v>724</v>
-      </c>
-      <c r="E279" s="23" t="s">
+      <c r="D279" s="26" t="s">
+        <v>728</v>
+      </c>
+      <c r="E279" s="24" t="s">
         <v>66</v>
       </c>
       <c r="F279" s="4"/>
     </row>
     <row r="280" ht="14.25">
-      <c r="A280" s="20" t="s">
-        <v>725</v>
+      <c r="A280" s="21" t="s">
+        <v>729</v>
       </c>
       <c r="B280" s="9"/>
       <c r="C280" s="1"/>
-      <c r="D280" s="25" t="s">
-        <v>726</v>
-      </c>
-      <c r="E280" s="21" t="s">
-        <v>10</v>
+      <c r="D280" s="26" t="s">
+        <v>730</v>
+      </c>
+      <c r="E280" s="24" t="s">
+        <v>66</v>
       </c>
       <c r="F280" s="4"/>
     </row>
     <row r="281" ht="14.25">
-      <c r="A281" s="20" t="s">
-        <v>727</v>
+      <c r="A281" s="21" t="s">
+        <v>731</v>
       </c>
       <c r="B281" s="9"/>
       <c r="C281" s="1"/>
-      <c r="D281" s="25" t="s">
-        <v>728</v>
-      </c>
-      <c r="E281" s="23" t="s">
-        <v>66</v>
+      <c r="D281" s="26" t="s">
+        <v>732</v>
+      </c>
+      <c r="E281" s="22" t="s">
+        <v>10</v>
       </c>
       <c r="F281" s="4"/>
     </row>
     <row r="282" ht="14.25">
-      <c r="A282" s="20" t="s">
-        <v>729</v>
+      <c r="A282" s="21" t="s">
+        <v>733</v>
       </c>
       <c r="B282" s="9"/>
       <c r="C282" s="1"/>
-      <c r="D282" s="25" t="s">
-        <v>730</v>
-      </c>
-      <c r="E282" s="21" t="s">
-        <v>10</v>
+      <c r="D282" s="26" t="s">
+        <v>734</v>
+      </c>
+      <c r="E282" s="24" t="s">
+        <v>66</v>
       </c>
       <c r="F282" s="4"/>
     </row>
     <row r="283" ht="14.25">
-      <c r="A283" s="20" t="s">
-        <v>731</v>
+      <c r="A283" s="21" t="s">
+        <v>735</v>
       </c>
       <c r="B283" s="9"/>
       <c r="C283" s="1"/>
-      <c r="D283" s="25" t="s">
-        <v>686</v>
-      </c>
-      <c r="E283" s="21" t="s">
+      <c r="D283" s="26" t="s">
+        <v>736</v>
+      </c>
+      <c r="E283" s="22" t="s">
         <v>10</v>
       </c>
       <c r="F283" s="4"/>
     </row>
     <row r="284" ht="14.25">
-      <c r="A284" s="20" t="s">
-        <v>732</v>
+      <c r="A284" s="21" t="s">
+        <v>737</v>
       </c>
       <c r="B284" s="9"/>
       <c r="C284" s="1"/>
-      <c r="D284" s="25" t="s">
-        <v>733</v>
-      </c>
-      <c r="E284" s="21" t="s">
+      <c r="D284" s="26" t="s">
+        <v>692</v>
+      </c>
+      <c r="E284" s="22" t="s">
         <v>10</v>
       </c>
       <c r="F284" s="4"/>
     </row>
     <row r="285" ht="14.25">
-      <c r="A285" s="20" t="s">
-        <v>516</v>
+      <c r="A285" s="21" t="s">
+        <v>738</v>
       </c>
       <c r="B285" s="9"/>
       <c r="C285" s="1"/>
-      <c r="D285" s="25" t="s">
-        <v>734</v>
-      </c>
-      <c r="E285" s="21" t="s">
+      <c r="D285" s="26" t="s">
+        <v>739</v>
+      </c>
+      <c r="E285" s="22" t="s">
         <v>10</v>
       </c>
       <c r="F285" s="4"/>
     </row>
     <row r="286" ht="14.25">
-      <c r="A286" s="20" t="s">
-        <v>735</v>
+      <c r="A286" s="21" t="s">
+        <v>522</v>
       </c>
       <c r="B286" s="9"/>
       <c r="C286" s="1"/>
-      <c r="D286" s="25" t="s">
-        <v>736</v>
-      </c>
-      <c r="E286" s="23" t="s">
-        <v>66</v>
+      <c r="D286" s="26" t="s">
+        <v>740</v>
+      </c>
+      <c r="E286" s="22" t="s">
+        <v>10</v>
       </c>
       <c r="F286" s="4"/>
     </row>
     <row r="287" ht="14.25">
-      <c r="A287" s="20" t="s">
-        <v>737</v>
+      <c r="A287" s="21" t="s">
+        <v>741</v>
       </c>
       <c r="B287" s="9"/>
       <c r="C287" s="1"/>
-      <c r="D287" s="25" t="s">
-        <v>738</v>
-      </c>
-      <c r="E287" s="21" t="s">
-        <v>10</v>
+      <c r="D287" s="26" t="s">
+        <v>742</v>
+      </c>
+      <c r="E287" s="24" t="s">
+        <v>66</v>
       </c>
       <c r="F287" s="4"/>
     </row>
     <row r="288" ht="14.25">
-      <c r="A288" s="20" t="s">
-        <v>739</v>
+      <c r="A288" s="21" t="s">
+        <v>743</v>
       </c>
       <c r="B288" s="9"/>
       <c r="C288" s="1"/>
-      <c r="D288" s="25" t="s">
-        <v>740</v>
-      </c>
-      <c r="E288" s="21" t="s">
+      <c r="D288" s="26" t="s">
+        <v>744</v>
+      </c>
+      <c r="E288" s="22" t="s">
         <v>10</v>
       </c>
       <c r="F288" s="4"/>
     </row>
     <row r="289" ht="14.25">
-      <c r="A289" s="20" t="s">
-        <v>741</v>
+      <c r="A289" s="21" t="s">
+        <v>745</v>
       </c>
       <c r="B289" s="9"/>
       <c r="C289" s="1"/>
-      <c r="D289" s="25" t="s">
-        <v>686</v>
-      </c>
-      <c r="E289" s="21" t="s">
+      <c r="D289" s="26" t="s">
+        <v>746</v>
+      </c>
+      <c r="E289" s="22" t="s">
         <v>10</v>
       </c>
       <c r="F289" s="4"/>
     </row>
     <row r="290" ht="14.25">
-      <c r="A290" s="20" t="s">
-        <v>742</v>
+      <c r="A290" s="21" t="s">
+        <v>747</v>
       </c>
       <c r="B290" s="9"/>
       <c r="C290" s="1"/>
-      <c r="D290" s="25" t="s">
-        <v>706</v>
-      </c>
-      <c r="E290" s="23" t="s">
-        <v>66</v>
+      <c r="D290" s="26" t="s">
+        <v>692</v>
+      </c>
+      <c r="E290" s="22" t="s">
+        <v>10</v>
       </c>
       <c r="F290" s="4"/>
     </row>
     <row r="291" ht="14.25">
-      <c r="A291" s="20" t="s">
-        <v>743</v>
+      <c r="A291" s="21" t="s">
+        <v>748</v>
       </c>
       <c r="B291" s="9"/>
       <c r="C291" s="1"/>
-      <c r="D291" s="25" t="s">
-        <v>744</v>
-      </c>
-      <c r="E291" s="16" t="s">
-        <v>10</v>
+      <c r="D291" s="26" t="s">
+        <v>712</v>
+      </c>
+      <c r="E291" s="24" t="s">
+        <v>66</v>
       </c>
       <c r="F291" s="4"/>
     </row>
     <row r="292" ht="14.25">
-      <c r="A292" s="4"/>
-      <c r="B292" s="4"/>
-      <c r="C292" s="4"/>
-      <c r="D292" s="4"/>
-      <c r="E292" s="4"/>
+      <c r="A292" s="21" t="s">
+        <v>749</v>
+      </c>
+      <c r="B292" s="9"/>
+      <c r="C292" s="1"/>
+      <c r="D292" s="26" t="s">
+        <v>750</v>
+      </c>
+      <c r="E292" s="16" t="s">
+        <v>10</v>
+      </c>
       <c r="F292" s="4"/>
     </row>
     <row r="293" ht="14.25">
-      <c r="C293"/>
-      <c r="D293"/>
-      <c r="E293"/>
-      <c r="F293"/>
+      <c r="A293" s="4"/>
+      <c r="B293" s="4"/>
+      <c r="C293" s="4"/>
+      <c r="D293" s="4"/>
+      <c r="E293" s="4"/>
+      <c r="F293" s="4"/>
     </row>
     <row r="294" ht="14.25">
       <c r="C294"/>
@@ -8735,7 +8865,7 @@
       <c r="F308"/>
     </row>
     <row r="309" ht="14.25">
-      <c r="C309" s="1"/>
+      <c r="C309"/>
       <c r="D309"/>
       <c r="E309"/>
       <c r="F309"/>
@@ -8813,6 +8943,7 @@
       <c r="F321"/>
     </row>
     <row r="322" ht="14.25">
+      <c r="C322" s="1"/>
       <c r="D322"/>
       <c r="E322"/>
       <c r="F322"/>
@@ -8872,7 +9003,11 @@
       <c r="E333"/>
       <c r="F333"/>
     </row>
-    <row r="334" ht="14.25"/>
+    <row r="334" ht="14.25">
+      <c r="D334"/>
+      <c r="E334"/>
+      <c r="F334"/>
+    </row>
     <row r="335" ht="14.25"/>
     <row r="336" ht="14.25"/>
     <row r="337" ht="14.25"/>
@@ -8882,6 +9017,7 @@
     <row r="341" ht="14.25"/>
     <row r="342" ht="14.25"/>
     <row r="343" ht="14.25"/>
+    <row r="344" ht="14.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="C5"/>
@@ -9000,7 +9136,7 @@
     <hyperlink r:id="rId114" ref="C130"/>
     <hyperlink r:id="rId115" ref="C131"/>
     <hyperlink r:id="rId116" ref="C132"/>
-    <hyperlink r:id="rId117" ref="C148"/>
+    <hyperlink r:id="rId117" ref="C133"/>
     <hyperlink r:id="rId118" ref="C149"/>
     <hyperlink r:id="rId119" ref="C150"/>
     <hyperlink r:id="rId120" ref="C151"/>
@@ -9011,6 +9147,8 @@
     <hyperlink r:id="rId125" ref="C156"/>
     <hyperlink r:id="rId126" ref="C157"/>
     <hyperlink r:id="rId127" ref="C158"/>
+    <hyperlink r:id="rId128" ref="C159"/>
+    <hyperlink r:id="rId129" ref="C160"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>